<commit_message>
filtered master_svpr to search dropped vets, added dropped vets to assam_elecroll
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$969</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$971:$G$1035</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11798" uniqueCount="8234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12058" uniqueCount="8335">
   <si>
     <t>1994</t>
   </si>
@@ -24972,6 +24972,309 @@
   </si>
   <si>
     <t>UPDATE PHONE</t>
+  </si>
+  <si>
+    <t>Dr. (Ms.) Rupjyoti Ojah/</t>
+  </si>
+  <si>
+    <t>502 Funjan Tower Parag Das Road RP FCI P.O. Bamuni Maidam Guwahati-21 Kamrup (M)</t>
+  </si>
+  <si>
+    <t>Dr. Dipanka Choudhury /Shri Raghu Nath Choudhury</t>
+  </si>
+  <si>
+    <t>H.No.36 Brindaban path Rupnagar P.O. Indrapur Guwahati-781032.</t>
+  </si>
+  <si>
+    <t>Dr. Khagendra Nath Sarmah/</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Dr. Uday Kumar Saha/</t>
+  </si>
+  <si>
+    <t>Dr. Ratna Bahadur Pradhan/</t>
+  </si>
+  <si>
+    <t>Dr. Jadav Sarmah/Late Dandapani Sarmah</t>
+  </si>
+  <si>
+    <t>Department of Pharmacology College of Veterinary Science Assam Agricultural University Khanapara Guwahati-22</t>
+  </si>
+  <si>
+    <t>Dr. Mohanlal Smith/</t>
+  </si>
+  <si>
+    <t>H/N.-24 lane No. 9 (West) Zoo Road Tiniali R.G.B. Road Guwahati-781024</t>
+  </si>
+  <si>
+    <t>Dr. Dandeswar Deka / Sri Harendra Nath Deka</t>
+  </si>
+  <si>
+    <t>Dagaon Kamrup pin.-781133</t>
+  </si>
+  <si>
+    <t>Dr. Satya Dutta Choudhury/</t>
+  </si>
+  <si>
+    <t>Dr. Ikramul Haque/</t>
+  </si>
+  <si>
+    <t>Dr. Umesh Chandra Das/</t>
+  </si>
+  <si>
+    <t>Dr. Gagan Chandra Das/</t>
+  </si>
+  <si>
+    <t>E.O. (Vety.) Gossaigaon Dev. Block Dist. Kokrajhar Assam</t>
+  </si>
+  <si>
+    <t>Dr. Chatra Dhar Borah/</t>
+  </si>
+  <si>
+    <t>E.O. (Vety.) North Lakhimpur Dist. Lakhimpur Assam</t>
+  </si>
+  <si>
+    <t>Dr. Shirajul Hoque/</t>
+  </si>
+  <si>
+    <t>W/No.-4 (Surjyakhata) P.O.&amp; P.S. Bilasipara Dist. Dhubri pin.-783348.</t>
+  </si>
+  <si>
+    <t>Dr. Manoj Kumar Goswami / Sri Haladhar Goswami</t>
+  </si>
+  <si>
+    <t>H.No.-28A Pragati path Chandan Nagar Ghoramara Bhetapara p.o. Beltola Ghy.-28.</t>
+  </si>
+  <si>
+    <t>Dr. Digendra Talukdar /Late Debendra Nath Talukdar</t>
+  </si>
+  <si>
+    <t>Dr. Krishna Pathak/</t>
+  </si>
+  <si>
+    <t>Dr. Girindra Nath Sen / Sri Gajendra Nath Sen</t>
+  </si>
+  <si>
+    <t>VAS. Kokrajhar Vety. Hospital P.O. Titaguri Dist. Kokrajhar (BTC) Pin- 783374</t>
+  </si>
+  <si>
+    <t>Dr. Pranab Das /Sri Uttam Chandra Das</t>
+  </si>
+  <si>
+    <t>Birkuchi Malabhaban Near CanaraBank Assam carbon Road Narengi Guwahati-26.</t>
+  </si>
+  <si>
+    <t>Dr. Jayanta Kumar Talukdar /Sri Sarat Chandra Talukdar</t>
+  </si>
+  <si>
+    <t>State Vety. Dispensary Hailakandi P.O. Hailakandi Dist.Hailakandi</t>
+  </si>
+  <si>
+    <t>Dr. Nilutpal Kakati /Late Pitram Nath</t>
+  </si>
+  <si>
+    <t>Eragaon W.No.-6 Morigaon P.O. P.S. &amp; Dist. Morigaon pin.-782105.</t>
+  </si>
+  <si>
+    <t>Dr. Lalit Chandra Lahon / Late Padmeswar Lahon</t>
+  </si>
+  <si>
+    <t>H.No.-72 Homeopethic College Road Byelane No.-2(East) Panjabari Guwahati-781037.</t>
+  </si>
+  <si>
+    <t>Dr. Pranab Chandra Kalita/Sri Tarini Kanta Kalita</t>
+  </si>
+  <si>
+    <t>Asstt. Professor College of Vety. Sc. &amp; A.H. CAU Deptt. of Anatomy &amp; Histology Selesin Aizawl Mizoram Pin-796014</t>
+  </si>
+  <si>
+    <t>Dr. Md. Isfaqul Hussain / Md. Safiqul Hussain</t>
+  </si>
+  <si>
+    <t>Dr. Harabinda Saharia /Sri Baneswar Saharia</t>
+  </si>
+  <si>
+    <t>Dr. Kamal Sarma / Sri Binode Kumar Sarma</t>
+  </si>
+  <si>
+    <t>Dr. Sashanka Sekhar Dutta /Mr. Kamaleswar Dutta</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Geetima Barman /Mr. Kanak Chandra Barman</t>
+  </si>
+  <si>
+    <t>Dr. Parimal Roychoudhury /Dr. R.K. Roychoudhury</t>
+  </si>
+  <si>
+    <t>Asstt. Professor Dept. of Vety. Microbiology CVSC. &amp; A.H. CAU Selesit Aizawl Mizoram</t>
+  </si>
+  <si>
+    <t>Dr. Ditul Barman /Sri Bipin Chandra Barman</t>
+  </si>
+  <si>
+    <t>Dr. Gargo Ram Mahilary /Sri Kameswar Mahilary</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Kaberi Deka / Dr. Bhumidhar Deka</t>
+  </si>
+  <si>
+    <t>H.No.-63 Opp. T.C. Girls' School G.N.B. Road Guwahati pin.-781003</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Manika Buragohain/ Sri Kanak Buragohain (F)</t>
+  </si>
+  <si>
+    <t>Dr. Bhupesh Chandra Bhattacharyya /Sri Golok Bhattacharyya</t>
+  </si>
+  <si>
+    <t>Dr. Siddhartha Kumar Barooah/</t>
+  </si>
+  <si>
+    <t>Dr. Ikramul Hussain Sarkar /Md. Aftabuddin Ahmed</t>
+  </si>
+  <si>
+    <t>VAS. State Vety. Dispensary Fakuagram Karimganj</t>
+  </si>
+  <si>
+    <t>Dr. Deepak Sarma / Sri M.N. Sarma</t>
+  </si>
+  <si>
+    <t>Dr. Prabhat Basumatary /Sri Ramesh Chandra Basumatary</t>
+  </si>
+  <si>
+    <t>Dr. Mridul Nath /Mr. Nalini Kanta Nath</t>
+  </si>
+  <si>
+    <t>Vill. &amp; P.O. Bahalpar Dist. Dhubri</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Rumi Gogoi /Sri Jogeswar Gogoi (F)</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Monalisa Saikia /Mr. Nabin Chandra Saikia (F)</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Tripti Buragohain /Mr. Biren Buragohain</t>
+  </si>
+  <si>
+    <t>Bamun para Milan Nagar Lokhra Guwahati Assam</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Kakali Basumatary /Sri S. Basumatari (F)</t>
+  </si>
+  <si>
+    <t>Dr. Surajit Nath /Sri S.C. Nath</t>
+  </si>
+  <si>
+    <t>Dr. Hiranya Kumar Das / Sri Dinesh Chandra Das</t>
+  </si>
+  <si>
+    <t>Metuakuchi Barpeta Dist- Barpeta PIN-781301 Assam</t>
+  </si>
+  <si>
+    <t>Dr. Sanjib Khargharia /Sri Prafulla Chandra Khargharia</t>
+  </si>
+  <si>
+    <t>Dr. Runtu Gogoi /Sri Rama Kanta Gogoi</t>
+  </si>
+  <si>
+    <t>Dr. Biraj Jyoti Deuri /Sri Krishna Kanta Deuri</t>
+  </si>
+  <si>
+    <t>Dr. Subodh Kumar Singh / Sri Ram Hilish Singh</t>
+  </si>
+  <si>
+    <t>Sukadh Hotel Silapathar P.O. Silapathar Main Road Dist. Dhemaji.</t>
+  </si>
+  <si>
+    <t>Dr. Ranjan Kumar Das / Mr. Bhupen Chandra Das</t>
+  </si>
+  <si>
+    <t>Dr. Nilim Kumar Kakati / Sri Paban Kakati</t>
+  </si>
+  <si>
+    <t>Dr. Denish Gogoi /Mr. Uttam Chandra Gogoi</t>
+  </si>
+  <si>
+    <t>Dr. (Ms) Irin Jebin / (F) - Late Dr. Farid Ali</t>
+  </si>
+  <si>
+    <t>Dr. Kolhite Rhakho /(F) - Late Kelhitsuryi</t>
+  </si>
+  <si>
+    <t>Patgaon P.O. Azara Campus Pin- 781017</t>
+  </si>
+  <si>
+    <t>Dr. Kangkan Deka /(F) - Parikshit Deka</t>
+  </si>
+  <si>
+    <t>Vill. Danghapara P.O. Banekuchi Dist. Nalbari Pin- 781340</t>
+  </si>
+  <si>
+    <t>Dr. Malek Ali /(F) - Akbar Ali</t>
+  </si>
+  <si>
+    <t>Vill. Bandali P.O. Jatradia P.S. Tarabari Dist. Barpeta- 781305</t>
+  </si>
+  <si>
+    <t>Dr. Sayashree Rabha /(F) - Karuna Kanta Rabha</t>
+  </si>
+  <si>
+    <t>Vill. Mirza Near- Mirza Post Office House No. 122 Kamrup (R) Assam- 781125</t>
+  </si>
+  <si>
+    <t>Dr. Nitu Thengal /F.Namr- Punaram Thengal</t>
+  </si>
+  <si>
+    <t>Vill. Chawdung Pather Merachuk P.O. Chawdung Pather Dist. Golaghat Pin.-785705.</t>
+  </si>
+  <si>
+    <t>Dr. Neelakshi Duttabaruah /(F) - Mrinal Duttabaruah</t>
+  </si>
+  <si>
+    <t>Amingaon Madhyam Amingaon Guwahati-781031</t>
+  </si>
+  <si>
+    <t>Dr. Akash Jyoti Moral /(F) - Hiren Moral</t>
+  </si>
+  <si>
+    <t>Latakata Ganeshnagar Path H./No109 Opp. CID Quarters P.O.&amp; P.S. Basistha Chariali Guwahati-781029.</t>
+  </si>
+  <si>
+    <t>Dr. Pabitra Bortamuly / (F) - Gonesh Bortamuly</t>
+  </si>
+  <si>
+    <t>Vill. Lukumaigaon P.O. Halodhibari P.S. Dergaon Dist. Golaghat Pin.- 785618</t>
+  </si>
+  <si>
+    <t>Dr. pollabi Kachari /(F) - Punaram Kachari</t>
+  </si>
+  <si>
+    <t>Bojalbari Gaon Titabar P.O. Boruajan Dist. Jorhat Pin.-785630</t>
+  </si>
+  <si>
+    <t>Dr. Bhargab Jyoti Sarmah/Madhu Dev Sarmah</t>
+  </si>
+  <si>
+    <t>Vill: Gerimari Joy Nagar Near Law College Mangaldoi Darrang Assam - 784125</t>
+  </si>
+  <si>
+    <t>Dr. Jyoti Doley/Durgeswar Doley</t>
+  </si>
+  <si>
+    <t>House No 49 Rangaihabi Gaon Row Riah Jorhat Assam Pin 785004</t>
+  </si>
+  <si>
+    <t>Dr. Bikash Kumar Pandey/Oshihar Pandey</t>
+  </si>
+  <si>
+    <t>Sinatolia Near Asian Public School North Lakhimpur Assam Pin 787031</t>
+  </si>
+  <si>
+    <t>NEW ENTRY</t>
   </si>
 </sst>
 </file>
@@ -25045,7 +25348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -25090,6 +25393,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -25479,30 +25789,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U969"/>
+  <dimension ref="A1:U1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A969" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K971" sqref="K971"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="24" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="5"/>
     <col min="13" max="13" width="19.85546875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="28" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="27.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="37.140625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="18" max="18" width="37.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" customWidth="1"/>
     <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -86171,6 +86481,1286 @@
         <v>7002243237</v>
       </c>
     </row>
+    <row r="971" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="E971" s="11" t="s">
+        <v>8234</v>
+      </c>
+      <c r="F971" s="16">
+        <v>21922</v>
+      </c>
+      <c r="G971" s="11" t="s">
+        <v>8235</v>
+      </c>
+      <c r="H971" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J971" s="17">
+        <v>9864132078</v>
+      </c>
+      <c r="K971" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="972" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="E972" s="11" t="s">
+        <v>8236</v>
+      </c>
+      <c r="F972" s="16">
+        <v>22482</v>
+      </c>
+      <c r="G972" s="11" t="s">
+        <v>8237</v>
+      </c>
+      <c r="H972" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J972" s="17">
+        <v>7896194704</v>
+      </c>
+      <c r="K972" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="973" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="E973" s="11" t="s">
+        <v>8238</v>
+      </c>
+      <c r="F973" s="16">
+        <v>22706</v>
+      </c>
+      <c r="G973" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H973" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J973" s="17">
+        <v>9435185211</v>
+      </c>
+      <c r="K973" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="974" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="E974" s="11" t="s">
+        <v>8240</v>
+      </c>
+      <c r="F974" s="16">
+        <v>22288</v>
+      </c>
+      <c r="G974" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H974" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J974" s="17">
+        <v>9435007601</v>
+      </c>
+      <c r="K974" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="975" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="E975" s="11" t="s">
+        <v>8241</v>
+      </c>
+      <c r="F975" s="16">
+        <v>21620</v>
+      </c>
+      <c r="G975" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H975" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J975" s="17">
+        <v>7086329911</v>
+      </c>
+      <c r="K975" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="976" spans="1:21" ht="120" x14ac:dyDescent="0.25">
+      <c r="E976" s="11" t="s">
+        <v>8242</v>
+      </c>
+      <c r="F976" s="16">
+        <v>23798</v>
+      </c>
+      <c r="G976" s="11" t="s">
+        <v>8243</v>
+      </c>
+      <c r="H976" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J976" s="17">
+        <v>9435749321</v>
+      </c>
+      <c r="K976" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="977" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E977" s="11" t="s">
+        <v>8244</v>
+      </c>
+      <c r="F977" s="16">
+        <v>20375</v>
+      </c>
+      <c r="G977" s="11" t="s">
+        <v>8245</v>
+      </c>
+      <c r="H977" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J977" s="17">
+        <v>9435195118</v>
+      </c>
+      <c r="K977" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="978" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E978" s="11" t="s">
+        <v>8246</v>
+      </c>
+      <c r="F978" s="16">
+        <v>24167</v>
+      </c>
+      <c r="G978" s="11" t="s">
+        <v>8247</v>
+      </c>
+      <c r="H978" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J978" s="17">
+        <v>9435110761</v>
+      </c>
+      <c r="K978" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="979" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E979" s="11" t="s">
+        <v>8248</v>
+      </c>
+      <c r="F979" s="16">
+        <v>23429</v>
+      </c>
+      <c r="G979" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H979" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J979" s="17">
+        <v>8638428450</v>
+      </c>
+      <c r="K979" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="980" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E980" s="11" t="s">
+        <v>8249</v>
+      </c>
+      <c r="F980" s="16">
+        <v>23102</v>
+      </c>
+      <c r="G980" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H980" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J980" s="17">
+        <v>9435127577</v>
+      </c>
+      <c r="K980" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="981" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E981" s="11" t="s">
+        <v>8250</v>
+      </c>
+      <c r="F981" s="16">
+        <v>22287</v>
+      </c>
+      <c r="G981" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H981" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J981" s="17">
+        <v>9577011722</v>
+      </c>
+      <c r="K981" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="982" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E982" s="11" t="s">
+        <v>8251</v>
+      </c>
+      <c r="F982" s="16">
+        <v>24110</v>
+      </c>
+      <c r="G982" s="11" t="s">
+        <v>8252</v>
+      </c>
+      <c r="H982" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J982" s="17">
+        <v>9954425354</v>
+      </c>
+      <c r="K982" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="983" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E983" s="11" t="s">
+        <v>8253</v>
+      </c>
+      <c r="F983" s="16">
+        <v>23224</v>
+      </c>
+      <c r="G983" s="11" t="s">
+        <v>8254</v>
+      </c>
+      <c r="H983" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J983" s="17"/>
+      <c r="K983" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="984" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E984" s="11" t="s">
+        <v>8255</v>
+      </c>
+      <c r="F984" s="16">
+        <v>24166</v>
+      </c>
+      <c r="G984" s="11" t="s">
+        <v>8256</v>
+      </c>
+      <c r="H984" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J984" s="17">
+        <v>7002655615</v>
+      </c>
+      <c r="K984" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="985" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E985" s="11" t="s">
+        <v>8257</v>
+      </c>
+      <c r="F985" s="16">
+        <v>24929</v>
+      </c>
+      <c r="G985" s="11" t="s">
+        <v>8258</v>
+      </c>
+      <c r="H985" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J985" s="17">
+        <v>9435082741</v>
+      </c>
+      <c r="K985" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="986" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E986" s="11" t="s">
+        <v>8259</v>
+      </c>
+      <c r="F986" s="16">
+        <v>24504</v>
+      </c>
+      <c r="G986" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H986" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J986" s="17">
+        <v>9435505584</v>
+      </c>
+      <c r="K986" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="987" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E987" s="11" t="s">
+        <v>8260</v>
+      </c>
+      <c r="F987" s="16">
+        <v>24193</v>
+      </c>
+      <c r="G987" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H987" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J987" s="17"/>
+      <c r="K987" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="988" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E988" s="11" t="s">
+        <v>8261</v>
+      </c>
+      <c r="F988" s="16">
+        <v>25263</v>
+      </c>
+      <c r="G988" s="11" t="s">
+        <v>8262</v>
+      </c>
+      <c r="H988" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J988" s="17">
+        <v>9854289976</v>
+      </c>
+      <c r="K988" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="989" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E989" s="11" t="s">
+        <v>8263</v>
+      </c>
+      <c r="F989" s="16">
+        <v>24286</v>
+      </c>
+      <c r="G989" s="11" t="s">
+        <v>8264</v>
+      </c>
+      <c r="H989" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J989" s="17">
+        <v>7002852103</v>
+      </c>
+      <c r="K989" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="990" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E990" s="11" t="s">
+        <v>8265</v>
+      </c>
+      <c r="F990" s="16">
+        <v>24898</v>
+      </c>
+      <c r="G990" s="11" t="s">
+        <v>8266</v>
+      </c>
+      <c r="H990" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J990" s="17">
+        <v>9101892538</v>
+      </c>
+      <c r="K990" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="991" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E991" s="11" t="s">
+        <v>8267</v>
+      </c>
+      <c r="F991" s="16">
+        <v>24898</v>
+      </c>
+      <c r="G991" s="11" t="s">
+        <v>8268</v>
+      </c>
+      <c r="H991" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J991" s="17">
+        <v>7086409597</v>
+      </c>
+      <c r="K991" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="992" spans="5:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="E992" s="11" t="s">
+        <v>8269</v>
+      </c>
+      <c r="F992" s="16">
+        <v>19360</v>
+      </c>
+      <c r="G992" s="11" t="s">
+        <v>8270</v>
+      </c>
+      <c r="H992" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J992" s="17">
+        <v>9435303966</v>
+      </c>
+      <c r="K992" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="993" spans="5:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="E993" s="11" t="s">
+        <v>8271</v>
+      </c>
+      <c r="F993" s="16">
+        <v>25263</v>
+      </c>
+      <c r="G993" s="11" t="s">
+        <v>8272</v>
+      </c>
+      <c r="H993" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J993" s="17"/>
+      <c r="K993" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="994" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E994" s="11" t="s">
+        <v>8273</v>
+      </c>
+      <c r="F994" s="16">
+        <v>24926</v>
+      </c>
+      <c r="G994" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H994" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J994" s="17">
+        <v>9419011945</v>
+      </c>
+      <c r="K994" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="995" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E995" s="11" t="s">
+        <v>8274</v>
+      </c>
+      <c r="F995" s="16">
+        <v>25628</v>
+      </c>
+      <c r="G995" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H995" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J995" s="17">
+        <v>9435083281</v>
+      </c>
+      <c r="K995" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="996" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E996" s="11" t="s">
+        <v>8275</v>
+      </c>
+      <c r="F996" s="16">
+        <v>26682</v>
+      </c>
+      <c r="G996" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H996" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J996" s="17"/>
+      <c r="K996" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="997" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E997" s="11" t="s">
+        <v>8276</v>
+      </c>
+      <c r="F997" s="16">
+        <v>27082</v>
+      </c>
+      <c r="G997" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H997" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J997" s="17"/>
+      <c r="K997" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="998" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E998" s="11" t="s">
+        <v>8277</v>
+      </c>
+      <c r="F998" s="16">
+        <v>27049</v>
+      </c>
+      <c r="G998" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H998" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J998" s="17">
+        <v>8811014787</v>
+      </c>
+      <c r="K998" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="999" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E999" s="11" t="s">
+        <v>8278</v>
+      </c>
+      <c r="F999" s="16">
+        <v>27287</v>
+      </c>
+      <c r="G999" s="11" t="s">
+        <v>8279</v>
+      </c>
+      <c r="H999" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J999" s="17">
+        <v>8837262227</v>
+      </c>
+      <c r="K999" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1000" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1000" s="11" t="s">
+        <v>8280</v>
+      </c>
+      <c r="F1000" s="16">
+        <v>27504</v>
+      </c>
+      <c r="G1000" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1000" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1000" s="17">
+        <v>9854047807</v>
+      </c>
+      <c r="K1000" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1001" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1001" s="11" t="s">
+        <v>8281</v>
+      </c>
+      <c r="F1001" s="16">
+        <v>25902</v>
+      </c>
+      <c r="G1001" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1001" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1001" s="17">
+        <v>8011785954</v>
+      </c>
+      <c r="K1001" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1002" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1002" s="11" t="s">
+        <v>8282</v>
+      </c>
+      <c r="F1002" s="16">
+        <v>26011</v>
+      </c>
+      <c r="G1002" s="11" t="s">
+        <v>8283</v>
+      </c>
+      <c r="H1002" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1002" s="17">
+        <v>9435702388</v>
+      </c>
+      <c r="K1002" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1003" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1003" s="11" t="s">
+        <v>8284</v>
+      </c>
+      <c r="F1003" s="16">
+        <v>27334</v>
+      </c>
+      <c r="G1003" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1003" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1003" s="17">
+        <v>8753885884</v>
+      </c>
+      <c r="K1003" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1004" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1004" s="11" t="s">
+        <v>8285</v>
+      </c>
+      <c r="F1004" s="16">
+        <v>26724</v>
+      </c>
+      <c r="G1004" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1004" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1004" s="17">
+        <v>9435041951</v>
+      </c>
+      <c r="K1004" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1005" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1005" s="11" t="s">
+        <v>8286</v>
+      </c>
+      <c r="F1005" s="16">
+        <v>27426</v>
+      </c>
+      <c r="G1005" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1005" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1005" s="17">
+        <v>8402046333</v>
+      </c>
+      <c r="K1005" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1006" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1006" s="11" t="s">
+        <v>8287</v>
+      </c>
+      <c r="F1006" s="16">
+        <v>26724</v>
+      </c>
+      <c r="G1006" s="11" t="s">
+        <v>8288</v>
+      </c>
+      <c r="H1006" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1006" s="17">
+        <v>7002585745</v>
+      </c>
+      <c r="K1006" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1007" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1007" s="11" t="s">
+        <v>8289</v>
+      </c>
+      <c r="F1007" s="16">
+        <v>25993</v>
+      </c>
+      <c r="G1007" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1007" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1007" s="17">
+        <v>9435182806</v>
+      </c>
+      <c r="K1007" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1008" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1008" s="11" t="s">
+        <v>8290</v>
+      </c>
+      <c r="F1008" s="16">
+        <v>24926</v>
+      </c>
+      <c r="G1008" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1008" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1008" s="17">
+        <v>9435125082</v>
+      </c>
+      <c r="K1008" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1009" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1009" s="11" t="s">
+        <v>8291</v>
+      </c>
+      <c r="F1009" s="16">
+        <v>27072</v>
+      </c>
+      <c r="G1009" s="11" t="s">
+        <v>8292</v>
+      </c>
+      <c r="H1009" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1009" s="17">
+        <v>7002324548</v>
+      </c>
+      <c r="K1009" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1010" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1010" s="11" t="s">
+        <v>8293</v>
+      </c>
+      <c r="F1010" s="16">
+        <v>27791</v>
+      </c>
+      <c r="G1010" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1010" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1010" s="17">
+        <v>8473906605</v>
+      </c>
+      <c r="K1010" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1011" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1011" s="11" t="s">
+        <v>8294</v>
+      </c>
+      <c r="F1011" s="16">
+        <v>27608</v>
+      </c>
+      <c r="G1011" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1011" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1011" s="17"/>
+      <c r="K1011" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1012" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1012" s="11" t="s">
+        <v>8295</v>
+      </c>
+      <c r="F1012" s="16">
+        <v>27691</v>
+      </c>
+      <c r="G1012" s="11" t="s">
+        <v>8296</v>
+      </c>
+      <c r="H1012" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1012" s="17">
+        <v>8981558104</v>
+      </c>
+      <c r="K1012" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1013" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1013" s="11" t="s">
+        <v>8297</v>
+      </c>
+      <c r="F1013" s="16">
+        <v>26944</v>
+      </c>
+      <c r="G1013" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1013" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1013" s="17">
+        <v>9401057456</v>
+      </c>
+      <c r="K1013" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1014" spans="5:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="E1014" s="11" t="s">
+        <v>8298</v>
+      </c>
+      <c r="F1014" s="16">
+        <v>27023</v>
+      </c>
+      <c r="G1014" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1014" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1014" s="17">
+        <v>9818941573</v>
+      </c>
+      <c r="K1014" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1015" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1015" s="11" t="s">
+        <v>8299</v>
+      </c>
+      <c r="F1015" s="16">
+        <v>27819</v>
+      </c>
+      <c r="G1015" s="11" t="s">
+        <v>8300</v>
+      </c>
+      <c r="H1015" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1015" s="17">
+        <v>9854243438</v>
+      </c>
+      <c r="K1015" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1016" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1016" s="11" t="s">
+        <v>8301</v>
+      </c>
+      <c r="F1016" s="16">
+        <v>28185</v>
+      </c>
+      <c r="G1016" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1016" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1016" s="17"/>
+      <c r="K1016" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1017" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1017" s="11" t="s">
+        <v>8302</v>
+      </c>
+      <c r="F1017" s="16">
+        <v>27638</v>
+      </c>
+      <c r="G1017" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1017" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1017" s="17"/>
+      <c r="K1017" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1018" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1018" s="11" t="s">
+        <v>8303</v>
+      </c>
+      <c r="F1018" s="16">
+        <v>28156</v>
+      </c>
+      <c r="G1018" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1018" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1018" s="17"/>
+      <c r="K1018" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1019" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1019" s="11" t="s">
+        <v>8304</v>
+      </c>
+      <c r="F1019" s="16">
+        <v>27682</v>
+      </c>
+      <c r="G1019" s="11" t="s">
+        <v>8305</v>
+      </c>
+      <c r="H1019" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1019" s="17">
+        <v>7002039865</v>
+      </c>
+      <c r="K1019" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1020" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1020" s="11" t="s">
+        <v>8306</v>
+      </c>
+      <c r="F1020" s="16">
+        <v>29027</v>
+      </c>
+      <c r="G1020" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1020" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1020" s="17">
+        <v>9866421693</v>
+      </c>
+      <c r="K1020" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1021" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1021" s="11" t="s">
+        <v>8307</v>
+      </c>
+      <c r="F1021" s="16">
+        <v>29646</v>
+      </c>
+      <c r="G1021" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1021" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1021" s="17"/>
+      <c r="K1021" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1022" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1022" s="11" t="s">
+        <v>8308</v>
+      </c>
+      <c r="F1022" s="16">
+        <v>29281</v>
+      </c>
+      <c r="G1022" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1022" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1022" s="17"/>
+      <c r="K1022" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1023" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1023" s="11" t="s">
+        <v>8309</v>
+      </c>
+      <c r="F1023" s="16">
+        <v>31803</v>
+      </c>
+      <c r="G1023" s="11" t="s">
+        <v>8239</v>
+      </c>
+      <c r="H1023" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1023" s="17"/>
+      <c r="K1023" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1024" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1024" s="11" t="s">
+        <v>8310</v>
+      </c>
+      <c r="F1024" s="16">
+        <v>25628</v>
+      </c>
+      <c r="G1024" s="11" t="s">
+        <v>8311</v>
+      </c>
+      <c r="H1024" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1024" s="17">
+        <v>8473085326</v>
+      </c>
+      <c r="K1024" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1025" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1025" s="11" t="s">
+        <v>8312</v>
+      </c>
+      <c r="F1025" s="16">
+        <v>34360</v>
+      </c>
+      <c r="G1025" s="11" t="s">
+        <v>8313</v>
+      </c>
+      <c r="H1025" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1025" s="17">
+        <v>7002739184</v>
+      </c>
+      <c r="K1025" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1026" spans="5:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="E1026" s="11" t="s">
+        <v>8314</v>
+      </c>
+      <c r="F1026" s="16">
+        <v>34366</v>
+      </c>
+      <c r="G1026" s="11" t="s">
+        <v>8315</v>
+      </c>
+      <c r="H1026" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1026" s="17">
+        <v>9707989486</v>
+      </c>
+      <c r="K1026" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1027" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1027" s="11" t="s">
+        <v>8316</v>
+      </c>
+      <c r="F1027" s="16"/>
+      <c r="G1027" s="11" t="s">
+        <v>8317</v>
+      </c>
+      <c r="H1027" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1027" s="17">
+        <v>7086644885</v>
+      </c>
+      <c r="K1027" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1028" spans="5:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="E1028" s="11" t="s">
+        <v>8318</v>
+      </c>
+      <c r="F1028" s="16">
+        <v>35751</v>
+      </c>
+      <c r="G1028" s="11" t="s">
+        <v>8319</v>
+      </c>
+      <c r="H1028" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1028" s="17">
+        <v>8638086379</v>
+      </c>
+      <c r="K1028" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1029" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1029" s="11" t="s">
+        <v>8320</v>
+      </c>
+      <c r="F1029" s="16">
+        <v>35363</v>
+      </c>
+      <c r="G1029" s="11" t="s">
+        <v>8321</v>
+      </c>
+      <c r="H1029" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1029" s="17">
+        <v>8486568013</v>
+      </c>
+      <c r="K1029" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1030" spans="5:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="E1030" s="11" t="s">
+        <v>8322</v>
+      </c>
+      <c r="F1030" s="16">
+        <v>35474</v>
+      </c>
+      <c r="G1030" s="11" t="s">
+        <v>8323</v>
+      </c>
+      <c r="H1030" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1030" s="17">
+        <v>9085388367</v>
+      </c>
+      <c r="K1030" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1031" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1031" s="11" t="s">
+        <v>8324</v>
+      </c>
+      <c r="F1031" s="16">
+        <v>35080</v>
+      </c>
+      <c r="G1031" s="11" t="s">
+        <v>8325</v>
+      </c>
+      <c r="H1031" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1031" s="17">
+        <v>8822340659</v>
+      </c>
+      <c r="K1031" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1032" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1032" s="11" t="s">
+        <v>8326</v>
+      </c>
+      <c r="F1032" s="16">
+        <v>35869</v>
+      </c>
+      <c r="G1032" s="11" t="s">
+        <v>8327</v>
+      </c>
+      <c r="H1032" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1032" s="17">
+        <v>8135949992</v>
+      </c>
+      <c r="K1032" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1033" spans="5:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="E1033" s="11" t="s">
+        <v>8328</v>
+      </c>
+      <c r="F1033" s="16">
+        <v>35861</v>
+      </c>
+      <c r="G1033" s="11" t="s">
+        <v>8329</v>
+      </c>
+      <c r="H1033" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1033" s="17">
+        <v>9101370189</v>
+      </c>
+      <c r="K1033" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1034" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1034" s="11" t="s">
+        <v>8330</v>
+      </c>
+      <c r="F1034" s="16">
+        <v>35828</v>
+      </c>
+      <c r="G1034" s="11" t="s">
+        <v>8331</v>
+      </c>
+      <c r="H1034" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1034" s="17">
+        <v>9101126144</v>
+      </c>
+      <c r="K1034" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1035" spans="5:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1035" s="11" t="s">
+        <v>8332</v>
+      </c>
+      <c r="F1035" s="16">
+        <v>36011</v>
+      </c>
+      <c r="G1035" s="11" t="s">
+        <v>8333</v>
+      </c>
+      <c r="H1035" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1035" s="17">
+        <v>6000925311</v>
+      </c>
+      <c r="K1035" t="s">
+        <v>8334</v>
+      </c>
+    </row>
+    <row r="1036" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H1036" s="18"/>
+    </row>
+    <row r="1037" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H1037" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
properly added the dropped vets to the assam_elecroll
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12058" uniqueCount="8335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12123" uniqueCount="8400">
   <si>
     <t>1994</t>
   </si>
@@ -25275,6 +25275,201 @@
   </si>
   <si>
     <t>NEW ENTRY</t>
+  </si>
+  <si>
+    <t>ASM/0013/1984</t>
+  </si>
+  <si>
+    <t>ASM/0410/1985</t>
+  </si>
+  <si>
+    <t>ASM/0440/1985</t>
+  </si>
+  <si>
+    <t>ASM/0635/1988</t>
+  </si>
+  <si>
+    <t>ASM/0654/1988</t>
+  </si>
+  <si>
+    <t>ASM/0690/1988</t>
+  </si>
+  <si>
+    <t>ASM/0714/1988</t>
+  </si>
+  <si>
+    <t>ASM/0842/1989</t>
+  </si>
+  <si>
+    <t>ASM/0856/1989</t>
+  </si>
+  <si>
+    <t>ASM/0863/1989</t>
+  </si>
+  <si>
+    <t>ASM/0870/1989</t>
+  </si>
+  <si>
+    <t>ASM/0884/1990</t>
+  </si>
+  <si>
+    <t>ASM/0979/1991</t>
+  </si>
+  <si>
+    <t>ASM/1036/1991</t>
+  </si>
+  <si>
+    <t>ASM/1061/1991</t>
+  </si>
+  <si>
+    <t>ASM/1089/1991</t>
+  </si>
+  <si>
+    <t>ASM/1105/1991</t>
+  </si>
+  <si>
+    <t>ASM/1136/1992</t>
+  </si>
+  <si>
+    <t>ASM/1184/1992</t>
+  </si>
+  <si>
+    <t>ASM/1196/1992</t>
+  </si>
+  <si>
+    <t>ASM/1208/1992</t>
+  </si>
+  <si>
+    <t>ASM/1250/1993</t>
+  </si>
+  <si>
+    <t>ASM/1287/1994</t>
+  </si>
+  <si>
+    <t>ASM/1289/1994</t>
+  </si>
+  <si>
+    <t>ASM/1469/1995</t>
+  </si>
+  <si>
+    <t>ASM/1523/1996</t>
+  </si>
+  <si>
+    <t>ASM/1608/1997</t>
+  </si>
+  <si>
+    <t>ASM/1626/1997</t>
+  </si>
+  <si>
+    <t>ASM/1651/1997</t>
+  </si>
+  <si>
+    <t>ASM/1681/1998</t>
+  </si>
+  <si>
+    <t>ASM/1684/1998</t>
+  </si>
+  <si>
+    <t>ASM/1690/1998</t>
+  </si>
+  <si>
+    <t>ASM/1698/1998</t>
+  </si>
+  <si>
+    <t>ASM/1713/1998</t>
+  </si>
+  <si>
+    <t>ASM/1722/1998</t>
+  </si>
+  <si>
+    <t>ASM/1730/1998</t>
+  </si>
+  <si>
+    <t>ASM/1765/1998</t>
+  </si>
+  <si>
+    <t>ASM/1766/1998</t>
+  </si>
+  <si>
+    <t>ASM/1793/1998</t>
+  </si>
+  <si>
+    <t>ASM/1806/1999</t>
+  </si>
+  <si>
+    <t>ASM/1832/1999</t>
+  </si>
+  <si>
+    <t>ASM/1833/1999</t>
+  </si>
+  <si>
+    <t>ASM/1870/1999</t>
+  </si>
+  <si>
+    <t>ASM/1871/1999</t>
+  </si>
+  <si>
+    <t>ASM/1888/2000</t>
+  </si>
+  <si>
+    <t>ASM/1942/2001</t>
+  </si>
+  <si>
+    <t>ASM/1961/2001</t>
+  </si>
+  <si>
+    <t>ASM/1965/2001</t>
+  </si>
+  <si>
+    <t>ASM/1966/2001</t>
+  </si>
+  <si>
+    <t>ASM/2149/2004</t>
+  </si>
+  <si>
+    <t>ASM/2426/2009</t>
+  </si>
+  <si>
+    <t>ASM/2427/2009</t>
+  </si>
+  <si>
+    <t>ASM/2585/2011</t>
+  </si>
+  <si>
+    <t>ASM/2912/2017</t>
+  </si>
+  <si>
+    <t>ASM/2986/2018</t>
+  </si>
+  <si>
+    <t>ASM/3042/2019</t>
+  </si>
+  <si>
+    <t>ASM/3185/2020</t>
+  </si>
+  <si>
+    <t>ASM/3212/2022</t>
+  </si>
+  <si>
+    <t>ASM/3221/2022</t>
+  </si>
+  <si>
+    <t>ASM/3222/2022</t>
+  </si>
+  <si>
+    <t>ASM/3224/2022</t>
+  </si>
+  <si>
+    <t>ASM/3225/2022</t>
+  </si>
+  <si>
+    <t>ASM/3278/2023</t>
+  </si>
+  <si>
+    <t>ASM/3280/2023</t>
+  </si>
+  <si>
+    <t>ASM/3281/2023</t>
   </si>
 </sst>
 </file>
@@ -25395,11 +25590,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -25791,8 +25988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1037"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A969" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K971" sqref="K971"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -86482,1284 +86679,1739 @@
       </c>
     </row>
     <row r="971" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="E971" s="11" t="s">
+      <c r="A971" s="1"/>
+      <c r="B971" s="1"/>
+      <c r="C971" s="1"/>
+      <c r="D971" s="1"/>
+      <c r="E971" s="1" t="s">
         <v>8234</v>
       </c>
-      <c r="F971" s="16">
+      <c r="F971" s="17">
         <v>21922</v>
       </c>
-      <c r="G971" s="11" t="s">
+      <c r="G971" s="1" t="s">
         <v>8235</v>
       </c>
       <c r="H971" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J971" s="17">
+      <c r="I971" s="1" t="s">
+        <v>8335</v>
+      </c>
+      <c r="J971" s="15">
         <v>9864132078</v>
       </c>
-      <c r="K971" t="s">
+      <c r="K971" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
     <row r="972" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="E972" s="11" t="s">
+      <c r="A972" s="1"/>
+      <c r="B972" s="1"/>
+      <c r="C972" s="1"/>
+      <c r="D972" s="1"/>
+      <c r="E972" s="1" t="s">
         <v>8236</v>
       </c>
-      <c r="F972" s="16">
+      <c r="F972" s="17">
         <v>22482</v>
       </c>
-      <c r="G972" s="11" t="s">
+      <c r="G972" s="1" t="s">
         <v>8237</v>
       </c>
       <c r="H972" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J972" s="17">
+      <c r="I972" s="1" t="s">
+        <v>8336</v>
+      </c>
+      <c r="J972" s="15">
         <v>7896194704</v>
       </c>
-      <c r="K972" t="s">
+      <c r="K972" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
     <row r="973" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="E973" s="11" t="s">
+      <c r="A973" s="1"/>
+      <c r="B973" s="1"/>
+      <c r="C973" s="1"/>
+      <c r="D973" s="1"/>
+      <c r="E973" s="1" t="s">
         <v>8238</v>
       </c>
-      <c r="F973" s="16">
+      <c r="F973" s="17">
         <v>22706</v>
       </c>
-      <c r="G973" s="11" t="s">
+      <c r="G973" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H973" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J973" s="17">
+      <c r="I973" s="1" t="s">
+        <v>8337</v>
+      </c>
+      <c r="J973" s="15">
         <v>9435185211</v>
       </c>
-      <c r="K973" t="s">
+      <c r="K973" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
     <row r="974" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="E974" s="11" t="s">
+      <c r="A974" s="1"/>
+      <c r="B974" s="1"/>
+      <c r="C974" s="1"/>
+      <c r="D974" s="1"/>
+      <c r="E974" s="1" t="s">
         <v>8240</v>
       </c>
-      <c r="F974" s="16">
+      <c r="F974" s="17">
         <v>22288</v>
       </c>
-      <c r="G974" s="11" t="s">
+      <c r="G974" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H974" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J974" s="17">
+      <c r="I974" s="1" t="s">
+        <v>8338</v>
+      </c>
+      <c r="J974" s="15">
         <v>9435007601</v>
       </c>
-      <c r="K974" t="s">
+      <c r="K974" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
     <row r="975" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="E975" s="11" t="s">
+      <c r="A975" s="1"/>
+      <c r="B975" s="1"/>
+      <c r="C975" s="1"/>
+      <c r="D975" s="1"/>
+      <c r="E975" s="1" t="s">
         <v>8241</v>
       </c>
-      <c r="F975" s="16">
+      <c r="F975" s="17">
         <v>21620</v>
       </c>
-      <c r="G975" s="11" t="s">
+      <c r="G975" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H975" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J975" s="17">
+      <c r="I975" s="1" t="s">
+        <v>8339</v>
+      </c>
+      <c r="J975" s="15">
         <v>7086329911</v>
       </c>
-      <c r="K975" t="s">
+      <c r="K975" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
     <row r="976" spans="1:21" ht="120" x14ac:dyDescent="0.25">
-      <c r="E976" s="11" t="s">
+      <c r="A976" s="1"/>
+      <c r="B976" s="1"/>
+      <c r="C976" s="1"/>
+      <c r="D976" s="1"/>
+      <c r="E976" s="1" t="s">
         <v>8242</v>
       </c>
-      <c r="F976" s="16">
+      <c r="F976" s="17">
         <v>23798</v>
       </c>
-      <c r="G976" s="11" t="s">
+      <c r="G976" s="1" t="s">
         <v>8243</v>
       </c>
       <c r="H976" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J976" s="17">
+      <c r="I976" s="1" t="s">
+        <v>8340</v>
+      </c>
+      <c r="J976" s="15">
         <v>9435749321</v>
       </c>
-      <c r="K976" t="s">
+      <c r="K976" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="977" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E977" s="11" t="s">
+    <row r="977" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A977" s="1"/>
+      <c r="B977" s="1"/>
+      <c r="C977" s="1"/>
+      <c r="D977" s="1"/>
+      <c r="E977" s="1" t="s">
         <v>8244</v>
       </c>
-      <c r="F977" s="16">
+      <c r="F977" s="17">
         <v>20375</v>
       </c>
-      <c r="G977" s="11" t="s">
+      <c r="G977" s="1" t="s">
         <v>8245</v>
       </c>
       <c r="H977" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J977" s="17">
+      <c r="I977" s="1" t="s">
+        <v>8341</v>
+      </c>
+      <c r="J977" s="15">
         <v>9435195118</v>
       </c>
-      <c r="K977" t="s">
+      <c r="K977" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="978" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E978" s="11" t="s">
+    <row r="978" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A978" s="1"/>
+      <c r="B978" s="1"/>
+      <c r="C978" s="1"/>
+      <c r="D978" s="1"/>
+      <c r="E978" s="1" t="s">
         <v>8246</v>
       </c>
-      <c r="F978" s="16">
+      <c r="F978" s="17">
         <v>24167</v>
       </c>
-      <c r="G978" s="11" t="s">
+      <c r="G978" s="1" t="s">
         <v>8247</v>
       </c>
       <c r="H978" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J978" s="17">
+      <c r="I978" s="1" t="s">
+        <v>8342</v>
+      </c>
+      <c r="J978" s="15">
         <v>9435110761</v>
       </c>
-      <c r="K978" t="s">
+      <c r="K978" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="979" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E979" s="11" t="s">
+    <row r="979" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A979" s="1"/>
+      <c r="B979" s="1"/>
+      <c r="C979" s="1"/>
+      <c r="D979" s="1"/>
+      <c r="E979" s="1" t="s">
         <v>8248</v>
       </c>
-      <c r="F979" s="16">
+      <c r="F979" s="17">
         <v>23429</v>
       </c>
-      <c r="G979" s="11" t="s">
+      <c r="G979" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H979" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J979" s="17">
+      <c r="I979" s="1" t="s">
+        <v>8343</v>
+      </c>
+      <c r="J979" s="15">
         <v>8638428450</v>
       </c>
-      <c r="K979" t="s">
+      <c r="K979" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="980" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E980" s="11" t="s">
+    <row r="980" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A980" s="1"/>
+      <c r="B980" s="1"/>
+      <c r="C980" s="1"/>
+      <c r="D980" s="1"/>
+      <c r="E980" s="1" t="s">
         <v>8249</v>
       </c>
-      <c r="F980" s="16">
+      <c r="F980" s="17">
         <v>23102</v>
       </c>
-      <c r="G980" s="11" t="s">
+      <c r="G980" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H980" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J980" s="17">
+      <c r="I980" s="1" t="s">
+        <v>8344</v>
+      </c>
+      <c r="J980" s="15">
         <v>9435127577</v>
       </c>
-      <c r="K980" t="s">
+      <c r="K980" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="981" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E981" s="11" t="s">
+    <row r="981" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A981" s="1"/>
+      <c r="B981" s="1"/>
+      <c r="C981" s="1"/>
+      <c r="D981" s="1"/>
+      <c r="E981" s="1" t="s">
         <v>8250</v>
       </c>
-      <c r="F981" s="16">
+      <c r="F981" s="17">
         <v>22287</v>
       </c>
-      <c r="G981" s="11" t="s">
+      <c r="G981" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H981" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J981" s="17">
+      <c r="I981" s="1" t="s">
+        <v>8345</v>
+      </c>
+      <c r="J981" s="15">
         <v>9577011722</v>
       </c>
-      <c r="K981" t="s">
+      <c r="K981" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="982" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E982" s="11" t="s">
+    <row r="982" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A982" s="1"/>
+      <c r="B982" s="1"/>
+      <c r="C982" s="1"/>
+      <c r="D982" s="1"/>
+      <c r="E982" s="1" t="s">
         <v>8251</v>
       </c>
-      <c r="F982" s="16">
+      <c r="F982" s="17">
         <v>24110</v>
       </c>
-      <c r="G982" s="11" t="s">
+      <c r="G982" s="1" t="s">
         <v>8252</v>
       </c>
       <c r="H982" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J982" s="17">
+      <c r="I982" s="1" t="s">
+        <v>8346</v>
+      </c>
+      <c r="J982" s="15">
         <v>9954425354</v>
       </c>
-      <c r="K982" t="s">
+      <c r="K982" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="983" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E983" s="11" t="s">
+    <row r="983" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A983" s="1"/>
+      <c r="B983" s="1"/>
+      <c r="C983" s="1"/>
+      <c r="D983" s="1"/>
+      <c r="E983" s="1" t="s">
         <v>8253</v>
       </c>
-      <c r="F983" s="16">
+      <c r="F983" s="17">
         <v>23224</v>
       </c>
-      <c r="G983" s="11" t="s">
+      <c r="G983" s="1" t="s">
         <v>8254</v>
       </c>
       <c r="H983" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J983" s="17"/>
-      <c r="K983" t="s">
+      <c r="I983" s="1" t="s">
+        <v>8347</v>
+      </c>
+      <c r="J983" s="15"/>
+      <c r="K983" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="984" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E984" s="11" t="s">
+    <row r="984" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A984" s="1"/>
+      <c r="B984" s="1"/>
+      <c r="C984" s="1"/>
+      <c r="D984" s="1"/>
+      <c r="E984" s="1" t="s">
         <v>8255</v>
       </c>
-      <c r="F984" s="16">
+      <c r="F984" s="17">
         <v>24166</v>
       </c>
-      <c r="G984" s="11" t="s">
+      <c r="G984" s="1" t="s">
         <v>8256</v>
       </c>
       <c r="H984" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J984" s="17">
+      <c r="I984" s="1" t="s">
+        <v>8348</v>
+      </c>
+      <c r="J984" s="15">
         <v>7002655615</v>
       </c>
-      <c r="K984" t="s">
+      <c r="K984" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="985" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E985" s="11" t="s">
+    <row r="985" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A985" s="1"/>
+      <c r="B985" s="1"/>
+      <c r="C985" s="1"/>
+      <c r="D985" s="1"/>
+      <c r="E985" s="1" t="s">
         <v>8257</v>
       </c>
-      <c r="F985" s="16">
+      <c r="F985" s="17">
         <v>24929</v>
       </c>
-      <c r="G985" s="11" t="s">
+      <c r="G985" s="1" t="s">
         <v>8258</v>
       </c>
       <c r="H985" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J985" s="17">
+      <c r="I985" s="1" t="s">
+        <v>8349</v>
+      </c>
+      <c r="J985" s="15">
         <v>9435082741</v>
       </c>
-      <c r="K985" t="s">
+      <c r="K985" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="986" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E986" s="11" t="s">
+    <row r="986" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A986" s="1"/>
+      <c r="B986" s="1"/>
+      <c r="C986" s="1"/>
+      <c r="D986" s="1"/>
+      <c r="E986" s="1" t="s">
         <v>8259</v>
       </c>
-      <c r="F986" s="16">
+      <c r="F986" s="17">
         <v>24504</v>
       </c>
-      <c r="G986" s="11" t="s">
+      <c r="G986" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H986" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J986" s="17">
+      <c r="I986" s="1" t="s">
+        <v>8350</v>
+      </c>
+      <c r="J986" s="15">
         <v>9435505584</v>
       </c>
-      <c r="K986" t="s">
+      <c r="K986" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="987" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E987" s="11" t="s">
+    <row r="987" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A987" s="1"/>
+      <c r="B987" s="1"/>
+      <c r="C987" s="1"/>
+      <c r="D987" s="1"/>
+      <c r="E987" s="1" t="s">
         <v>8260</v>
       </c>
-      <c r="F987" s="16">
+      <c r="F987" s="17">
         <v>24193</v>
       </c>
-      <c r="G987" s="11" t="s">
+      <c r="G987" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H987" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J987" s="17"/>
-      <c r="K987" t="s">
+      <c r="I987" s="1" t="s">
+        <v>8351</v>
+      </c>
+      <c r="J987" s="15"/>
+      <c r="K987" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="988" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E988" s="11" t="s">
+    <row r="988" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A988" s="1"/>
+      <c r="B988" s="1"/>
+      <c r="C988" s="1"/>
+      <c r="D988" s="1"/>
+      <c r="E988" s="1" t="s">
         <v>8261</v>
       </c>
-      <c r="F988" s="16">
+      <c r="F988" s="17">
         <v>25263</v>
       </c>
-      <c r="G988" s="11" t="s">
+      <c r="G988" s="1" t="s">
         <v>8262</v>
       </c>
       <c r="H988" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J988" s="17">
+      <c r="I988" s="1" t="s">
+        <v>8352</v>
+      </c>
+      <c r="J988" s="15">
         <v>9854289976</v>
       </c>
-      <c r="K988" t="s">
+      <c r="K988" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="989" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E989" s="11" t="s">
+    <row r="989" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A989" s="1"/>
+      <c r="B989" s="1"/>
+      <c r="C989" s="1"/>
+      <c r="D989" s="1"/>
+      <c r="E989" s="1" t="s">
         <v>8263</v>
       </c>
-      <c r="F989" s="16">
+      <c r="F989" s="17">
         <v>24286</v>
       </c>
-      <c r="G989" s="11" t="s">
+      <c r="G989" s="1" t="s">
         <v>8264</v>
       </c>
       <c r="H989" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J989" s="17">
+      <c r="I989" s="1" t="s">
+        <v>8353</v>
+      </c>
+      <c r="J989" s="15">
         <v>7002852103</v>
       </c>
-      <c r="K989" t="s">
+      <c r="K989" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="990" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E990" s="11" t="s">
+    <row r="990" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A990" s="1"/>
+      <c r="B990" s="1"/>
+      <c r="C990" s="1"/>
+      <c r="D990" s="1"/>
+      <c r="E990" s="1" t="s">
         <v>8265</v>
       </c>
-      <c r="F990" s="16">
+      <c r="F990" s="17">
         <v>24898</v>
       </c>
-      <c r="G990" s="11" t="s">
+      <c r="G990" s="1" t="s">
         <v>8266</v>
       </c>
       <c r="H990" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J990" s="17">
+      <c r="I990" s="1" t="s">
+        <v>8354</v>
+      </c>
+      <c r="J990" s="15">
         <v>9101892538</v>
       </c>
-      <c r="K990" t="s">
+      <c r="K990" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="991" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E991" s="11" t="s">
+    <row r="991" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A991" s="1"/>
+      <c r="B991" s="1"/>
+      <c r="C991" s="1"/>
+      <c r="D991" s="1"/>
+      <c r="E991" s="1" t="s">
         <v>8267</v>
       </c>
-      <c r="F991" s="16">
+      <c r="F991" s="17">
         <v>24898</v>
       </c>
-      <c r="G991" s="11" t="s">
+      <c r="G991" s="1" t="s">
         <v>8268</v>
       </c>
       <c r="H991" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J991" s="17">
+      <c r="I991" s="1" t="s">
+        <v>8355</v>
+      </c>
+      <c r="J991" s="15">
         <v>7086409597</v>
       </c>
-      <c r="K991" t="s">
+      <c r="K991" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="992" spans="5:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="E992" s="11" t="s">
+    <row r="992" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A992" s="1"/>
+      <c r="B992" s="1"/>
+      <c r="C992" s="1"/>
+      <c r="D992" s="1"/>
+      <c r="E992" s="1" t="s">
         <v>8269</v>
       </c>
-      <c r="F992" s="16">
+      <c r="F992" s="17">
         <v>19360</v>
       </c>
-      <c r="G992" s="11" t="s">
+      <c r="G992" s="1" t="s">
         <v>8270</v>
       </c>
       <c r="H992" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J992" s="17">
+      <c r="I992" s="1" t="s">
+        <v>8356</v>
+      </c>
+      <c r="J992" s="15">
         <v>9435303966</v>
       </c>
-      <c r="K992" t="s">
+      <c r="K992" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="993" spans="5:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="E993" s="11" t="s">
+    <row r="993" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
+      <c r="C993" s="1"/>
+      <c r="D993" s="1"/>
+      <c r="E993" s="1" t="s">
         <v>8271</v>
       </c>
-      <c r="F993" s="16">
+      <c r="F993" s="17">
         <v>25263</v>
       </c>
-      <c r="G993" s="11" t="s">
+      <c r="G993" s="1" t="s">
         <v>8272</v>
       </c>
       <c r="H993" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J993" s="17"/>
-      <c r="K993" t="s">
+      <c r="I993" s="1" t="s">
+        <v>8357</v>
+      </c>
+      <c r="J993" s="15"/>
+      <c r="K993" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="994" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E994" s="11" t="s">
+    <row r="994" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+      <c r="D994" s="1"/>
+      <c r="E994" s="1" t="s">
         <v>8273</v>
       </c>
-      <c r="F994" s="16">
+      <c r="F994" s="17">
         <v>24926</v>
       </c>
-      <c r="G994" s="11" t="s">
+      <c r="G994" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H994" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J994" s="17">
+      <c r="I994" s="1" t="s">
+        <v>8358</v>
+      </c>
+      <c r="J994" s="15">
         <v>9419011945</v>
       </c>
-      <c r="K994" t="s">
+      <c r="K994" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="995" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E995" s="11" t="s">
+    <row r="995" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A995" s="1"/>
+      <c r="B995" s="1"/>
+      <c r="C995" s="1"/>
+      <c r="D995" s="1"/>
+      <c r="E995" s="1" t="s">
         <v>8274</v>
       </c>
-      <c r="F995" s="16">
+      <c r="F995" s="17">
         <v>25628</v>
       </c>
-      <c r="G995" s="11" t="s">
+      <c r="G995" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H995" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J995" s="17">
+      <c r="I995" s="1" t="s">
+        <v>8359</v>
+      </c>
+      <c r="J995" s="15">
         <v>9435083281</v>
       </c>
-      <c r="K995" t="s">
+      <c r="K995" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="996" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E996" s="11" t="s">
+    <row r="996" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A996" s="1"/>
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+      <c r="D996" s="1"/>
+      <c r="E996" s="1" t="s">
         <v>8275</v>
       </c>
-      <c r="F996" s="16">
+      <c r="F996" s="17">
         <v>26682</v>
       </c>
-      <c r="G996" s="11" t="s">
+      <c r="G996" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H996" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J996" s="17"/>
-      <c r="K996" t="s">
+      <c r="I996" s="1" t="s">
+        <v>8360</v>
+      </c>
+      <c r="J996" s="15"/>
+      <c r="K996" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="997" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E997" s="11" t="s">
+    <row r="997" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="1"/>
+      <c r="E997" s="1" t="s">
         <v>8276</v>
       </c>
-      <c r="F997" s="16">
+      <c r="F997" s="17">
         <v>27082</v>
       </c>
-      <c r="G997" s="11" t="s">
+      <c r="G997" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H997" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J997" s="17"/>
-      <c r="K997" t="s">
+      <c r="I997" s="1" t="s">
+        <v>8361</v>
+      </c>
+      <c r="J997" s="15"/>
+      <c r="K997" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="998" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E998" s="11" t="s">
+    <row r="998" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="1"/>
+      <c r="E998" s="1" t="s">
         <v>8277</v>
       </c>
-      <c r="F998" s="16">
+      <c r="F998" s="17">
         <v>27049</v>
       </c>
-      <c r="G998" s="11" t="s">
+      <c r="G998" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H998" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J998" s="17">
+      <c r="I998" s="1" t="s">
+        <v>8362</v>
+      </c>
+      <c r="J998" s="15">
         <v>8811014787</v>
       </c>
-      <c r="K998" t="s">
+      <c r="K998" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="999" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E999" s="11" t="s">
+    <row r="999" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="1"/>
+      <c r="E999" s="1" t="s">
         <v>8278</v>
       </c>
-      <c r="F999" s="16">
+      <c r="F999" s="17">
         <v>27287</v>
       </c>
-      <c r="G999" s="11" t="s">
+      <c r="G999" s="1" t="s">
         <v>8279</v>
       </c>
       <c r="H999" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J999" s="17">
+      <c r="I999" s="1" t="s">
+        <v>8363</v>
+      </c>
+      <c r="J999" s="15">
         <v>8837262227</v>
       </c>
-      <c r="K999" t="s">
+      <c r="K999" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1000" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1000" s="11" t="s">
+    <row r="1000" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1" t="s">
         <v>8280</v>
       </c>
-      <c r="F1000" s="16">
+      <c r="F1000" s="17">
         <v>27504</v>
       </c>
-      <c r="G1000" s="11" t="s">
+      <c r="G1000" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1000" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1000" s="17">
+      <c r="I1000" s="1" t="s">
+        <v>8364</v>
+      </c>
+      <c r="J1000" s="15">
         <v>9854047807</v>
       </c>
-      <c r="K1000" t="s">
+      <c r="K1000" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1001" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1001" s="11" t="s">
+    <row r="1001" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1" t="s">
         <v>8281</v>
       </c>
-      <c r="F1001" s="16">
+      <c r="F1001" s="17">
         <v>25902</v>
       </c>
-      <c r="G1001" s="11" t="s">
+      <c r="G1001" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1001" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1001" s="17">
+      <c r="I1001" s="1" t="s">
+        <v>8365</v>
+      </c>
+      <c r="J1001" s="15">
         <v>8011785954</v>
       </c>
-      <c r="K1001" t="s">
+      <c r="K1001" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1002" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1002" s="11" t="s">
+    <row r="1002" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1" t="s">
         <v>8282</v>
       </c>
-      <c r="F1002" s="16">
+      <c r="F1002" s="17">
         <v>26011</v>
       </c>
-      <c r="G1002" s="11" t="s">
+      <c r="G1002" s="1" t="s">
         <v>8283</v>
       </c>
       <c r="H1002" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1002" s="17">
+      <c r="I1002" s="1" t="s">
+        <v>8366</v>
+      </c>
+      <c r="J1002" s="15">
         <v>9435702388</v>
       </c>
-      <c r="K1002" t="s">
+      <c r="K1002" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1003" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1003" s="11" t="s">
+    <row r="1003" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1" t="s">
         <v>8284</v>
       </c>
-      <c r="F1003" s="16">
+      <c r="F1003" s="17">
         <v>27334</v>
       </c>
-      <c r="G1003" s="11" t="s">
+      <c r="G1003" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1003" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1003" s="17">
+      <c r="I1003" s="1" t="s">
+        <v>8367</v>
+      </c>
+      <c r="J1003" s="15">
         <v>8753885884</v>
       </c>
-      <c r="K1003" t="s">
+      <c r="K1003" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1004" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1004" s="11" t="s">
+    <row r="1004" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1" t="s">
         <v>8285</v>
       </c>
-      <c r="F1004" s="16">
+      <c r="F1004" s="17">
         <v>26724</v>
       </c>
-      <c r="G1004" s="11" t="s">
+      <c r="G1004" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1004" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1004" s="17">
+      <c r="I1004" s="1" t="s">
+        <v>8368</v>
+      </c>
+      <c r="J1004" s="15">
         <v>9435041951</v>
       </c>
-      <c r="K1004" t="s">
+      <c r="K1004" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1005" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E1005" s="11" t="s">
+    <row r="1005" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1" t="s">
         <v>8286</v>
       </c>
-      <c r="F1005" s="16">
+      <c r="F1005" s="17">
         <v>27426</v>
       </c>
-      <c r="G1005" s="11" t="s">
+      <c r="G1005" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1005" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1005" s="17">
+      <c r="I1005" s="1" t="s">
+        <v>8369</v>
+      </c>
+      <c r="J1005" s="15">
         <v>8402046333</v>
       </c>
-      <c r="K1005" t="s">
+      <c r="K1005" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1006" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1006" s="11" t="s">
+    <row r="1006" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1" t="s">
         <v>8287</v>
       </c>
-      <c r="F1006" s="16">
+      <c r="F1006" s="17">
         <v>26724</v>
       </c>
-      <c r="G1006" s="11" t="s">
+      <c r="G1006" s="1" t="s">
         <v>8288</v>
       </c>
       <c r="H1006" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1006" s="17">
+      <c r="I1006" s="1" t="s">
+        <v>8370</v>
+      </c>
+      <c r="J1006" s="15">
         <v>7002585745</v>
       </c>
-      <c r="K1006" t="s">
+      <c r="K1006" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1007" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E1007" s="11" t="s">
+    <row r="1007" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="1" t="s">
         <v>8289</v>
       </c>
-      <c r="F1007" s="16">
+      <c r="F1007" s="17">
         <v>25993</v>
       </c>
-      <c r="G1007" s="11" t="s">
+      <c r="G1007" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1007" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1007" s="17">
+      <c r="I1007" s="1" t="s">
+        <v>8371</v>
+      </c>
+      <c r="J1007" s="15">
         <v>9435182806</v>
       </c>
-      <c r="K1007" t="s">
+      <c r="K1007" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1008" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1008" s="11" t="s">
+    <row r="1008" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="1" t="s">
         <v>8290</v>
       </c>
-      <c r="F1008" s="16">
+      <c r="F1008" s="17">
         <v>24926</v>
       </c>
-      <c r="G1008" s="11" t="s">
+      <c r="G1008" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1008" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1008" s="17">
+      <c r="I1008" s="1" t="s">
+        <v>8372</v>
+      </c>
+      <c r="J1008" s="15">
         <v>9435125082</v>
       </c>
-      <c r="K1008" t="s">
+      <c r="K1008" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1009" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E1009" s="11" t="s">
+    <row r="1009" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="1" t="s">
         <v>8291</v>
       </c>
-      <c r="F1009" s="16">
+      <c r="F1009" s="17">
         <v>27072</v>
       </c>
-      <c r="G1009" s="11" t="s">
+      <c r="G1009" s="1" t="s">
         <v>8292</v>
       </c>
       <c r="H1009" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1009" s="17">
+      <c r="I1009" s="1" t="s">
+        <v>8373</v>
+      </c>
+      <c r="J1009" s="15">
         <v>7002324548</v>
       </c>
-      <c r="K1009" t="s">
+      <c r="K1009" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1010" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1010" s="11" t="s">
+    <row r="1010" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="1" t="s">
         <v>8293</v>
       </c>
-      <c r="F1010" s="16">
+      <c r="F1010" s="17">
         <v>27791</v>
       </c>
-      <c r="G1010" s="11" t="s">
+      <c r="G1010" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1010" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1010" s="17">
+      <c r="I1010" s="1" t="s">
+        <v>8374</v>
+      </c>
+      <c r="J1010" s="15">
         <v>8473906605</v>
       </c>
-      <c r="K1010" t="s">
+      <c r="K1010" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1011" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1011" s="11" t="s">
+    <row r="1011" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="1"/>
+      <c r="E1011" s="1" t="s">
         <v>8294</v>
       </c>
-      <c r="F1011" s="16">
+      <c r="F1011" s="17">
         <v>27608</v>
       </c>
-      <c r="G1011" s="11" t="s">
+      <c r="G1011" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1011" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1011" s="17"/>
-      <c r="K1011" t="s">
+      <c r="I1011" s="1" t="s">
+        <v>8375</v>
+      </c>
+      <c r="J1011" s="15"/>
+      <c r="K1011" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1012" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1012" s="11" t="s">
+    <row r="1012" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="1"/>
+      <c r="E1012" s="1" t="s">
         <v>8295</v>
       </c>
-      <c r="F1012" s="16">
+      <c r="F1012" s="17">
         <v>27691</v>
       </c>
-      <c r="G1012" s="11" t="s">
+      <c r="G1012" s="1" t="s">
         <v>8296</v>
       </c>
       <c r="H1012" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1012" s="17">
+      <c r="I1012" s="1" t="s">
+        <v>8376</v>
+      </c>
+      <c r="J1012" s="15">
         <v>8981558104</v>
       </c>
-      <c r="K1012" t="s">
+      <c r="K1012" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1013" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1013" s="11" t="s">
+    <row r="1013" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="1"/>
+      <c r="E1013" s="1" t="s">
         <v>8297</v>
       </c>
-      <c r="F1013" s="16">
+      <c r="F1013" s="17">
         <v>26944</v>
       </c>
-      <c r="G1013" s="11" t="s">
+      <c r="G1013" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1013" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1013" s="17">
+      <c r="I1013" s="1" t="s">
+        <v>8377</v>
+      </c>
+      <c r="J1013" s="15">
         <v>9401057456</v>
       </c>
-      <c r="K1013" t="s">
+      <c r="K1013" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1014" spans="5:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E1014" s="11" t="s">
+    <row r="1014" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+      <c r="D1014" s="1"/>
+      <c r="E1014" s="1" t="s">
         <v>8298</v>
       </c>
-      <c r="F1014" s="16">
+      <c r="F1014" s="17">
         <v>27023</v>
       </c>
-      <c r="G1014" s="11" t="s">
+      <c r="G1014" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1014" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1014" s="17">
+      <c r="I1014" s="1" t="s">
+        <v>8378</v>
+      </c>
+      <c r="J1014" s="15">
         <v>9818941573</v>
       </c>
-      <c r="K1014" t="s">
+      <c r="K1014" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1015" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1015" s="11" t="s">
+    <row r="1015" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="1"/>
+      <c r="E1015" s="1" t="s">
         <v>8299</v>
       </c>
-      <c r="F1015" s="16">
+      <c r="F1015" s="17">
         <v>27819</v>
       </c>
-      <c r="G1015" s="11" t="s">
+      <c r="G1015" s="1" t="s">
         <v>8300</v>
       </c>
       <c r="H1015" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1015" s="17">
+      <c r="I1015" s="1" t="s">
+        <v>8379</v>
+      </c>
+      <c r="J1015" s="15">
         <v>9854243438</v>
       </c>
-      <c r="K1015" t="s">
+      <c r="K1015" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1016" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1016" s="11" t="s">
+    <row r="1016" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+      <c r="E1016" s="1" t="s">
         <v>8301</v>
       </c>
-      <c r="F1016" s="16">
+      <c r="F1016" s="17">
         <v>28185</v>
       </c>
-      <c r="G1016" s="11" t="s">
+      <c r="G1016" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1016" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1016" s="17"/>
-      <c r="K1016" t="s">
+      <c r="I1016" s="1" t="s">
+        <v>8380</v>
+      </c>
+      <c r="J1016" s="15"/>
+      <c r="K1016" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1017" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1017" s="11" t="s">
+    <row r="1017" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1017" s="1"/>
+      <c r="B1017" s="1"/>
+      <c r="C1017" s="1"/>
+      <c r="D1017" s="1"/>
+      <c r="E1017" s="1" t="s">
         <v>8302</v>
       </c>
-      <c r="F1017" s="16">
+      <c r="F1017" s="17">
         <v>27638</v>
       </c>
-      <c r="G1017" s="11" t="s">
+      <c r="G1017" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1017" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1017" s="17"/>
-      <c r="K1017" t="s">
+      <c r="I1017" s="1" t="s">
+        <v>8381</v>
+      </c>
+      <c r="J1017" s="15"/>
+      <c r="K1017" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1018" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1018" s="11" t="s">
+    <row r="1018" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="1"/>
+      <c r="C1018" s="1"/>
+      <c r="D1018" s="1"/>
+      <c r="E1018" s="1" t="s">
         <v>8303</v>
       </c>
-      <c r="F1018" s="16">
+      <c r="F1018" s="17">
         <v>28156</v>
       </c>
-      <c r="G1018" s="11" t="s">
+      <c r="G1018" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1018" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1018" s="17"/>
-      <c r="K1018" t="s">
+      <c r="I1018" s="1" t="s">
+        <v>8382</v>
+      </c>
+      <c r="J1018" s="15"/>
+      <c r="K1018" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1019" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1019" s="11" t="s">
+    <row r="1019" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="1"/>
+      <c r="C1019" s="1"/>
+      <c r="D1019" s="1"/>
+      <c r="E1019" s="1" t="s">
         <v>8304</v>
       </c>
-      <c r="F1019" s="16">
+      <c r="F1019" s="17">
         <v>27682</v>
       </c>
-      <c r="G1019" s="11" t="s">
+      <c r="G1019" s="1" t="s">
         <v>8305</v>
       </c>
       <c r="H1019" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1019" s="17">
+      <c r="I1019" s="1" t="s">
+        <v>8383</v>
+      </c>
+      <c r="J1019" s="15">
         <v>7002039865</v>
       </c>
-      <c r="K1019" t="s">
+      <c r="K1019" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1020" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1020" s="11" t="s">
+    <row r="1020" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="1"/>
+      <c r="C1020" s="1"/>
+      <c r="D1020" s="1"/>
+      <c r="E1020" s="1" t="s">
         <v>8306</v>
       </c>
-      <c r="F1020" s="16">
+      <c r="F1020" s="17">
         <v>29027</v>
       </c>
-      <c r="G1020" s="11" t="s">
+      <c r="G1020" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1020" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1020" s="17">
+      <c r="I1020" s="1" t="s">
+        <v>8384</v>
+      </c>
+      <c r="J1020" s="15">
         <v>9866421693</v>
       </c>
-      <c r="K1020" t="s">
+      <c r="K1020" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1021" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1021" s="11" t="s">
+    <row r="1021" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="1"/>
+      <c r="E1021" s="1" t="s">
         <v>8307</v>
       </c>
-      <c r="F1021" s="16">
+      <c r="F1021" s="17">
         <v>29646</v>
       </c>
-      <c r="G1021" s="11" t="s">
+      <c r="G1021" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1021" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1021" s="17"/>
-      <c r="K1021" t="s">
+      <c r="I1021" s="1" t="s">
+        <v>8385</v>
+      </c>
+      <c r="J1021" s="15"/>
+      <c r="K1021" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1022" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1022" s="11" t="s">
+    <row r="1022" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="1"/>
+      <c r="E1022" s="1" t="s">
         <v>8308</v>
       </c>
-      <c r="F1022" s="16">
+      <c r="F1022" s="17">
         <v>29281</v>
       </c>
-      <c r="G1022" s="11" t="s">
+      <c r="G1022" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1022" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1022" s="17"/>
-      <c r="K1022" t="s">
+      <c r="I1022" s="1" t="s">
+        <v>8386</v>
+      </c>
+      <c r="J1022" s="15"/>
+      <c r="K1022" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1023" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1023" s="11" t="s">
+    <row r="1023" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="1"/>
+      <c r="E1023" s="1" t="s">
         <v>8309</v>
       </c>
-      <c r="F1023" s="16">
+      <c r="F1023" s="17">
         <v>31803</v>
       </c>
-      <c r="G1023" s="11" t="s">
+      <c r="G1023" s="1" t="s">
         <v>8239</v>
       </c>
       <c r="H1023" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1023" s="17"/>
-      <c r="K1023" t="s">
+      <c r="I1023" s="1" t="s">
+        <v>8387</v>
+      </c>
+      <c r="J1023" s="15"/>
+      <c r="K1023" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1024" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1024" s="11" t="s">
+    <row r="1024" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="1"/>
+      <c r="E1024" s="1" t="s">
         <v>8310</v>
       </c>
-      <c r="F1024" s="16">
+      <c r="F1024" s="17">
         <v>25628</v>
       </c>
-      <c r="G1024" s="11" t="s">
+      <c r="G1024" s="1" t="s">
         <v>8311</v>
       </c>
       <c r="H1024" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1024" s="17">
+      <c r="I1024" s="1" t="s">
+        <v>8388</v>
+      </c>
+      <c r="J1024" s="15">
         <v>8473085326</v>
       </c>
-      <c r="K1024" t="s">
+      <c r="K1024" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1025" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E1025" s="11" t="s">
+    <row r="1025" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="1"/>
+      <c r="E1025" s="1" t="s">
         <v>8312</v>
       </c>
-      <c r="F1025" s="16">
+      <c r="F1025" s="17">
         <v>34360</v>
       </c>
-      <c r="G1025" s="11" t="s">
+      <c r="G1025" s="1" t="s">
         <v>8313</v>
       </c>
       <c r="H1025" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1025" s="17">
+      <c r="I1025" s="1" t="s">
+        <v>8389</v>
+      </c>
+      <c r="J1025" s="15">
         <v>7002739184</v>
       </c>
-      <c r="K1025" t="s">
+      <c r="K1025" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1026" spans="5:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E1026" s="11" t="s">
+    <row r="1026" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1"/>
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+      <c r="E1026" s="1" t="s">
         <v>8314</v>
       </c>
-      <c r="F1026" s="16">
+      <c r="F1026" s="17">
         <v>34366</v>
       </c>
-      <c r="G1026" s="11" t="s">
+      <c r="G1026" s="1" t="s">
         <v>8315</v>
       </c>
       <c r="H1026" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1026" s="17">
+      <c r="I1026" s="1" t="s">
+        <v>8390</v>
+      </c>
+      <c r="J1026" s="15">
         <v>9707989486</v>
       </c>
-      <c r="K1026" t="s">
+      <c r="K1026" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1027" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1027" s="11" t="s">
+    <row r="1027" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="1"/>
+      <c r="C1027" s="1"/>
+      <c r="D1027" s="1"/>
+      <c r="E1027" s="1" t="s">
         <v>8316</v>
       </c>
-      <c r="F1027" s="16"/>
-      <c r="G1027" s="11" t="s">
+      <c r="F1027" s="17"/>
+      <c r="G1027" s="1" t="s">
         <v>8317</v>
       </c>
       <c r="H1027" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1027" s="17">
+      <c r="I1027" s="1" t="s">
+        <v>8391</v>
+      </c>
+      <c r="J1027" s="15">
         <v>7086644885</v>
       </c>
-      <c r="K1027" t="s">
+      <c r="K1027" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1028" spans="5:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="E1028" s="11" t="s">
+    <row r="1028" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+      <c r="E1028" s="1" t="s">
         <v>8318</v>
       </c>
-      <c r="F1028" s="16">
+      <c r="F1028" s="17">
         <v>35751</v>
       </c>
-      <c r="G1028" s="11" t="s">
+      <c r="G1028" s="1" t="s">
         <v>8319</v>
       </c>
       <c r="H1028" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1028" s="17">
+      <c r="I1028" s="1" t="s">
+        <v>8392</v>
+      </c>
+      <c r="J1028" s="15">
         <v>8638086379</v>
       </c>
-      <c r="K1028" t="s">
+      <c r="K1028" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1029" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1029" s="11" t="s">
+    <row r="1029" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+      <c r="E1029" s="1" t="s">
         <v>8320</v>
       </c>
-      <c r="F1029" s="16">
+      <c r="F1029" s="17">
         <v>35363</v>
       </c>
-      <c r="G1029" s="11" t="s">
+      <c r="G1029" s="1" t="s">
         <v>8321</v>
       </c>
       <c r="H1029" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1029" s="17">
+      <c r="I1029" s="1" t="s">
+        <v>8393</v>
+      </c>
+      <c r="J1029" s="15">
         <v>8486568013</v>
       </c>
-      <c r="K1029" t="s">
+      <c r="K1029" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1030" spans="5:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="E1030" s="11" t="s">
+    <row r="1030" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+      <c r="E1030" s="1" t="s">
         <v>8322</v>
       </c>
-      <c r="F1030" s="16">
+      <c r="F1030" s="17">
         <v>35474</v>
       </c>
-      <c r="G1030" s="11" t="s">
+      <c r="G1030" s="1" t="s">
         <v>8323</v>
       </c>
       <c r="H1030" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1030" s="17">
+      <c r="I1030" s="1" t="s">
+        <v>8394</v>
+      </c>
+      <c r="J1030" s="15">
         <v>9085388367</v>
       </c>
-      <c r="K1030" t="s">
+      <c r="K1030" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1031" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1031" s="11" t="s">
+    <row r="1031" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1" t="s">
         <v>8324</v>
       </c>
-      <c r="F1031" s="16">
+      <c r="F1031" s="17">
         <v>35080</v>
       </c>
-      <c r="G1031" s="11" t="s">
+      <c r="G1031" s="1" t="s">
         <v>8325</v>
       </c>
       <c r="H1031" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1031" s="17">
+      <c r="I1031" s="1" t="s">
+        <v>8395</v>
+      </c>
+      <c r="J1031" s="15">
         <v>8822340659</v>
       </c>
-      <c r="K1031" t="s">
+      <c r="K1031" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1032" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1032" s="11" t="s">
+    <row r="1032" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1032" s="1"/>
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+      <c r="E1032" s="1" t="s">
         <v>8326</v>
       </c>
-      <c r="F1032" s="16">
+      <c r="F1032" s="17">
         <v>35869</v>
       </c>
-      <c r="G1032" s="11" t="s">
+      <c r="G1032" s="1" t="s">
         <v>8327</v>
       </c>
       <c r="H1032" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1032" s="17">
+      <c r="I1032" s="1" t="s">
+        <v>8396</v>
+      </c>
+      <c r="J1032" s="15">
         <v>8135949992</v>
       </c>
-      <c r="K1032" t="s">
+      <c r="K1032" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1033" spans="5:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E1033" s="11" t="s">
+    <row r="1033" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1033" s="1"/>
+      <c r="B1033" s="1"/>
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+      <c r="E1033" s="1" t="s">
         <v>8328</v>
       </c>
-      <c r="F1033" s="16">
+      <c r="F1033" s="17">
         <v>35861</v>
       </c>
-      <c r="G1033" s="11" t="s">
+      <c r="G1033" s="1" t="s">
         <v>8329</v>
       </c>
       <c r="H1033" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1033" s="17">
+      <c r="I1033" s="1" t="s">
+        <v>8397</v>
+      </c>
+      <c r="J1033" s="15">
         <v>9101370189</v>
       </c>
-      <c r="K1033" t="s">
+      <c r="K1033" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1034" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1034" s="11" t="s">
+    <row r="1034" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1034" s="1"/>
+      <c r="B1034" s="1"/>
+      <c r="C1034" s="1"/>
+      <c r="D1034" s="1"/>
+      <c r="E1034" s="1" t="s">
         <v>8330</v>
       </c>
-      <c r="F1034" s="16">
+      <c r="F1034" s="17">
         <v>35828</v>
       </c>
-      <c r="G1034" s="11" t="s">
+      <c r="G1034" s="1" t="s">
         <v>8331</v>
       </c>
       <c r="H1034" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1034" s="17">
+      <c r="I1034" s="1" t="s">
+        <v>8398</v>
+      </c>
+      <c r="J1034" s="15">
         <v>9101126144</v>
       </c>
-      <c r="K1034" t="s">
+      <c r="K1034" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1035" spans="5:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="E1035" s="11" t="s">
+    <row r="1035" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1035" s="1"/>
+      <c r="B1035" s="1"/>
+      <c r="C1035" s="1"/>
+      <c r="D1035" s="1"/>
+      <c r="E1035" s="1" t="s">
         <v>8332</v>
       </c>
-      <c r="F1035" s="16">
+      <c r="F1035" s="17">
         <v>36011</v>
       </c>
-      <c r="G1035" s="11" t="s">
+      <c r="G1035" s="1" t="s">
         <v>8333</v>
       </c>
       <c r="H1035" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1035" s="17">
+      <c r="I1035" s="1" t="s">
+        <v>8399</v>
+      </c>
+      <c r="J1035" s="15">
         <v>6000925311</v>
       </c>
-      <c r="K1035" t="s">
+      <c r="K1035" s="1" t="s">
         <v>8334</v>
       </c>
     </row>
-    <row r="1036" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="H1036" s="18"/>
-    </row>
-    <row r="1037" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="H1037" s="18"/>
+    <row r="1036" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1036" s="16"/>
+    </row>
+    <row r="1037" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H1037" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added portion of the ivpr numbers
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -14247,8 +14247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1159" sqref="B1159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49536,9 +49536,15 @@
     </row>
     <row r="1098" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1098" s="10"/>
-      <c r="B1098" s="10"/>
-      <c r="C1098" s="10"/>
-      <c r="D1098" s="10"/>
+      <c r="B1098" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1098" s="10">
+        <v>834</v>
+      </c>
+      <c r="D1098" s="10">
+        <v>397</v>
+      </c>
       <c r="E1098" s="10" t="s">
         <v>4221</v>
       </c>
@@ -49563,9 +49569,15 @@
     </row>
     <row r="1099" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1099" s="10"/>
-      <c r="B1099" s="10"/>
-      <c r="C1099" s="10"/>
-      <c r="D1099" s="10"/>
+      <c r="B1099" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1099" s="10">
+        <v>4692</v>
+      </c>
+      <c r="D1099" s="10">
+        <v>597</v>
+      </c>
       <c r="E1099" s="10" t="s">
         <v>4222</v>
       </c>
@@ -49588,9 +49600,15 @@
     </row>
     <row r="1100" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1100" s="10"/>
-      <c r="B1100" s="10"/>
-      <c r="C1100" s="10"/>
-      <c r="D1100" s="10"/>
+      <c r="B1100" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1100" s="10">
+        <v>1174</v>
+      </c>
+      <c r="D1100" s="10">
+        <v>415</v>
+      </c>
       <c r="E1100" s="10" t="s">
         <v>4223</v>
       </c>
@@ -49615,9 +49633,15 @@
     </row>
     <row r="1101" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1101" s="10"/>
-      <c r="B1101" s="10"/>
-      <c r="C1101" s="10"/>
-      <c r="D1101" s="10"/>
+      <c r="B1101" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1101" s="10">
+        <v>508</v>
+      </c>
+      <c r="D1101" s="10">
+        <v>539</v>
+      </c>
       <c r="E1101" s="10" t="s">
         <v>4224</v>
       </c>
@@ -49642,9 +49666,15 @@
     </row>
     <row r="1102" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1102" s="10"/>
-      <c r="B1102" s="10"/>
-      <c r="C1102" s="10"/>
-      <c r="D1102" s="10"/>
+      <c r="B1102" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1102" s="10">
+        <v>738</v>
+      </c>
+      <c r="D1102" s="10">
+        <v>551</v>
+      </c>
       <c r="E1102" s="10" t="s">
         <v>4225</v>
       </c>
@@ -49669,9 +49699,15 @@
     </row>
     <row r="1103" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1103" s="10"/>
-      <c r="B1103" s="10"/>
-      <c r="C1103" s="10"/>
-      <c r="D1103" s="10"/>
+      <c r="B1103" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1103" s="10">
+        <v>548</v>
+      </c>
+      <c r="D1103" s="10">
+        <v>541</v>
+      </c>
       <c r="E1103" s="10" t="s">
         <v>4226</v>
       </c>
@@ -49696,9 +49732,15 @@
     </row>
     <row r="1104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1104" s="10"/>
-      <c r="B1104" s="10"/>
-      <c r="C1104" s="10"/>
-      <c r="D1104" s="10"/>
+      <c r="B1104" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1104" s="10">
+        <v>648</v>
+      </c>
+      <c r="D1104" s="10">
+        <v>546</v>
+      </c>
       <c r="E1104" s="10" t="s">
         <v>4227</v>
       </c>
@@ -49723,9 +49765,15 @@
     </row>
     <row r="1105" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1105" s="10"/>
-      <c r="B1105" s="10"/>
-      <c r="C1105" s="10"/>
-      <c r="D1105" s="10"/>
+      <c r="B1105" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1105" s="10">
+        <v>1271</v>
+      </c>
+      <c r="D1105" s="10">
+        <v>579</v>
+      </c>
       <c r="E1105" s="10" t="s">
         <v>4228</v>
       </c>
@@ -49750,9 +49798,15 @@
     </row>
     <row r="1106" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1106" s="10"/>
-      <c r="B1106" s="10"/>
-      <c r="C1106" s="10"/>
-      <c r="D1106" s="10"/>
+      <c r="B1106" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1106" s="10">
+        <v>503</v>
+      </c>
+      <c r="D1106" s="10">
+        <v>539</v>
+      </c>
       <c r="E1106" s="10" t="s">
         <v>4229</v>
       </c>
@@ -49777,9 +49831,15 @@
     </row>
     <row r="1107" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1107" s="10"/>
-      <c r="B1107" s="10"/>
-      <c r="C1107" s="10"/>
-      <c r="D1107" s="10"/>
+      <c r="B1107" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1107" s="10">
+        <v>2248</v>
+      </c>
+      <c r="D1107" s="10">
+        <v>629</v>
+      </c>
       <c r="E1107" s="10" t="s">
         <v>4230</v>
       </c>
@@ -49804,9 +49864,15 @@
     </row>
     <row r="1108" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1108" s="10"/>
-      <c r="B1108" s="10"/>
-      <c r="C1108" s="10"/>
-      <c r="D1108" s="10"/>
+      <c r="B1108" s="10">
+        <v>1996</v>
+      </c>
+      <c r="C1108" s="10">
+        <v>864</v>
+      </c>
+      <c r="D1108" s="10">
+        <v>557</v>
+      </c>
       <c r="E1108" s="10" t="s">
         <v>4231</v>
       </c>
@@ -49881,9 +49947,15 @@
     </row>
     <row r="1111" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1111" s="10"/>
-      <c r="B1111" s="10"/>
-      <c r="C1111" s="10"/>
-      <c r="D1111" s="10"/>
+      <c r="B1111" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1111" s="10">
+        <v>908</v>
+      </c>
+      <c r="D1111" s="10">
+        <v>251</v>
+      </c>
       <c r="E1111" s="10" t="s">
         <v>4234</v>
       </c>
@@ -49935,9 +50007,15 @@
     </row>
     <row r="1113" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1113" s="10"/>
-      <c r="B1113" s="10"/>
-      <c r="C1113" s="10"/>
-      <c r="D1113" s="10"/>
+      <c r="B1113" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1113" s="10">
+        <v>2416</v>
+      </c>
+      <c r="D1113" s="10">
+        <v>352</v>
+      </c>
       <c r="E1113" s="10" t="s">
         <v>4236</v>
       </c>
@@ -49962,9 +50040,15 @@
     </row>
     <row r="1114" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1114" s="10"/>
-      <c r="B1114" s="10"/>
-      <c r="C1114" s="10"/>
-      <c r="D1114" s="10"/>
+      <c r="B1114" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1114" s="10">
+        <v>1346</v>
+      </c>
+      <c r="D1114" s="10">
+        <v>280</v>
+      </c>
       <c r="E1114" s="10" t="s">
         <v>4237</v>
       </c>
@@ -49989,9 +50073,15 @@
     </row>
     <row r="1115" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1115" s="10"/>
-      <c r="B1115" s="10"/>
-      <c r="C1115" s="10"/>
-      <c r="D1115" s="10"/>
+      <c r="B1115" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1115" s="10">
+        <v>545</v>
+      </c>
+      <c r="D1115" s="10">
+        <v>227</v>
+      </c>
       <c r="E1115" s="10" t="s">
         <v>4238</v>
       </c>
@@ -50016,9 +50106,15 @@
     </row>
     <row r="1116" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1116" s="10"/>
-      <c r="B1116" s="10"/>
-      <c r="C1116" s="10"/>
-      <c r="D1116" s="10"/>
+      <c r="B1116" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1116" s="10">
+        <v>913</v>
+      </c>
+      <c r="D1116" s="10">
+        <v>251</v>
+      </c>
       <c r="E1116" s="10" t="s">
         <v>4239</v>
       </c>
@@ -50041,9 +50137,15 @@
     </row>
     <row r="1117" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1117" s="10"/>
-      <c r="B1117" s="10"/>
-      <c r="C1117" s="10"/>
-      <c r="D1117" s="10"/>
+      <c r="B1117" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1117" s="10">
+        <v>5994</v>
+      </c>
+      <c r="D1117" s="10">
+        <v>590</v>
+      </c>
       <c r="E1117" s="10" t="s">
         <v>4240</v>
       </c>
@@ -50091,9 +50193,15 @@
     </row>
     <row r="1119" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1119" s="10"/>
-      <c r="B1119" s="10"/>
-      <c r="C1119" s="10"/>
-      <c r="D1119" s="10"/>
+      <c r="B1119" s="10">
+        <v>1998</v>
+      </c>
+      <c r="C1119" s="10">
+        <v>5991</v>
+      </c>
+      <c r="D1119" s="10">
+        <v>590</v>
+      </c>
       <c r="E1119" s="10" t="s">
         <v>4242</v>
       </c>
@@ -50116,9 +50224,15 @@
     </row>
     <row r="1120" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1120" s="10"/>
-      <c r="B1120" s="10"/>
-      <c r="C1120" s="10"/>
-      <c r="D1120" s="10"/>
+      <c r="B1120" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1120" s="10">
+        <v>497</v>
+      </c>
+      <c r="D1120" s="10">
+        <v>195</v>
+      </c>
       <c r="E1120" s="10" t="s">
         <v>4243</v>
       </c>
@@ -50143,9 +50257,15 @@
     </row>
     <row r="1121" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1121" s="10"/>
-      <c r="B1121" s="10"/>
-      <c r="C1121" s="10"/>
-      <c r="D1121" s="10"/>
+      <c r="B1121" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1121" s="10">
+        <v>324</v>
+      </c>
+      <c r="D1121" s="10">
+        <v>185</v>
+      </c>
       <c r="E1121" s="10" t="s">
         <v>4244</v>
       </c>
@@ -50168,9 +50288,15 @@
     </row>
     <row r="1122" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1122" s="10"/>
-      <c r="B1122" s="10"/>
-      <c r="C1122" s="10"/>
-      <c r="D1122" s="10"/>
+      <c r="B1122" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1122" s="10">
+        <v>1211</v>
+      </c>
+      <c r="D1122" s="10">
+        <v>237</v>
+      </c>
       <c r="E1122" s="10" t="s">
         <v>4245</v>
       </c>
@@ -50195,9 +50321,15 @@
     </row>
     <row r="1123" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1123" s="10"/>
-      <c r="B1123" s="10"/>
-      <c r="C1123" s="10"/>
-      <c r="D1123" s="10"/>
+      <c r="B1123" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1123" s="10">
+        <v>704</v>
+      </c>
+      <c r="D1123" s="10">
+        <v>207</v>
+      </c>
       <c r="E1123" s="10" t="s">
         <v>4246</v>
       </c>
@@ -50222,9 +50354,15 @@
     </row>
     <row r="1124" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1124" s="10"/>
-      <c r="B1124" s="10"/>
-      <c r="C1124" s="10"/>
-      <c r="D1124" s="10"/>
+      <c r="B1124" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1124" s="10">
+        <v>264</v>
+      </c>
+      <c r="D1124" s="10">
+        <v>181</v>
+      </c>
       <c r="E1124" s="10" t="s">
         <v>4247</v>
       </c>
@@ -50247,9 +50385,15 @@
     </row>
     <row r="1125" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1125" s="10"/>
-      <c r="B1125" s="10"/>
-      <c r="C1125" s="10"/>
-      <c r="D1125" s="10"/>
+      <c r="B1125" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1125" s="10">
+        <v>1210</v>
+      </c>
+      <c r="D1125" s="10">
+        <v>237</v>
+      </c>
       <c r="E1125" s="10" t="s">
         <v>4248</v>
       </c>
@@ -50272,9 +50416,15 @@
     </row>
     <row r="1126" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1126" s="10"/>
-      <c r="B1126" s="10"/>
-      <c r="C1126" s="10"/>
-      <c r="D1126" s="10"/>
+      <c r="B1126" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1126" s="10">
+        <v>287</v>
+      </c>
+      <c r="D1126" s="10">
+        <v>182</v>
+      </c>
       <c r="E1126" s="10" t="s">
         <v>4249</v>
       </c>
@@ -50299,9 +50449,15 @@
     </row>
     <row r="1127" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1127" s="10"/>
-      <c r="B1127" s="10"/>
-      <c r="C1127" s="10"/>
-      <c r="D1127" s="10"/>
+      <c r="B1127" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1127" s="10">
+        <v>686</v>
+      </c>
+      <c r="D1127" s="10">
+        <v>206</v>
+      </c>
       <c r="E1127" s="10" t="s">
         <v>4250</v>
       </c>
@@ -50326,9 +50482,15 @@
     </row>
     <row r="1128" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1128" s="10"/>
-      <c r="B1128" s="10"/>
-      <c r="C1128" s="10"/>
-      <c r="D1128" s="10"/>
+      <c r="B1128" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1128" s="10">
+        <v>831</v>
+      </c>
+      <c r="D1128" s="10">
+        <v>214</v>
+      </c>
       <c r="E1128" s="10" t="s">
         <v>4251</v>
       </c>
@@ -50351,9 +50513,15 @@
     </row>
     <row r="1129" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1129" s="10"/>
-      <c r="B1129" s="10"/>
-      <c r="C1129" s="10"/>
-      <c r="D1129" s="10"/>
+      <c r="B1129" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C1129" s="10">
+        <v>1829</v>
+      </c>
+      <c r="D1129" s="10">
+        <v>406</v>
+      </c>
       <c r="E1129" s="10" t="s">
         <v>4252</v>
       </c>
@@ -50378,9 +50546,15 @@
     </row>
     <row r="1130" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1130" s="10"/>
-      <c r="B1130" s="10"/>
-      <c r="C1130" s="10"/>
-      <c r="D1130" s="10"/>
+      <c r="B1130" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C1130" s="10">
+        <v>667</v>
+      </c>
+      <c r="D1130" s="10">
+        <v>300</v>
+      </c>
       <c r="E1130" s="10" t="s">
         <v>4253</v>
       </c>
@@ -50403,9 +50577,15 @@
     </row>
     <row r="1131" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1131" s="10"/>
-      <c r="B1131" s="10"/>
-      <c r="C1131" s="10"/>
-      <c r="D1131" s="10"/>
+      <c r="B1131" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1131" s="10">
+        <v>683</v>
+      </c>
+      <c r="D1131" s="10">
+        <v>262</v>
+      </c>
       <c r="E1131" s="10" t="s">
         <v>4254</v>
       </c>
@@ -50428,9 +50608,15 @@
     </row>
     <row r="1132" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1132" s="10"/>
-      <c r="B1132" s="10"/>
-      <c r="C1132" s="10"/>
-      <c r="D1132" s="10"/>
+      <c r="B1132" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1132" s="10">
+        <v>485</v>
+      </c>
+      <c r="D1132" s="10">
+        <v>246</v>
+      </c>
       <c r="E1132" s="10" t="s">
         <v>4255</v>
       </c>
@@ -50455,9 +50641,15 @@
     </row>
     <row r="1133" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1133" s="10"/>
-      <c r="B1133" s="10"/>
-      <c r="C1133" s="10"/>
-      <c r="D1133" s="10"/>
+      <c r="B1133" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1133" s="10">
+        <v>2106</v>
+      </c>
+      <c r="D1133" s="10">
+        <v>381</v>
+      </c>
       <c r="E1133" s="10" t="s">
         <v>4256</v>
       </c>
@@ -50482,9 +50674,15 @@
     </row>
     <row r="1134" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1134" s="10"/>
-      <c r="B1134" s="10"/>
-      <c r="C1134" s="10"/>
-      <c r="D1134" s="10"/>
+      <c r="B1134" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1134" s="10">
+        <v>399</v>
+      </c>
+      <c r="D1134" s="10">
+        <v>239</v>
+      </c>
       <c r="E1134" s="10" t="s">
         <v>4257</v>
       </c>
@@ -50509,9 +50707,15 @@
     </row>
     <row r="1135" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1135" s="10"/>
-      <c r="B1135" s="10"/>
-      <c r="C1135" s="10"/>
-      <c r="D1135" s="10"/>
+      <c r="B1135" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1135" s="10">
+        <v>544</v>
+      </c>
+      <c r="D1135" s="10">
+        <v>251</v>
+      </c>
       <c r="E1135" s="10" t="s">
         <v>4258</v>
       </c>
@@ -50534,9 +50738,15 @@
     </row>
     <row r="1136" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1136" s="10"/>
-      <c r="B1136" s="10"/>
-      <c r="C1136" s="10"/>
-      <c r="D1136" s="10"/>
+      <c r="B1136" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1136" s="10">
+        <v>1375</v>
+      </c>
+      <c r="D1136" s="10">
+        <v>320</v>
+      </c>
       <c r="E1136" s="10" t="s">
         <v>4259</v>
       </c>
@@ -50559,9 +50769,15 @@
     </row>
     <row r="1137" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1137" s="10"/>
-      <c r="B1137" s="10"/>
-      <c r="C1137" s="10"/>
-      <c r="D1137" s="10"/>
+      <c r="B1137" s="10">
+        <v>2001</v>
+      </c>
+      <c r="C1137" s="10">
+        <v>1508</v>
+      </c>
+      <c r="D1137" s="10">
+        <v>331</v>
+      </c>
       <c r="E1137" s="10" t="s">
         <v>4260</v>
       </c>
@@ -50586,9 +50802,15 @@
     </row>
     <row r="1138" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1138" s="10"/>
-      <c r="B1138" s="10"/>
-      <c r="C1138" s="10"/>
-      <c r="D1138" s="10"/>
+      <c r="B1138" s="10">
+        <v>2002</v>
+      </c>
+      <c r="C1138" s="10">
+        <v>569</v>
+      </c>
+      <c r="D1138" s="10">
+        <v>208</v>
+      </c>
       <c r="E1138" s="10" t="s">
         <v>4261</v>
       </c>
@@ -50613,9 +50835,15 @@
     </row>
     <row r="1139" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1139" s="10"/>
-      <c r="B1139" s="10"/>
-      <c r="C1139" s="10"/>
-      <c r="D1139" s="10"/>
+      <c r="B1139" s="10">
+        <v>2002</v>
+      </c>
+      <c r="C1139" s="10">
+        <v>320</v>
+      </c>
+      <c r="D1139" s="10">
+        <v>184</v>
+      </c>
       <c r="E1139" s="10" t="s">
         <v>4262</v>
       </c>
@@ -50640,9 +50868,15 @@
     </row>
     <row r="1140" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1140" s="10"/>
-      <c r="B1140" s="10"/>
-      <c r="C1140" s="10"/>
-      <c r="D1140" s="10"/>
+      <c r="B1140" s="10">
+        <v>2002</v>
+      </c>
+      <c r="C1140" s="10">
+        <v>37</v>
+      </c>
+      <c r="D1140" s="10">
+        <v>155</v>
+      </c>
       <c r="E1140" s="10" t="s">
         <v>4263</v>
       </c>
@@ -50665,9 +50899,15 @@
     </row>
     <row r="1141" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1141" s="10"/>
-      <c r="B1141" s="10"/>
-      <c r="C1141" s="10"/>
-      <c r="D1141" s="10"/>
+      <c r="B1141" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1141" s="10">
+        <v>203</v>
+      </c>
+      <c r="D1141" s="10">
+        <v>121</v>
+      </c>
       <c r="E1141" s="10" t="s">
         <v>4264</v>
       </c>
@@ -50692,9 +50932,15 @@
     </row>
     <row r="1142" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1142" s="10"/>
-      <c r="B1142" s="10"/>
-      <c r="C1142" s="10"/>
-      <c r="D1142" s="10"/>
+      <c r="B1142" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1142" s="10">
+        <v>376</v>
+      </c>
+      <c r="D1142" s="10">
+        <v>131</v>
+      </c>
       <c r="E1142" s="10" t="s">
         <v>4265</v>
       </c>
@@ -50717,9 +50963,15 @@
     </row>
     <row r="1143" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1143" s="10"/>
-      <c r="B1143" s="10"/>
-      <c r="C1143" s="10"/>
-      <c r="D1143" s="10"/>
+      <c r="B1143" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1143" s="10">
+        <v>1123</v>
+      </c>
+      <c r="D1143" s="10">
+        <v>176</v>
+      </c>
       <c r="E1143" s="10" t="s">
         <v>4266</v>
       </c>
@@ -50744,9 +50996,15 @@
     </row>
     <row r="1144" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1144" s="10"/>
-      <c r="B1144" s="10"/>
-      <c r="C1144" s="10"/>
-      <c r="D1144" s="10"/>
+      <c r="B1144" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1144" s="10">
+        <v>1047</v>
+      </c>
+      <c r="D1144" s="10">
+        <v>172</v>
+      </c>
       <c r="E1144" s="10" t="s">
         <v>4267</v>
       </c>
@@ -50771,9 +51029,15 @@
     </row>
     <row r="1145" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1145" s="10"/>
-      <c r="B1145" s="10"/>
-      <c r="C1145" s="10"/>
-      <c r="D1145" s="10"/>
+      <c r="B1145" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1145" s="10">
+        <v>303</v>
+      </c>
+      <c r="D1145" s="10">
+        <v>127</v>
+      </c>
       <c r="E1145" s="10" t="s">
         <v>4268</v>
       </c>
@@ -50796,9 +51060,15 @@
     </row>
     <row r="1146" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1146" s="10"/>
-      <c r="B1146" s="10"/>
-      <c r="C1146" s="10"/>
-      <c r="D1146" s="10"/>
+      <c r="B1146" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1146" s="10">
+        <v>356</v>
+      </c>
+      <c r="D1146" s="10">
+        <v>130</v>
+      </c>
       <c r="E1146" s="10" t="s">
         <v>4269</v>
       </c>
@@ -50821,9 +51091,15 @@
     </row>
     <row r="1147" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1147" s="10"/>
-      <c r="B1147" s="10"/>
-      <c r="C1147" s="10"/>
-      <c r="D1147" s="10"/>
+      <c r="B1147" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1147" s="10">
+        <v>239</v>
+      </c>
+      <c r="D1147" s="10">
+        <v>123</v>
+      </c>
       <c r="E1147" s="10" t="s">
         <v>4270</v>
       </c>
@@ -50848,9 +51124,15 @@
     </row>
     <row r="1148" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1148" s="10"/>
-      <c r="B1148" s="10"/>
-      <c r="C1148" s="10"/>
-      <c r="D1148" s="10"/>
+      <c r="B1148" s="10">
+        <v>2003</v>
+      </c>
+      <c r="C1148" s="10">
+        <v>353</v>
+      </c>
+      <c r="D1148" s="10">
+        <v>130</v>
+      </c>
       <c r="E1148" s="10" t="s">
         <v>4271</v>
       </c>
@@ -50875,9 +51157,15 @@
     </row>
     <row r="1149" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1149" s="10"/>
-      <c r="B1149" s="10"/>
-      <c r="C1149" s="10"/>
-      <c r="D1149" s="10"/>
+      <c r="B1149" s="10">
+        <v>2004</v>
+      </c>
+      <c r="C1149" s="10">
+        <v>270</v>
+      </c>
+      <c r="D1149" s="10">
+        <v>142</v>
+      </c>
       <c r="E1149" s="10" t="s">
         <v>4272</v>
       </c>
@@ -50900,9 +51188,15 @@
     </row>
     <row r="1150" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1150" s="10"/>
-      <c r="B1150" s="10"/>
-      <c r="C1150" s="10"/>
-      <c r="D1150" s="10"/>
+      <c r="B1150" s="10">
+        <v>2004</v>
+      </c>
+      <c r="C1150" s="10">
+        <v>1074</v>
+      </c>
+      <c r="D1150" s="10">
+        <v>202</v>
+      </c>
       <c r="E1150" s="10" t="s">
         <v>4273</v>
       </c>
@@ -50927,9 +51221,15 @@
     </row>
     <row r="1151" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A1151" s="10"/>
-      <c r="B1151" s="10"/>
-      <c r="C1151" s="10"/>
-      <c r="D1151" s="10"/>
+      <c r="B1151" s="10">
+        <v>2004</v>
+      </c>
+      <c r="C1151" s="10">
+        <v>289</v>
+      </c>
+      <c r="D1151" s="10">
+        <v>143</v>
+      </c>
       <c r="E1151" s="10" t="s">
         <v>4274</v>
       </c>
@@ -50954,9 +51254,15 @@
     </row>
     <row r="1152" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1152" s="10"/>
-      <c r="B1152" s="10"/>
-      <c r="C1152" s="10"/>
-      <c r="D1152" s="10"/>
+      <c r="B1152" s="10">
+        <v>2004</v>
+      </c>
+      <c r="C1152" s="10">
+        <v>205</v>
+      </c>
+      <c r="D1152" s="10">
+        <v>137</v>
+      </c>
       <c r="E1152" s="10" t="s">
         <v>4275</v>
       </c>
@@ -50981,9 +51287,15 @@
     </row>
     <row r="1153" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1153" s="10"/>
-      <c r="B1153" s="10"/>
-      <c r="C1153" s="10"/>
-      <c r="D1153" s="10"/>
+      <c r="B1153" s="10">
+        <v>2005</v>
+      </c>
+      <c r="C1153" s="10">
+        <v>141</v>
+      </c>
+      <c r="D1153" s="10">
+        <v>101</v>
+      </c>
       <c r="E1153" s="10" t="s">
         <v>4276</v>
       </c>
@@ -51006,9 +51318,15 @@
     </row>
     <row r="1154" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1154" s="10"/>
-      <c r="B1154" s="10"/>
-      <c r="C1154" s="10"/>
-      <c r="D1154" s="10"/>
+      <c r="B1154" s="10">
+        <v>2006</v>
+      </c>
+      <c r="C1154" s="10">
+        <v>446</v>
+      </c>
+      <c r="D1154" s="10">
+        <v>345</v>
+      </c>
       <c r="E1154" s="10" t="s">
         <v>4277</v>
       </c>
@@ -51033,9 +51351,15 @@
     </row>
     <row r="1155" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1155" s="10"/>
-      <c r="B1155" s="10"/>
-      <c r="C1155" s="10"/>
-      <c r="D1155" s="10"/>
+      <c r="B1155" s="10">
+        <v>2006</v>
+      </c>
+      <c r="C1155" s="10">
+        <v>3628</v>
+      </c>
+      <c r="D1155" s="10">
+        <v>634</v>
+      </c>
       <c r="E1155" s="10" t="s">
         <v>4278</v>
       </c>
@@ -51060,9 +51384,15 @@
     </row>
     <row r="1156" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1156" s="10"/>
-      <c r="B1156" s="10"/>
-      <c r="C1156" s="10"/>
-      <c r="D1156" s="10"/>
+      <c r="B1156" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1156" s="10">
+        <v>287</v>
+      </c>
+      <c r="D1156" s="10">
+        <v>304</v>
+      </c>
       <c r="E1156" s="10" t="s">
         <v>4279</v>
       </c>
@@ -51085,9 +51415,15 @@
     </row>
     <row r="1157" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1157" s="10"/>
-      <c r="B1157" s="10"/>
-      <c r="C1157" s="10"/>
-      <c r="D1157" s="10"/>
+      <c r="B1157" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1157" s="10">
+        <v>1937</v>
+      </c>
+      <c r="D1157" s="10">
+        <v>469</v>
+      </c>
       <c r="E1157" s="10" t="s">
         <v>4280</v>
       </c>
@@ -51110,9 +51446,15 @@
     </row>
     <row r="1158" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1158" s="10"/>
-      <c r="B1158" s="10"/>
-      <c r="C1158" s="10"/>
-      <c r="D1158" s="10"/>
+      <c r="B1158" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1158" s="10">
+        <v>310</v>
+      </c>
+      <c r="D1158" s="10">
+        <v>307</v>
+      </c>
       <c r="E1158" s="10" t="s">
         <v>4281</v>
       </c>

</xml_diff>

<commit_message>
completely added first set of ivpr numbers, remaining set 2
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -14247,8 +14247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1159" sqref="B1159"/>
+    <sheetView tabSelected="1" topLeftCell="A1236" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1241" sqref="L1241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51477,9 +51477,15 @@
     </row>
     <row r="1159" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1159" s="10"/>
-      <c r="B1159" s="10"/>
-      <c r="C1159" s="10"/>
-      <c r="D1159" s="10"/>
+      <c r="B1159" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1159" s="10">
+        <v>1938</v>
+      </c>
+      <c r="D1159" s="10">
+        <v>469</v>
+      </c>
       <c r="E1159" s="10" t="s">
         <v>4282</v>
       </c>
@@ -51529,9 +51535,15 @@
     </row>
     <row r="1161" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1161" s="10"/>
-      <c r="B1161" s="10"/>
-      <c r="C1161" s="10"/>
-      <c r="D1161" s="10"/>
+      <c r="B1161" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1161" s="10">
+        <v>591</v>
+      </c>
+      <c r="D1161" s="10">
+        <v>335</v>
+      </c>
       <c r="E1161" s="10" t="s">
         <v>4284</v>
       </c>
@@ -51554,9 +51566,15 @@
     </row>
     <row r="1162" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1162" s="10"/>
-      <c r="B1162" s="10"/>
-      <c r="C1162" s="10"/>
-      <c r="D1162" s="10"/>
+      <c r="B1162" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1162" s="10">
+        <v>538</v>
+      </c>
+      <c r="D1162" s="10">
+        <v>329</v>
+      </c>
       <c r="E1162" s="10" t="s">
         <v>4285</v>
       </c>
@@ -51579,9 +51597,15 @@
     </row>
     <row r="1163" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1163" s="10"/>
-      <c r="B1163" s="10"/>
-      <c r="C1163" s="10"/>
-      <c r="D1163" s="10"/>
+      <c r="B1163" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1163" s="10">
+        <v>322</v>
+      </c>
+      <c r="D1163" s="10">
+        <v>308</v>
+      </c>
       <c r="E1163" s="10" t="s">
         <v>4286</v>
       </c>
@@ -51604,9 +51628,15 @@
     </row>
     <row r="1164" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1164" s="10"/>
-      <c r="B1164" s="10"/>
-      <c r="C1164" s="10"/>
-      <c r="D1164" s="10"/>
+      <c r="B1164" s="10">
+        <v>2007</v>
+      </c>
+      <c r="C1164" s="10">
+        <v>1943</v>
+      </c>
+      <c r="D1164" s="10">
+        <v>470</v>
+      </c>
       <c r="E1164" s="10" t="s">
         <v>4287</v>
       </c>
@@ -51629,9 +51659,15 @@
     </row>
     <row r="1165" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1165" s="10"/>
-      <c r="B1165" s="10"/>
-      <c r="C1165" s="10"/>
-      <c r="D1165" s="10"/>
+      <c r="B1165" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1165" s="10">
+        <v>1501</v>
+      </c>
+      <c r="D1165" s="10">
+        <v>1974</v>
+      </c>
       <c r="E1165" s="10" t="s">
         <v>4288</v>
       </c>
@@ -51656,9 +51692,15 @@
     </row>
     <row r="1166" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1166" s="10"/>
-      <c r="B1166" s="10"/>
-      <c r="C1166" s="10"/>
-      <c r="D1166" s="10"/>
+      <c r="B1166" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1166" s="10">
+        <v>847</v>
+      </c>
+      <c r="D1166" s="10">
+        <v>1933</v>
+      </c>
       <c r="E1166" s="10" t="s">
         <v>4289</v>
       </c>
@@ -51683,9 +51725,15 @@
     </row>
     <row r="1167" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1167" s="10"/>
-      <c r="B1167" s="10"/>
-      <c r="C1167" s="10"/>
-      <c r="D1167" s="10"/>
+      <c r="B1167" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1167" s="10">
+        <v>505</v>
+      </c>
+      <c r="D1167" s="10">
+        <v>1912</v>
+      </c>
       <c r="E1167" s="10" t="s">
         <v>4290</v>
       </c>
@@ -51708,9 +51756,15 @@
     </row>
     <row r="1168" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1168" s="10"/>
-      <c r="B1168" s="10"/>
-      <c r="C1168" s="10"/>
-      <c r="D1168" s="10"/>
+      <c r="B1168" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1168" s="10">
+        <v>262</v>
+      </c>
+      <c r="D1168" s="10">
+        <v>1897</v>
+      </c>
       <c r="E1168" s="10" t="s">
         <v>4291</v>
       </c>
@@ -51733,9 +51787,15 @@
     </row>
     <row r="1169" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1169" s="10"/>
-      <c r="B1169" s="10"/>
-      <c r="C1169" s="10"/>
-      <c r="D1169" s="10"/>
+      <c r="B1169" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1169" s="10">
+        <v>394</v>
+      </c>
+      <c r="D1169" s="10">
+        <v>1905</v>
+      </c>
       <c r="E1169" s="10" t="s">
         <v>4292</v>
       </c>
@@ -51760,9 +51820,15 @@
     </row>
     <row r="1170" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1170" s="10"/>
-      <c r="B1170" s="10"/>
-      <c r="C1170" s="10"/>
-      <c r="D1170" s="10"/>
+      <c r="B1170" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1170" s="10">
+        <v>40</v>
+      </c>
+      <c r="D1170" s="10">
+        <v>1883</v>
+      </c>
       <c r="E1170" s="10" t="s">
         <v>4293</v>
       </c>
@@ -51785,9 +51851,15 @@
     </row>
     <row r="1171" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1171" s="10"/>
-      <c r="B1171" s="10"/>
-      <c r="C1171" s="10"/>
-      <c r="D1171" s="10"/>
+      <c r="B1171" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1171" s="10">
+        <v>819</v>
+      </c>
+      <c r="D1171" s="10">
+        <v>1932</v>
+      </c>
       <c r="E1171" s="10" t="s">
         <v>4294</v>
       </c>
@@ -51810,9 +51882,15 @@
     </row>
     <row r="1172" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1172" s="10"/>
-      <c r="B1172" s="10"/>
-      <c r="C1172" s="10"/>
-      <c r="D1172" s="10"/>
+      <c r="B1172" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1172" s="10">
+        <v>704</v>
+      </c>
+      <c r="D1172" s="10">
+        <v>1924</v>
+      </c>
       <c r="E1172" s="10" t="s">
         <v>4295</v>
       </c>
@@ -51837,9 +51915,15 @@
     </row>
     <row r="1173" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1173" s="10"/>
-      <c r="B1173" s="10"/>
-      <c r="C1173" s="10"/>
-      <c r="D1173" s="10"/>
+      <c r="B1173" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1173" s="10">
+        <v>1409</v>
+      </c>
+      <c r="D1173" s="10">
+        <v>1969</v>
+      </c>
       <c r="E1173" s="10" t="s">
         <v>4296</v>
       </c>
@@ -51864,9 +51948,15 @@
     </row>
     <row r="1174" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1174" s="10"/>
-      <c r="B1174" s="10"/>
-      <c r="C1174" s="10"/>
-      <c r="D1174" s="10"/>
+      <c r="B1174" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1174" s="10">
+        <v>977</v>
+      </c>
+      <c r="D1174" s="10">
+        <v>1942</v>
+      </c>
       <c r="E1174" s="10" t="s">
         <v>4297</v>
       </c>
@@ -51889,9 +51979,15 @@
     </row>
     <row r="1175" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1175" s="10"/>
-      <c r="B1175" s="10"/>
-      <c r="C1175" s="10"/>
-      <c r="D1175" s="10"/>
+      <c r="B1175" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1175" s="10">
+        <v>622</v>
+      </c>
+      <c r="D1175" s="10">
+        <v>1919</v>
+      </c>
       <c r="E1175" s="10" t="s">
         <v>4298</v>
       </c>
@@ -51914,9 +52010,15 @@
     </row>
     <row r="1176" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1176" s="10"/>
-      <c r="B1176" s="10"/>
-      <c r="C1176" s="10"/>
-      <c r="D1176" s="10"/>
+      <c r="B1176" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1176" s="10">
+        <v>395</v>
+      </c>
+      <c r="D1176" s="10">
+        <v>1905</v>
+      </c>
       <c r="E1176" s="10" t="s">
         <v>4299</v>
       </c>
@@ -51939,9 +52041,15 @@
     </row>
     <row r="1177" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1177" s="10"/>
-      <c r="B1177" s="10"/>
-      <c r="C1177" s="10"/>
-      <c r="D1177" s="10"/>
+      <c r="B1177" s="10">
+        <v>2008</v>
+      </c>
+      <c r="C1177" s="10">
+        <v>638</v>
+      </c>
+      <c r="D1177" s="10">
+        <v>1920</v>
+      </c>
       <c r="E1177" s="10" t="s">
         <v>4300</v>
       </c>
@@ -51966,9 +52074,15 @@
     </row>
     <row r="1178" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1178" s="10"/>
-      <c r="B1178" s="10"/>
-      <c r="C1178" s="10"/>
-      <c r="D1178" s="10"/>
+      <c r="B1178" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1178" s="10">
+        <v>465</v>
+      </c>
+      <c r="D1178" s="10">
+        <v>332</v>
+      </c>
       <c r="E1178" s="10" t="s">
         <v>4301</v>
       </c>
@@ -51993,9 +52107,15 @@
     </row>
     <row r="1179" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1179" s="10"/>
-      <c r="B1179" s="10"/>
-      <c r="C1179" s="10"/>
-      <c r="D1179" s="10"/>
+      <c r="B1179" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1179" s="10">
+        <v>623</v>
+      </c>
+      <c r="D1179" s="10">
+        <v>341</v>
+      </c>
       <c r="E1179" s="10" t="s">
         <v>4302</v>
       </c>
@@ -52020,9 +52140,15 @@
     </row>
     <row r="1180" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1180" s="10"/>
-      <c r="B1180" s="10"/>
-      <c r="C1180" s="10"/>
-      <c r="D1180" s="10"/>
+      <c r="B1180" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1180" s="10">
+        <v>2352</v>
+      </c>
+      <c r="D1180" s="10">
+        <v>450</v>
+      </c>
       <c r="E1180" s="10" t="s">
         <v>4303</v>
       </c>
@@ -52047,9 +52173,15 @@
     </row>
     <row r="1181" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1181" s="10"/>
-      <c r="B1181" s="10"/>
-      <c r="C1181" s="10"/>
-      <c r="D1181" s="10"/>
+      <c r="B1181" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1181" s="10">
+        <v>961</v>
+      </c>
+      <c r="D1181" s="10">
+        <v>363</v>
+      </c>
       <c r="E1181" s="10" t="s">
         <v>4304</v>
       </c>
@@ -52072,9 +52204,15 @@
     </row>
     <row r="1182" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1182" s="10"/>
-      <c r="B1182" s="10"/>
-      <c r="C1182" s="10"/>
-      <c r="D1182" s="10"/>
+      <c r="B1182" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1182" s="10">
+        <v>385</v>
+      </c>
+      <c r="D1182" s="10">
+        <v>327</v>
+      </c>
       <c r="E1182" s="10" t="s">
         <v>4305</v>
       </c>
@@ -52099,9 +52237,15 @@
     </row>
     <row r="1183" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1183" s="10"/>
-      <c r="B1183" s="10"/>
-      <c r="C1183" s="10"/>
-      <c r="D1183" s="10"/>
+      <c r="B1183" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1183" s="10">
+        <v>72</v>
+      </c>
+      <c r="D1183" s="10">
+        <v>307</v>
+      </c>
       <c r="E1183" s="10" t="s">
         <v>4306</v>
       </c>
@@ -52126,9 +52270,15 @@
     </row>
     <row r="1184" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1184" s="10"/>
-      <c r="B1184" s="10"/>
-      <c r="C1184" s="10"/>
-      <c r="D1184" s="10"/>
+      <c r="B1184" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1184" s="10">
+        <v>811</v>
+      </c>
+      <c r="D1184" s="10">
+        <v>353</v>
+      </c>
       <c r="E1184" s="10" t="s">
         <v>4307</v>
       </c>
@@ -52151,9 +52301,15 @@
     </row>
     <row r="1185" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1185" s="10"/>
-      <c r="B1185" s="10"/>
-      <c r="C1185" s="10"/>
-      <c r="D1185" s="10"/>
+      <c r="B1185" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1185" s="10">
+        <v>713</v>
+      </c>
+      <c r="D1185" s="10">
+        <v>347</v>
+      </c>
       <c r="E1185" s="10" t="s">
         <v>4308</v>
       </c>
@@ -52176,9 +52332,15 @@
     </row>
     <row r="1186" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1186" s="10"/>
-      <c r="B1186" s="10"/>
-      <c r="C1186" s="10"/>
-      <c r="D1186" s="10"/>
+      <c r="B1186" s="10">
+        <v>2009</v>
+      </c>
+      <c r="C1186" s="10">
+        <v>1933</v>
+      </c>
+      <c r="D1186" s="10">
+        <v>423</v>
+      </c>
       <c r="E1186" s="10" t="s">
         <v>4309</v>
       </c>
@@ -52226,9 +52388,15 @@
     </row>
     <row r="1188" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1188" s="10"/>
-      <c r="B1188" s="10"/>
-      <c r="C1188" s="10"/>
-      <c r="D1188" s="10"/>
+      <c r="B1188" s="10">
+        <v>2010</v>
+      </c>
+      <c r="C1188" s="10">
+        <v>2514</v>
+      </c>
+      <c r="D1188" s="10">
+        <v>396</v>
+      </c>
       <c r="E1188" s="10" t="s">
         <v>4311</v>
       </c>
@@ -52251,9 +52419,15 @@
     </row>
     <row r="1189" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1189" s="10"/>
-      <c r="B1189" s="10"/>
-      <c r="C1189" s="10"/>
-      <c r="D1189" s="10"/>
+      <c r="B1189" s="10">
+        <v>2010</v>
+      </c>
+      <c r="C1189" s="10">
+        <v>538</v>
+      </c>
+      <c r="D1189" s="10">
+        <v>272</v>
+      </c>
       <c r="E1189" s="10" t="s">
         <v>4312</v>
       </c>
@@ -52278,9 +52452,15 @@
     </row>
     <row r="1190" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1190" s="10"/>
-      <c r="B1190" s="10"/>
-      <c r="C1190" s="10"/>
-      <c r="D1190" s="10"/>
+      <c r="B1190" s="10">
+        <v>2010</v>
+      </c>
+      <c r="C1190" s="10">
+        <v>2835</v>
+      </c>
+      <c r="D1190" s="10">
+        <v>416</v>
+      </c>
       <c r="E1190" s="10" t="s">
         <v>4313</v>
       </c>
@@ -52303,9 +52483,15 @@
     </row>
     <row r="1191" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1191" s="10"/>
-      <c r="B1191" s="10"/>
-      <c r="C1191" s="10"/>
-      <c r="D1191" s="10"/>
+      <c r="B1191" s="10">
+        <v>2011</v>
+      </c>
+      <c r="C1191" s="10">
+        <v>1584</v>
+      </c>
+      <c r="D1191" s="10">
+        <v>281</v>
+      </c>
       <c r="E1191" s="10" t="s">
         <v>4314</v>
       </c>
@@ -52328,9 +52514,15 @@
     </row>
     <row r="1192" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1192" s="10"/>
-      <c r="B1192" s="10"/>
-      <c r="C1192" s="10"/>
-      <c r="D1192" s="10"/>
+      <c r="B1192" s="10">
+        <v>2011</v>
+      </c>
+      <c r="C1192" s="10">
+        <v>488</v>
+      </c>
+      <c r="D1192" s="10">
+        <v>212</v>
+      </c>
       <c r="E1192" s="10" t="s">
         <v>4315</v>
       </c>
@@ -52355,9 +52547,15 @@
     </row>
     <row r="1193" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1193" s="10"/>
-      <c r="B1193" s="10"/>
-      <c r="C1193" s="10"/>
-      <c r="D1193" s="10"/>
+      <c r="B1193" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C1193" s="10">
+        <v>372</v>
+      </c>
+      <c r="D1193" s="10">
+        <v>114</v>
+      </c>
       <c r="E1193" s="10" t="s">
         <v>4316</v>
       </c>
@@ -52382,9 +52580,15 @@
     </row>
     <row r="1194" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1194" s="10"/>
-      <c r="B1194" s="10"/>
-      <c r="C1194" s="10"/>
-      <c r="D1194" s="10"/>
+      <c r="B1194" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C1194" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1194" s="10">
+        <v>92</v>
+      </c>
       <c r="E1194" s="10" t="s">
         <v>4317</v>
       </c>
@@ -52407,9 +52611,15 @@
     </row>
     <row r="1195" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1195" s="10"/>
-      <c r="B1195" s="10"/>
-      <c r="C1195" s="10"/>
-      <c r="D1195" s="10"/>
+      <c r="B1195" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C1195" s="10">
+        <v>993</v>
+      </c>
+      <c r="D1195" s="10">
+        <v>153</v>
+      </c>
       <c r="E1195" s="10" t="s">
         <v>4318</v>
       </c>
@@ -52432,9 +52642,15 @@
     </row>
     <row r="1196" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1196" s="10"/>
-      <c r="B1196" s="10"/>
-      <c r="C1196" s="10"/>
-      <c r="D1196" s="10"/>
+      <c r="B1196" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C1196" s="10">
+        <v>735</v>
+      </c>
+      <c r="D1196" s="10">
+        <v>136</v>
+      </c>
       <c r="E1196" s="10" t="s">
         <v>4319</v>
       </c>
@@ -52459,9 +52675,15 @@
     </row>
     <row r="1197" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1197" s="10"/>
-      <c r="B1197" s="10"/>
-      <c r="C1197" s="10"/>
-      <c r="D1197" s="10"/>
+      <c r="B1197" s="10">
+        <v>2012</v>
+      </c>
+      <c r="C1197" s="10">
+        <v>313</v>
+      </c>
+      <c r="D1197" s="10">
+        <v>110</v>
+      </c>
       <c r="E1197" s="10" t="s">
         <v>4320</v>
       </c>
@@ -52484,9 +52706,15 @@
     </row>
     <row r="1198" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1198" s="10"/>
-      <c r="B1198" s="10"/>
-      <c r="C1198" s="10"/>
-      <c r="D1198" s="10"/>
+      <c r="B1198" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1198" s="10">
+        <v>339</v>
+      </c>
+      <c r="D1198" s="10">
+        <v>178</v>
+      </c>
       <c r="E1198" s="10" t="s">
         <v>4321</v>
       </c>
@@ -52509,9 +52737,15 @@
     </row>
     <row r="1199" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1199" s="10"/>
-      <c r="B1199" s="10"/>
-      <c r="C1199" s="10"/>
-      <c r="D1199" s="10"/>
+      <c r="B1199" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1199" s="10">
+        <v>397</v>
+      </c>
+      <c r="D1199" s="10">
+        <v>181</v>
+      </c>
       <c r="E1199" s="10" t="s">
         <v>4322</v>
       </c>
@@ -52534,9 +52768,15 @@
     </row>
     <row r="1200" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1200" s="10"/>
-      <c r="B1200" s="10"/>
-      <c r="C1200" s="10"/>
-      <c r="D1200" s="10"/>
+      <c r="B1200" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1200" s="10">
+        <v>1069</v>
+      </c>
+      <c r="D1200" s="10">
+        <v>209</v>
+      </c>
       <c r="E1200" s="10" t="s">
         <v>4323</v>
       </c>
@@ -52561,9 +52801,15 @@
     </row>
     <row r="1201" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1201" s="10"/>
-      <c r="B1201" s="10"/>
-      <c r="C1201" s="10"/>
-      <c r="D1201" s="10"/>
+      <c r="B1201" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1201" s="10">
+        <v>691</v>
+      </c>
+      <c r="D1201" s="10">
+        <v>193</v>
+      </c>
       <c r="E1201" s="10" t="s">
         <v>4324</v>
       </c>
@@ -52588,9 +52834,15 @@
     </row>
     <row r="1202" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1202" s="10"/>
-      <c r="B1202" s="10"/>
-      <c r="C1202" s="10"/>
-      <c r="D1202" s="10"/>
+      <c r="B1202" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1202" s="10">
+        <v>1272</v>
+      </c>
+      <c r="D1202" s="10">
+        <v>217</v>
+      </c>
       <c r="E1202" s="10" t="s">
         <v>4325</v>
       </c>
@@ -52613,9 +52865,15 @@
     </row>
     <row r="1203" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1203" s="10"/>
-      <c r="B1203" s="10"/>
-      <c r="C1203" s="10"/>
-      <c r="D1203" s="10"/>
+      <c r="B1203" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1203" s="10">
+        <v>520</v>
+      </c>
+      <c r="D1203" s="10">
+        <v>186</v>
+      </c>
       <c r="E1203" s="10" t="s">
         <v>4326</v>
       </c>
@@ -52638,9 +52896,15 @@
     </row>
     <row r="1204" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1204" s="10"/>
-      <c r="B1204" s="10"/>
-      <c r="C1204" s="10"/>
-      <c r="D1204" s="10"/>
+      <c r="B1204" s="10">
+        <v>2013</v>
+      </c>
+      <c r="C1204" s="10">
+        <v>513</v>
+      </c>
+      <c r="D1204" s="10">
+        <v>186</v>
+      </c>
       <c r="E1204" s="10" t="s">
         <v>4327</v>
       </c>
@@ -52665,9 +52929,15 @@
     </row>
     <row r="1205" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1205" s="10"/>
-      <c r="B1205" s="10"/>
-      <c r="C1205" s="10"/>
-      <c r="D1205" s="10"/>
+      <c r="B1205" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1205" s="10">
+        <v>955</v>
+      </c>
+      <c r="D1205" s="10">
+        <v>217</v>
+      </c>
       <c r="E1205" s="10" t="s">
         <v>4328</v>
       </c>
@@ -52690,9 +52960,15 @@
     </row>
     <row r="1206" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1206" s="10"/>
-      <c r="B1206" s="10"/>
-      <c r="C1206" s="10"/>
-      <c r="D1206" s="10"/>
+      <c r="B1206" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1206" s="10">
+        <v>1180</v>
+      </c>
+      <c r="D1206" s="10">
+        <v>230</v>
+      </c>
       <c r="E1206" s="10" t="s">
         <v>4329</v>
       </c>
@@ -52715,9 +52991,15 @@
     </row>
     <row r="1207" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1207" s="10"/>
-      <c r="B1207" s="10"/>
-      <c r="C1207" s="10"/>
-      <c r="D1207" s="10"/>
+      <c r="B1207" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1207" s="10">
+        <v>1549</v>
+      </c>
+      <c r="D1207" s="10">
+        <v>250</v>
+      </c>
       <c r="E1207" s="10" t="s">
         <v>4330</v>
       </c>
@@ -52742,9 +53024,15 @@
     </row>
     <row r="1208" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1208" s="10"/>
-      <c r="B1208" s="10"/>
-      <c r="C1208" s="10"/>
-      <c r="D1208" s="10"/>
+      <c r="B1208" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1208" s="10">
+        <v>1191</v>
+      </c>
+      <c r="D1208" s="10">
+        <v>230</v>
+      </c>
       <c r="E1208" s="10" t="s">
         <v>4331</v>
       </c>
@@ -52769,9 +53057,15 @@
     </row>
     <row r="1209" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1209" s="10"/>
-      <c r="B1209" s="10"/>
-      <c r="C1209" s="10"/>
-      <c r="D1209" s="10"/>
+      <c r="B1209" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1209" s="10">
+        <v>1634</v>
+      </c>
+      <c r="D1209" s="10">
+        <v>254</v>
+      </c>
       <c r="E1209" s="10" t="s">
         <v>4332</v>
       </c>
@@ -52794,9 +53088,15 @@
     </row>
     <row r="1210" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1210" s="10"/>
-      <c r="B1210" s="10"/>
-      <c r="C1210" s="10"/>
-      <c r="D1210" s="10"/>
+      <c r="B1210" s="10">
+        <v>2014</v>
+      </c>
+      <c r="C1210" s="10">
+        <v>1296</v>
+      </c>
+      <c r="D1210" s="10">
+        <v>236</v>
+      </c>
       <c r="E1210" s="10" t="s">
         <v>4333</v>
       </c>
@@ -52819,9 +53119,15 @@
     </row>
     <row r="1211" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1211" s="10"/>
-      <c r="B1211" s="10"/>
-      <c r="C1211" s="10"/>
-      <c r="D1211" s="10"/>
+      <c r="B1211" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1211" s="10">
+        <v>208</v>
+      </c>
+      <c r="D1211" s="10">
+        <v>154</v>
+      </c>
       <c r="E1211" s="10" t="s">
         <v>4334</v>
       </c>
@@ -52846,9 +53152,15 @@
     </row>
     <row r="1212" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1212" s="10"/>
-      <c r="B1212" s="10"/>
-      <c r="C1212" s="10"/>
-      <c r="D1212" s="10"/>
+      <c r="B1212" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1212" s="10">
+        <v>231</v>
+      </c>
+      <c r="D1212" s="10">
+        <v>155</v>
+      </c>
       <c r="E1212" s="10" t="s">
         <v>4335</v>
       </c>
@@ -52871,9 +53183,15 @@
     </row>
     <row r="1213" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1213" s="10"/>
-      <c r="B1213" s="10"/>
-      <c r="C1213" s="10"/>
-      <c r="D1213" s="10"/>
+      <c r="B1213" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1213" s="10">
+        <v>248</v>
+      </c>
+      <c r="D1213" s="10">
+        <v>155</v>
+      </c>
       <c r="E1213" s="10" t="s">
         <v>4336</v>
       </c>
@@ -52896,9 +53214,15 @@
     </row>
     <row r="1214" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1214" s="10"/>
-      <c r="B1214" s="10"/>
-      <c r="C1214" s="10"/>
-      <c r="D1214" s="10"/>
+      <c r="B1214" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1214" s="10">
+        <v>252</v>
+      </c>
+      <c r="D1214" s="10">
+        <v>155</v>
+      </c>
       <c r="E1214" s="10" t="s">
         <v>4337</v>
       </c>
@@ -52922,7 +53246,9 @@
     <row r="1215" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1215" s="10"/>
       <c r="B1215" s="10"/>
-      <c r="C1215" s="10"/>
+      <c r="C1215" s="10">
+        <v>261</v>
+      </c>
       <c r="D1215" s="10"/>
       <c r="E1215" s="10" t="s">
         <v>4338</v>
@@ -52946,9 +53272,15 @@
     </row>
     <row r="1216" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1216" s="10"/>
-      <c r="B1216" s="10"/>
-      <c r="C1216" s="10"/>
-      <c r="D1216" s="10"/>
+      <c r="B1216" s="10">
+        <v>2015</v>
+      </c>
+      <c r="C1216" s="10">
+        <v>256</v>
+      </c>
+      <c r="D1216" s="10">
+        <v>155</v>
+      </c>
       <c r="E1216" s="10" t="s">
         <v>4339</v>
       </c>
@@ -52973,9 +53305,15 @@
     </row>
     <row r="1217" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1217" s="10"/>
-      <c r="B1217" s="10"/>
-      <c r="C1217" s="10"/>
-      <c r="D1217" s="10"/>
+      <c r="B1217" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1217" s="10">
+        <v>178</v>
+      </c>
+      <c r="D1217" s="10">
+        <v>276</v>
+      </c>
       <c r="E1217" s="10" t="s">
         <v>4340</v>
       </c>
@@ -53000,9 +53338,15 @@
     </row>
     <row r="1218" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1218" s="10"/>
-      <c r="B1218" s="10"/>
-      <c r="C1218" s="10"/>
-      <c r="D1218" s="10"/>
+      <c r="B1218" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1218" s="10">
+        <v>181</v>
+      </c>
+      <c r="D1218" s="10">
+        <v>276</v>
+      </c>
       <c r="E1218" s="10" t="s">
         <v>4341</v>
       </c>
@@ -53027,9 +53371,15 @@
     </row>
     <row r="1219" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1219" s="10"/>
-      <c r="B1219" s="10"/>
-      <c r="C1219" s="10"/>
-      <c r="D1219" s="10"/>
+      <c r="B1219" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1219" s="10">
+        <v>193</v>
+      </c>
+      <c r="D1219" s="10">
+        <v>276</v>
+      </c>
       <c r="E1219" s="10" t="s">
         <v>4342</v>
       </c>
@@ -53054,9 +53404,15 @@
     </row>
     <row r="1220" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1220" s="10"/>
-      <c r="B1220" s="10"/>
-      <c r="C1220" s="10"/>
-      <c r="D1220" s="10"/>
+      <c r="B1220" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1220" s="10">
+        <v>194</v>
+      </c>
+      <c r="D1220" s="10">
+        <v>276</v>
+      </c>
       <c r="E1220" s="10" t="s">
         <v>4343</v>
       </c>
@@ -53081,9 +53437,15 @@
     </row>
     <row r="1221" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1221" s="10"/>
-      <c r="B1221" s="10"/>
-      <c r="C1221" s="10"/>
-      <c r="D1221" s="10"/>
+      <c r="B1221" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1221" s="10">
+        <v>206</v>
+      </c>
+      <c r="D1221" s="10">
+        <v>277</v>
+      </c>
       <c r="E1221" s="10" t="s">
         <v>4344</v>
       </c>
@@ -53108,9 +53470,15 @@
     </row>
     <row r="1222" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1222" s="10"/>
-      <c r="B1222" s="10"/>
-      <c r="C1222" s="10"/>
-      <c r="D1222" s="10"/>
+      <c r="B1222" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1222" s="10">
+        <v>219</v>
+      </c>
+      <c r="D1222" s="10">
+        <v>277</v>
+      </c>
       <c r="E1222" s="10" t="s">
         <v>4345</v>
       </c>
@@ -53135,9 +53503,15 @@
     </row>
     <row r="1223" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1223" s="10"/>
-      <c r="B1223" s="10"/>
-      <c r="C1223" s="10"/>
-      <c r="D1223" s="10"/>
+      <c r="B1223" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1223" s="10">
+        <v>243</v>
+      </c>
+      <c r="D1223" s="10">
+        <v>278</v>
+      </c>
       <c r="E1223" s="10" t="s">
         <v>4346</v>
       </c>
@@ -53162,9 +53536,15 @@
     </row>
     <row r="1224" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1224" s="10"/>
-      <c r="B1224" s="10"/>
-      <c r="C1224" s="10"/>
-      <c r="D1224" s="10"/>
+      <c r="B1224" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1224" s="10">
+        <v>249</v>
+      </c>
+      <c r="D1224" s="10">
+        <v>278</v>
+      </c>
       <c r="E1224" s="10" t="s">
         <v>4347</v>
       </c>
@@ -53189,9 +53569,15 @@
     </row>
     <row r="1225" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1225" s="10"/>
-      <c r="B1225" s="10"/>
-      <c r="C1225" s="10"/>
-      <c r="D1225" s="10"/>
+      <c r="B1225" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1225" s="10">
+        <v>264</v>
+      </c>
+      <c r="D1225" s="10">
+        <v>279</v>
+      </c>
       <c r="E1225" s="10" t="s">
         <v>4348</v>
       </c>
@@ -53216,9 +53602,15 @@
     </row>
     <row r="1226" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1226" s="10"/>
-      <c r="B1226" s="10"/>
-      <c r="C1226" s="10"/>
-      <c r="D1226" s="10"/>
+      <c r="B1226" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1226" s="10">
+        <v>270</v>
+      </c>
+      <c r="D1226" s="10">
+        <v>279</v>
+      </c>
       <c r="E1226" s="10" t="s">
         <v>4349</v>
       </c>
@@ -53243,9 +53635,15 @@
     </row>
     <row r="1227" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1227" s="10"/>
-      <c r="B1227" s="10"/>
-      <c r="C1227" s="10"/>
-      <c r="D1227" s="10"/>
+      <c r="B1227" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1227" s="10">
+        <v>282</v>
+      </c>
+      <c r="D1227" s="10">
+        <v>280</v>
+      </c>
       <c r="E1227" s="10" t="s">
         <v>4350</v>
       </c>
@@ -53270,9 +53668,15 @@
     </row>
     <row r="1228" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1228" s="10"/>
-      <c r="B1228" s="10"/>
-      <c r="C1228" s="10"/>
-      <c r="D1228" s="10"/>
+      <c r="B1228" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1228" s="10">
+        <v>300</v>
+      </c>
+      <c r="D1228" s="10">
+        <v>280</v>
+      </c>
       <c r="E1228" s="10" t="s">
         <v>4351</v>
       </c>
@@ -53297,9 +53701,15 @@
     </row>
     <row r="1229" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1229" s="10"/>
-      <c r="B1229" s="10"/>
-      <c r="C1229" s="10"/>
-      <c r="D1229" s="10"/>
+      <c r="B1229" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1229" s="10">
+        <v>312</v>
+      </c>
+      <c r="D1229" s="10">
+        <v>281</v>
+      </c>
       <c r="E1229" s="10" t="s">
         <v>4352</v>
       </c>
@@ -53324,9 +53734,15 @@
     </row>
     <row r="1230" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1230" s="10"/>
-      <c r="B1230" s="10"/>
-      <c r="C1230" s="10"/>
-      <c r="D1230" s="10"/>
+      <c r="B1230" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1230" s="10">
+        <v>313</v>
+      </c>
+      <c r="D1230" s="10">
+        <v>281</v>
+      </c>
       <c r="E1230" s="10" t="s">
         <v>4353</v>
       </c>
@@ -53351,9 +53767,15 @@
     </row>
     <row r="1231" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1231" s="10"/>
-      <c r="B1231" s="10"/>
-      <c r="C1231" s="10"/>
-      <c r="D1231" s="10"/>
+      <c r="B1231" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1231" s="10">
+        <v>314</v>
+      </c>
+      <c r="D1231" s="10">
+        <v>281</v>
+      </c>
       <c r="E1231" s="10" t="s">
         <v>4354</v>
       </c>
@@ -53378,9 +53800,15 @@
     </row>
     <row r="1232" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1232" s="10"/>
-      <c r="B1232" s="10"/>
-      <c r="C1232" s="10"/>
-      <c r="D1232" s="10"/>
+      <c r="B1232" s="10">
+        <v>2017</v>
+      </c>
+      <c r="C1232" s="10">
+        <v>317</v>
+      </c>
+      <c r="D1232" s="10">
+        <v>281</v>
+      </c>
       <c r="E1232" s="10" t="s">
         <v>4355</v>
       </c>
@@ -53405,9 +53833,15 @@
     </row>
     <row r="1233" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1233" s="10"/>
-      <c r="B1233" s="10"/>
-      <c r="C1233" s="10"/>
-      <c r="D1233" s="10"/>
+      <c r="B1233" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1233" s="10">
+        <v>195</v>
+      </c>
+      <c r="D1233" s="10">
+        <v>211</v>
+      </c>
       <c r="E1233" s="10" t="s">
         <v>4356</v>
       </c>
@@ -53432,9 +53866,15 @@
     </row>
     <row r="1234" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1234" s="10"/>
-      <c r="B1234" s="10"/>
-      <c r="C1234" s="10"/>
-      <c r="D1234" s="10"/>
+      <c r="B1234" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1234" s="10">
+        <v>212</v>
+      </c>
+      <c r="D1234" s="10">
+        <v>212</v>
+      </c>
       <c r="E1234" s="10" t="s">
         <v>4357</v>
       </c>
@@ -53459,9 +53899,15 @@
     </row>
     <row r="1235" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1235" s="10"/>
-      <c r="B1235" s="10"/>
-      <c r="C1235" s="10"/>
-      <c r="D1235" s="10"/>
+      <c r="B1235" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1235" s="10">
+        <v>217</v>
+      </c>
+      <c r="D1235" s="10">
+        <v>212</v>
+      </c>
       <c r="E1235" s="10" t="s">
         <v>4358</v>
       </c>
@@ -53486,9 +53932,15 @@
     </row>
     <row r="1236" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1236" s="10"/>
-      <c r="B1236" s="10"/>
-      <c r="C1236" s="10"/>
-      <c r="D1236" s="10"/>
+      <c r="B1236" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1236" s="10">
+        <v>229</v>
+      </c>
+      <c r="D1236" s="10">
+        <v>213</v>
+      </c>
       <c r="E1236" s="10" t="s">
         <v>4359</v>
       </c>
@@ -53513,9 +53965,15 @@
     </row>
     <row r="1237" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1237" s="10"/>
-      <c r="B1237" s="10"/>
-      <c r="C1237" s="10"/>
-      <c r="D1237" s="10"/>
+      <c r="B1237" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1237" s="10">
+        <v>230</v>
+      </c>
+      <c r="D1237" s="10">
+        <v>213</v>
+      </c>
       <c r="E1237" s="10" t="s">
         <v>4360</v>
       </c>
@@ -53540,9 +53998,15 @@
     </row>
     <row r="1238" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1238" s="10"/>
-      <c r="B1238" s="10"/>
-      <c r="C1238" s="10"/>
-      <c r="D1238" s="10"/>
+      <c r="B1238" s="10">
+        <v>2018</v>
+      </c>
+      <c r="C1238" s="10">
+        <v>242</v>
+      </c>
+      <c r="D1238" s="10">
+        <v>214</v>
+      </c>
       <c r="E1238" s="10" t="s">
         <v>4361</v>
       </c>
@@ -53567,9 +54031,15 @@
     </row>
     <row r="1239" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1239" s="10"/>
-      <c r="B1239" s="10"/>
-      <c r="C1239" s="10"/>
-      <c r="D1239" s="10"/>
+      <c r="B1239" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C1239" s="10">
+        <v>199</v>
+      </c>
+      <c r="D1239" s="10">
+        <v>142</v>
+      </c>
       <c r="E1239" s="10" t="s">
         <v>4362</v>
       </c>
@@ -53594,9 +54064,15 @@
     </row>
     <row r="1240" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1240" s="10"/>
-      <c r="B1240" s="10"/>
-      <c r="C1240" s="10"/>
-      <c r="D1240" s="10"/>
+      <c r="B1240" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C1240" s="10">
+        <v>216</v>
+      </c>
+      <c r="D1240" s="10">
+        <v>143</v>
+      </c>
       <c r="E1240" s="10" t="s">
         <v>4363</v>
       </c>
@@ -53621,9 +54097,15 @@
     </row>
     <row r="1241" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1241" s="10"/>
-      <c r="B1241" s="10"/>
-      <c r="C1241" s="10"/>
-      <c r="D1241" s="10"/>
+      <c r="B1241" s="10">
+        <v>2019</v>
+      </c>
+      <c r="C1241" s="10">
+        <v>245</v>
+      </c>
+      <c r="D1241" s="10">
+        <v>144</v>
+      </c>
       <c r="E1241" s="10" t="s">
         <v>4364</v>
       </c>

</xml_diff>

<commit_message>
added all ivpr in set 2, only not found ivpr remaining
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -14247,8 +14247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1236" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1241" sqref="L1241"/>
+    <sheetView tabSelected="1" topLeftCell="A1101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1095" sqref="C1095"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46182,9 +46182,15 @@
     </row>
     <row r="972" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A972" s="7"/>
-      <c r="B972" s="7"/>
-      <c r="C972" s="7"/>
-      <c r="D972" s="7"/>
+      <c r="B972" s="7">
+        <v>1994</v>
+      </c>
+      <c r="C972" s="7">
+        <v>312</v>
+      </c>
+      <c r="D972" s="7">
+        <v>274</v>
+      </c>
       <c r="E972" s="7" t="s">
         <v>3791</v>
       </c>
@@ -46955,9 +46961,15 @@
     </row>
     <row r="1001" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1001" s="7"/>
-      <c r="B1001" s="7"/>
-      <c r="C1001" s="7"/>
-      <c r="D1001" s="7"/>
+      <c r="B1001" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1001" s="7">
+        <v>233</v>
+      </c>
+      <c r="D1001" s="7">
+        <v>179</v>
+      </c>
       <c r="E1001" s="7" t="s">
         <v>3837</v>
       </c>
@@ -46982,9 +46994,15 @@
     </row>
     <row r="1002" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1002" s="7"/>
-      <c r="B1002" s="7"/>
-      <c r="C1002" s="7"/>
-      <c r="D1002" s="7"/>
+      <c r="B1002" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1002" s="7">
+        <v>1020</v>
+      </c>
+      <c r="D1002" s="7">
+        <v>225</v>
+      </c>
       <c r="E1002" s="7" t="s">
         <v>3838</v>
       </c>
@@ -47009,9 +47027,15 @@
     </row>
     <row r="1003" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1003" s="7"/>
-      <c r="B1003" s="7"/>
-      <c r="C1003" s="7"/>
-      <c r="D1003" s="7"/>
+      <c r="B1003" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1003" s="7">
+        <v>453</v>
+      </c>
+      <c r="D1003" s="7">
+        <v>192</v>
+      </c>
       <c r="E1003" s="7" t="s">
         <v>3839</v>
       </c>
@@ -47036,9 +47060,15 @@
     </row>
     <row r="1004" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1004" s="7"/>
-      <c r="B1004" s="7"/>
-      <c r="C1004" s="7"/>
-      <c r="D1004" s="7"/>
+      <c r="B1004" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1004" s="7">
+        <v>340</v>
+      </c>
+      <c r="D1004" s="7">
+        <v>185</v>
+      </c>
       <c r="E1004" s="7" t="s">
         <v>3841</v>
       </c>
@@ -47063,9 +47093,15 @@
     </row>
     <row r="1005" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1005" s="7"/>
-      <c r="B1005" s="7"/>
-      <c r="C1005" s="7"/>
-      <c r="D1005" s="7"/>
+      <c r="B1005" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1005" s="7">
+        <v>263</v>
+      </c>
+      <c r="D1005" s="7">
+        <v>181</v>
+      </c>
       <c r="E1005" s="7" t="s">
         <v>3842</v>
       </c>
@@ -47090,9 +47126,15 @@
     </row>
     <row r="1006" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1006" s="7"/>
-      <c r="B1006" s="7"/>
-      <c r="C1006" s="7"/>
-      <c r="D1006" s="7"/>
+      <c r="B1006" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1006" s="7">
+        <v>237</v>
+      </c>
+      <c r="D1006" s="7">
+        <v>179</v>
+      </c>
       <c r="E1006" s="7" t="s">
         <v>3843</v>
       </c>
@@ -47117,9 +47159,15 @@
     </row>
     <row r="1007" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1007" s="7"/>
-      <c r="B1007" s="7"/>
-      <c r="C1007" s="7"/>
-      <c r="D1007" s="7"/>
+      <c r="B1007" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1007" s="7">
+        <v>1774</v>
+      </c>
+      <c r="D1007" s="7">
+        <v>270</v>
+      </c>
       <c r="E1007" s="7" t="s">
         <v>3844</v>
       </c>
@@ -47144,9 +47192,15 @@
     </row>
     <row r="1008" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1008" s="7"/>
-      <c r="B1008" s="7"/>
-      <c r="C1008" s="7"/>
-      <c r="D1008" s="7"/>
+      <c r="B1008" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1008" s="7">
+        <v>1775</v>
+      </c>
+      <c r="D1008" s="7">
+        <v>270</v>
+      </c>
       <c r="E1008" s="7" t="s">
         <v>3846</v>
       </c>
@@ -47198,9 +47252,15 @@
     </row>
     <row r="1010" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1010" s="7"/>
-      <c r="B1010" s="7"/>
-      <c r="C1010" s="7"/>
-      <c r="D1010" s="7"/>
+      <c r="B1010" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C1010" s="7">
+        <v>1209</v>
+      </c>
+      <c r="D1010" s="7">
+        <v>237</v>
+      </c>
       <c r="E1010" s="7" t="s">
         <v>3848</v>
       </c>
@@ -47225,9 +47285,15 @@
     </row>
     <row r="1011" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1011" s="7"/>
-      <c r="B1011" s="7"/>
-      <c r="C1011" s="7"/>
-      <c r="D1011" s="7"/>
+      <c r="B1011" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C1011" s="7">
+        <v>740</v>
+      </c>
+      <c r="D1011" s="7">
+        <v>307</v>
+      </c>
       <c r="E1011" s="7" t="s">
         <v>3850</v>
       </c>
@@ -47331,9 +47397,15 @@
     </row>
     <row r="1015" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1015" s="7"/>
-      <c r="B1015" s="7"/>
-      <c r="C1015" s="7"/>
-      <c r="D1015" s="7"/>
+      <c r="B1015" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C1015" s="7">
+        <v>1433</v>
+      </c>
+      <c r="D1015" s="7">
+        <v>370</v>
+      </c>
       <c r="E1015" s="7" t="s">
         <v>3855</v>
       </c>
@@ -47358,9 +47430,15 @@
     </row>
     <row r="1016" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1016" s="7"/>
-      <c r="B1016" s="7"/>
-      <c r="C1016" s="7"/>
-      <c r="D1016" s="7"/>
+      <c r="B1016" s="7">
+        <v>2001</v>
+      </c>
+      <c r="C1016" s="7">
+        <v>499</v>
+      </c>
+      <c r="D1016" s="7">
+        <v>247</v>
+      </c>
       <c r="E1016" s="7" t="s">
         <v>3856</v>
       </c>
@@ -47487,9 +47565,15 @@
     </row>
     <row r="1021" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1021" s="7"/>
-      <c r="B1021" s="7"/>
-      <c r="C1021" s="7"/>
-      <c r="D1021" s="7"/>
+      <c r="B1021" s="7">
+        <v>2004</v>
+      </c>
+      <c r="C1021" s="7">
+        <v>271</v>
+      </c>
+      <c r="D1021" s="7">
+        <v>142</v>
+      </c>
       <c r="E1021" s="7" t="s">
         <v>3863</v>
       </c>
@@ -47539,9 +47623,15 @@
     </row>
     <row r="1023" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1023" s="7"/>
-      <c r="B1023" s="7"/>
-      <c r="C1023" s="7"/>
-      <c r="D1023" s="7"/>
+      <c r="B1023" s="7">
+        <v>2010</v>
+      </c>
+      <c r="C1023" s="7">
+        <v>753</v>
+      </c>
+      <c r="D1023" s="7">
+        <v>286</v>
+      </c>
       <c r="E1023" s="7" t="s">
         <v>3865</v>
       </c>
@@ -47564,9 +47654,15 @@
     </row>
     <row r="1024" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1024" s="7"/>
-      <c r="B1024" s="7"/>
-      <c r="C1024" s="7"/>
-      <c r="D1024" s="7"/>
+      <c r="B1024" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C1024" s="7">
+        <v>449</v>
+      </c>
+      <c r="D1024" s="7">
+        <v>119</v>
+      </c>
       <c r="E1024" s="7" t="s">
         <v>3866</v>
       </c>
@@ -47616,9 +47712,15 @@
     </row>
     <row r="1026" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1026" s="7"/>
-      <c r="B1026" s="7"/>
-      <c r="C1026" s="7"/>
-      <c r="D1026" s="7"/>
+      <c r="B1026" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C1026" s="7">
+        <v>204</v>
+      </c>
+      <c r="D1026" s="7">
+        <v>142</v>
+      </c>
       <c r="E1026" s="7" t="s">
         <v>3869</v>
       </c>
@@ -47644,7 +47746,9 @@
     <row r="1027" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1027" s="7"/>
       <c r="B1027" s="7"/>
-      <c r="C1027" s="7"/>
+      <c r="C1027" s="7">
+        <v>225</v>
+      </c>
       <c r="D1027" s="7"/>
       <c r="E1027" s="7" t="s">
         <v>3871</v>
@@ -47722,9 +47826,15 @@
     </row>
     <row r="1030" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1030" s="7"/>
-      <c r="B1030" s="7"/>
-      <c r="C1030" s="7"/>
-      <c r="D1030" s="7"/>
+      <c r="B1030" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C1030" s="7">
+        <v>429</v>
+      </c>
+      <c r="D1030" s="7">
+        <v>344</v>
+      </c>
       <c r="E1030" s="7" t="s">
         <v>3875</v>
       </c>
@@ -47749,9 +47859,15 @@
     </row>
     <row r="1031" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1031" s="7"/>
-      <c r="B1031" s="7"/>
-      <c r="C1031" s="7"/>
-      <c r="D1031" s="7"/>
+      <c r="B1031" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C1031" s="7">
+        <v>435</v>
+      </c>
+      <c r="D1031" s="7">
+        <v>344</v>
+      </c>
       <c r="E1031" s="7" t="s">
         <v>3877</v>
       </c>
@@ -47776,9 +47892,15 @@
     </row>
     <row r="1032" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1032" s="7"/>
-      <c r="B1032" s="7"/>
-      <c r="C1032" s="7"/>
-      <c r="D1032" s="7"/>
+      <c r="B1032" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C1032" s="7">
+        <v>436</v>
+      </c>
+      <c r="D1032" s="7">
+        <v>344</v>
+      </c>
       <c r="E1032" s="7" t="s">
         <v>3879</v>
       </c>
@@ -47803,9 +47925,15 @@
     </row>
     <row r="1033" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1033" s="7"/>
-      <c r="B1033" s="7"/>
-      <c r="C1033" s="7"/>
-      <c r="D1033" s="7"/>
+      <c r="B1033" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C1033" s="7">
+        <v>437</v>
+      </c>
+      <c r="D1033" s="7">
+        <v>344</v>
+      </c>
       <c r="E1033" s="7" t="s">
         <v>3881</v>
       </c>
@@ -47830,9 +47958,15 @@
     </row>
     <row r="1034" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1034" s="7"/>
-      <c r="B1034" s="7"/>
-      <c r="C1034" s="7"/>
-      <c r="D1034" s="7"/>
+      <c r="B1034" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C1034" s="7">
+        <v>438</v>
+      </c>
+      <c r="D1034" s="7">
+        <v>344</v>
+      </c>
       <c r="E1034" s="7" t="s">
         <v>3883</v>
       </c>
@@ -47857,9 +47991,15 @@
     </row>
     <row r="1035" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1035" s="7"/>
-      <c r="B1035" s="7"/>
-      <c r="C1035" s="7"/>
-      <c r="D1035" s="7"/>
+      <c r="B1035" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C1035" s="7">
+        <v>275</v>
+      </c>
+      <c r="D1035" s="7">
+        <v>319</v>
+      </c>
       <c r="E1035" s="7" t="s">
         <v>3885</v>
       </c>
@@ -47884,9 +48024,15 @@
     </row>
     <row r="1036" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1036" s="7"/>
-      <c r="B1036" s="7"/>
-      <c r="C1036" s="7"/>
-      <c r="D1036" s="7"/>
+      <c r="B1036" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C1036" s="7">
+        <v>276</v>
+      </c>
+      <c r="D1036" s="7">
+        <v>319</v>
+      </c>
       <c r="E1036" s="7" t="s">
         <v>3887</v>
       </c>
@@ -47911,9 +48057,15 @@
     </row>
     <row r="1037" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1037" s="7"/>
-      <c r="B1037" s="7"/>
-      <c r="C1037" s="7"/>
-      <c r="D1037" s="7"/>
+      <c r="B1037" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C1037" s="7">
+        <v>277</v>
+      </c>
+      <c r="D1037" s="7">
+        <v>319</v>
+      </c>
       <c r="E1037" s="7" t="s">
         <v>3889</v>
       </c>
@@ -47938,9 +48090,15 @@
     </row>
     <row r="1038" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1038" s="10"/>
-      <c r="B1038" s="10"/>
-      <c r="C1038" s="10"/>
-      <c r="D1038" s="10"/>
+      <c r="B1038" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1038" s="10">
+        <v>292</v>
+      </c>
+      <c r="D1038" s="10">
+        <v>273</v>
+      </c>
       <c r="E1038" s="10" t="s">
         <v>4161</v>
       </c>
@@ -47992,9 +48150,15 @@
     </row>
     <row r="1040" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1040" s="10"/>
-      <c r="B1040" s="10"/>
-      <c r="C1040" s="10"/>
-      <c r="D1040" s="10"/>
+      <c r="B1040" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1040" s="10">
+        <v>284</v>
+      </c>
+      <c r="D1040" s="10">
+        <v>272</v>
+      </c>
       <c r="E1040" s="10" t="s">
         <v>4163</v>
       </c>
@@ -48019,9 +48183,15 @@
     </row>
     <row r="1041" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1041" s="10"/>
-      <c r="B1041" s="10"/>
-      <c r="C1041" s="10"/>
-      <c r="D1041" s="10"/>
+      <c r="B1041" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1041" s="10">
+        <v>215</v>
+      </c>
+      <c r="D1041" s="10">
+        <v>269</v>
+      </c>
       <c r="E1041" s="10" t="s">
         <v>4164</v>
       </c>
@@ -48046,9 +48216,15 @@
     </row>
     <row r="1042" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1042" s="10"/>
-      <c r="B1042" s="10"/>
-      <c r="C1042" s="10"/>
-      <c r="D1042" s="10"/>
+      <c r="B1042" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1042" s="10">
+        <v>85</v>
+      </c>
+      <c r="D1042" s="10">
+        <v>263</v>
+      </c>
       <c r="E1042" s="10" t="s">
         <v>4165</v>
       </c>
@@ -48071,9 +48247,15 @@
     </row>
     <row r="1043" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1043" s="10"/>
-      <c r="B1043" s="10"/>
-      <c r="C1043" s="10"/>
-      <c r="D1043" s="10"/>
+      <c r="B1043" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1043" s="10">
+        <v>345</v>
+      </c>
+      <c r="D1043" s="10">
+        <v>275</v>
+      </c>
       <c r="E1043" s="10" t="s">
         <v>4166</v>
       </c>
@@ -48123,9 +48305,15 @@
     </row>
     <row r="1045" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A1045" s="10"/>
-      <c r="B1045" s="10"/>
-      <c r="C1045" s="10"/>
-      <c r="D1045" s="10"/>
+      <c r="B1045" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1045" s="10">
+        <v>309</v>
+      </c>
+      <c r="D1045" s="10">
+        <v>274</v>
+      </c>
       <c r="E1045" s="10" t="s">
         <v>4168</v>
       </c>
@@ -48150,9 +48338,15 @@
     </row>
     <row r="1046" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1046" s="10"/>
-      <c r="B1046" s="10"/>
-      <c r="C1046" s="10"/>
-      <c r="D1046" s="10"/>
+      <c r="B1046" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1046" s="10">
+        <v>95</v>
+      </c>
+      <c r="D1046" s="10">
+        <v>264</v>
+      </c>
       <c r="E1046" s="10" t="s">
         <v>4169</v>
       </c>
@@ -48177,9 +48371,15 @@
     </row>
     <row r="1047" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1047" s="10"/>
-      <c r="B1047" s="10"/>
-      <c r="C1047" s="10"/>
-      <c r="D1047" s="10"/>
+      <c r="B1047" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1047" s="10">
+        <v>96</v>
+      </c>
+      <c r="D1047" s="10">
+        <v>264</v>
+      </c>
       <c r="E1047" s="10" t="s">
         <v>4170</v>
       </c>
@@ -48204,9 +48404,15 @@
     </row>
     <row r="1048" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1048" s="10"/>
-      <c r="B1048" s="10"/>
-      <c r="C1048" s="10"/>
-      <c r="D1048" s="10"/>
+      <c r="B1048" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1048" s="10">
+        <v>485</v>
+      </c>
+      <c r="D1048" s="10">
+        <v>281</v>
+      </c>
       <c r="E1048" s="10" t="s">
         <v>4171</v>
       </c>
@@ -48231,9 +48437,15 @@
     </row>
     <row r="1049" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1049" s="10"/>
-      <c r="B1049" s="10"/>
-      <c r="C1049" s="10"/>
-      <c r="D1049" s="10"/>
+      <c r="B1049" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1049" s="10">
+        <v>437</v>
+      </c>
+      <c r="D1049" s="10">
+        <v>279</v>
+      </c>
       <c r="E1049" s="10" t="s">
         <v>4172</v>
       </c>
@@ -48258,9 +48470,15 @@
     </row>
     <row r="1050" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1050" s="10"/>
-      <c r="B1050" s="10"/>
-      <c r="C1050" s="10"/>
-      <c r="D1050" s="10"/>
+      <c r="B1050" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1050" s="10">
+        <v>546</v>
+      </c>
+      <c r="D1050" s="10">
+        <v>284</v>
+      </c>
       <c r="E1050" s="10" t="s">
         <v>4173</v>
       </c>
@@ -48312,9 +48530,15 @@
     </row>
     <row r="1052" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1052" s="10"/>
-      <c r="B1052" s="10"/>
-      <c r="C1052" s="10"/>
-      <c r="D1052" s="10"/>
+      <c r="B1052" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1052" s="10">
+        <v>588</v>
+      </c>
+      <c r="D1052" s="10">
+        <v>285</v>
+      </c>
       <c r="E1052" s="10" t="s">
         <v>4175</v>
       </c>
@@ -48339,9 +48563,15 @@
     </row>
     <row r="1053" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1053" s="10"/>
-      <c r="B1053" s="10"/>
-      <c r="C1053" s="10"/>
-      <c r="D1053" s="10"/>
+      <c r="B1053" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1053" s="10">
+        <v>556</v>
+      </c>
+      <c r="D1053" s="10">
+        <v>284</v>
+      </c>
       <c r="E1053" s="10" t="s">
         <v>4176</v>
       </c>
@@ -48393,9 +48623,15 @@
     </row>
     <row r="1055" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1055" s="10"/>
-      <c r="B1055" s="10"/>
-      <c r="C1055" s="10"/>
-      <c r="D1055" s="10"/>
+      <c r="B1055" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1055" s="10">
+        <v>684</v>
+      </c>
+      <c r="D1055" s="10">
+        <v>289</v>
+      </c>
       <c r="E1055" s="10" t="s">
         <v>4178</v>
       </c>
@@ -48420,9 +48656,15 @@
     </row>
     <row r="1056" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1056" s="10"/>
-      <c r="B1056" s="10"/>
-      <c r="C1056" s="10"/>
-      <c r="D1056" s="10"/>
+      <c r="B1056" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1056" s="10">
+        <v>616</v>
+      </c>
+      <c r="D1056" s="10">
+        <v>286</v>
+      </c>
       <c r="E1056" s="10" t="s">
         <v>4179</v>
       </c>
@@ -48445,9 +48687,15 @@
     </row>
     <row r="1057" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1057" s="10"/>
-      <c r="B1057" s="10"/>
-      <c r="C1057" s="10"/>
-      <c r="D1057" s="10"/>
+      <c r="B1057" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1057" s="10">
+        <v>640</v>
+      </c>
+      <c r="D1057" s="10">
+        <v>287</v>
+      </c>
       <c r="E1057" s="10" t="s">
         <v>4180</v>
       </c>
@@ -48472,9 +48720,15 @@
     </row>
     <row r="1058" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1058" s="10"/>
-      <c r="B1058" s="10"/>
-      <c r="C1058" s="10"/>
-      <c r="D1058" s="10"/>
+      <c r="B1058" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1058" s="10">
+        <v>593</v>
+      </c>
+      <c r="D1058" s="10">
+        <v>285</v>
+      </c>
       <c r="E1058" s="10" t="s">
         <v>4181</v>
       </c>
@@ -48499,9 +48753,15 @@
     </row>
     <row r="1059" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1059" s="10"/>
-      <c r="B1059" s="10"/>
-      <c r="C1059" s="10"/>
-      <c r="D1059" s="10"/>
+      <c r="B1059" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1059" s="10">
+        <v>560</v>
+      </c>
+      <c r="D1059" s="10">
+        <v>284</v>
+      </c>
       <c r="E1059" s="10" t="s">
         <v>4182</v>
       </c>
@@ -48526,9 +48786,15 @@
     </row>
     <row r="1060" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A1060" s="10"/>
-      <c r="B1060" s="10"/>
-      <c r="C1060" s="10"/>
-      <c r="D1060" s="10"/>
+      <c r="B1060" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1060" s="10">
+        <v>681</v>
+      </c>
+      <c r="D1060" s="10">
+        <v>288</v>
+      </c>
       <c r="E1060" s="10" t="s">
         <v>4183</v>
       </c>
@@ -48553,9 +48819,15 @@
     </row>
     <row r="1061" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1061" s="10"/>
-      <c r="B1061" s="10"/>
-      <c r="C1061" s="10"/>
-      <c r="D1061" s="10"/>
+      <c r="B1061" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1061" s="10">
+        <v>720</v>
+      </c>
+      <c r="D1061" s="10">
+        <v>290</v>
+      </c>
       <c r="E1061" s="10" t="s">
         <v>4184</v>
       </c>
@@ -48580,9 +48852,15 @@
     </row>
     <row r="1062" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1062" s="10"/>
-      <c r="B1062" s="10"/>
-      <c r="C1062" s="10"/>
-      <c r="D1062" s="10"/>
+      <c r="B1062" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1062" s="10">
+        <v>694</v>
+      </c>
+      <c r="D1062" s="10">
+        <v>289</v>
+      </c>
       <c r="E1062" s="10" t="s">
         <v>4185</v>
       </c>
@@ -48607,9 +48885,15 @@
     </row>
     <row r="1063" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1063" s="10"/>
-      <c r="B1063" s="10"/>
-      <c r="C1063" s="10"/>
-      <c r="D1063" s="10"/>
+      <c r="B1063" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1063" s="10">
+        <v>736</v>
+      </c>
+      <c r="D1063" s="10">
+        <v>290</v>
+      </c>
       <c r="E1063" s="10" t="s">
         <v>4186</v>
       </c>
@@ -48634,9 +48918,15 @@
     </row>
     <row r="1064" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1064" s="10"/>
-      <c r="B1064" s="10"/>
-      <c r="C1064" s="10"/>
-      <c r="D1064" s="10"/>
+      <c r="B1064" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1064" s="10">
+        <v>715</v>
+      </c>
+      <c r="D1064" s="10">
+        <v>289</v>
+      </c>
       <c r="E1064" s="10" t="s">
         <v>4187</v>
       </c>
@@ -48661,9 +48951,15 @@
     </row>
     <row r="1065" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1065" s="10"/>
-      <c r="B1065" s="10"/>
-      <c r="C1065" s="10"/>
-      <c r="D1065" s="10"/>
+      <c r="B1065" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1065" s="10">
+        <v>704</v>
+      </c>
+      <c r="D1065" s="10">
+        <v>289</v>
+      </c>
       <c r="E1065" s="10" t="s">
         <v>4188</v>
       </c>
@@ -48688,9 +48984,15 @@
     </row>
     <row r="1066" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1066" s="10"/>
-      <c r="B1066" s="10"/>
-      <c r="C1066" s="10"/>
-      <c r="D1066" s="10"/>
+      <c r="B1066" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1066" s="10">
+        <v>821</v>
+      </c>
+      <c r="D1066" s="10">
+        <v>293</v>
+      </c>
       <c r="E1066" s="10" t="s">
         <v>4189</v>
       </c>
@@ -48715,9 +49017,15 @@
     </row>
     <row r="1067" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1067" s="10"/>
-      <c r="B1067" s="10"/>
-      <c r="C1067" s="10"/>
-      <c r="D1067" s="10"/>
+      <c r="B1067" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1067" s="10">
+        <v>783</v>
+      </c>
+      <c r="D1067" s="10">
+        <v>292</v>
+      </c>
       <c r="E1067" s="10" t="s">
         <v>4190</v>
       </c>
@@ -48767,9 +49075,15 @@
     </row>
     <row r="1069" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1069" s="10"/>
-      <c r="B1069" s="10"/>
-      <c r="C1069" s="10"/>
-      <c r="D1069" s="10"/>
+      <c r="B1069" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1069" s="10">
+        <v>803</v>
+      </c>
+      <c r="D1069" s="10">
+        <v>292</v>
+      </c>
       <c r="E1069" s="10" t="s">
         <v>4192</v>
       </c>
@@ -48794,9 +49108,15 @@
     </row>
     <row r="1070" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1070" s="10"/>
-      <c r="B1070" s="10"/>
-      <c r="C1070" s="10"/>
-      <c r="D1070" s="10"/>
+      <c r="B1070" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1070" s="10">
+        <v>832</v>
+      </c>
+      <c r="D1070" s="10">
+        <v>294</v>
+      </c>
       <c r="E1070" s="10" t="s">
         <v>4193</v>
       </c>
@@ -48821,9 +49141,15 @@
     </row>
     <row r="1071" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1071" s="10"/>
-      <c r="B1071" s="10"/>
-      <c r="C1071" s="10"/>
-      <c r="D1071" s="10"/>
+      <c r="B1071" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1071" s="10">
+        <v>814</v>
+      </c>
+      <c r="D1071" s="10">
+        <v>293</v>
+      </c>
       <c r="E1071" s="10" t="s">
         <v>4194</v>
       </c>
@@ -48846,9 +49172,15 @@
     </row>
     <row r="1072" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1072" s="10"/>
-      <c r="B1072" s="10"/>
-      <c r="C1072" s="10"/>
-      <c r="D1072" s="10"/>
+      <c r="B1072" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1072" s="10">
+        <v>827</v>
+      </c>
+      <c r="D1072" s="10">
+        <v>293</v>
+      </c>
       <c r="E1072" s="10" t="s">
         <v>4195</v>
       </c>
@@ -48873,9 +49205,15 @@
     </row>
     <row r="1073" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1073" s="10"/>
-      <c r="B1073" s="10"/>
-      <c r="C1073" s="10"/>
-      <c r="D1073" s="10"/>
+      <c r="B1073" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1073" s="10">
+        <v>818</v>
+      </c>
+      <c r="D1073" s="10">
+        <v>293</v>
+      </c>
       <c r="E1073" s="10" t="s">
         <v>4196</v>
       </c>
@@ -48900,9 +49238,15 @@
     </row>
     <row r="1074" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1074" s="10"/>
-      <c r="B1074" s="10"/>
-      <c r="C1074" s="10"/>
-      <c r="D1074" s="10"/>
+      <c r="B1074" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1074" s="10">
+        <v>834</v>
+      </c>
+      <c r="D1074" s="10">
+        <v>294</v>
+      </c>
       <c r="E1074" s="10" t="s">
         <v>4197</v>
       </c>
@@ -48925,9 +49269,15 @@
     </row>
     <row r="1075" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1075" s="10"/>
-      <c r="B1075" s="10"/>
-      <c r="C1075" s="10"/>
-      <c r="D1075" s="10"/>
+      <c r="B1075" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1075" s="10">
+        <v>3542</v>
+      </c>
+      <c r="D1075" s="10">
+        <v>392</v>
+      </c>
       <c r="E1075" s="10" t="s">
         <v>4198</v>
       </c>
@@ -48952,9 +49302,15 @@
     </row>
     <row r="1076" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1076" s="10"/>
-      <c r="B1076" s="10"/>
-      <c r="C1076" s="10"/>
-      <c r="D1076" s="10"/>
+      <c r="B1076" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1076" s="10">
+        <v>3568</v>
+      </c>
+      <c r="D1076" s="10">
+        <v>393</v>
+      </c>
       <c r="E1076" s="10" t="s">
         <v>4199</v>
       </c>
@@ -48979,9 +49335,15 @@
     </row>
     <row r="1077" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1077" s="10"/>
-      <c r="B1077" s="10"/>
-      <c r="C1077" s="10"/>
-      <c r="D1077" s="10"/>
+      <c r="B1077" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1077" s="10">
+        <v>3636</v>
+      </c>
+      <c r="D1077" s="10">
+        <v>396</v>
+      </c>
       <c r="E1077" s="10" t="s">
         <v>4200</v>
       </c>
@@ -49004,9 +49366,15 @@
     </row>
     <row r="1078" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1078" s="10"/>
-      <c r="B1078" s="10"/>
-      <c r="C1078" s="10"/>
-      <c r="D1078" s="10"/>
+      <c r="B1078" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1078" s="10">
+        <v>3619</v>
+      </c>
+      <c r="D1078" s="10">
+        <v>395</v>
+      </c>
       <c r="E1078" s="10" t="s">
         <v>4201</v>
       </c>
@@ -49031,9 +49399,15 @@
     </row>
     <row r="1079" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1079" s="10"/>
-      <c r="B1079" s="10"/>
-      <c r="C1079" s="10"/>
-      <c r="D1079" s="10"/>
+      <c r="B1079" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1079" s="10">
+        <v>3537</v>
+      </c>
+      <c r="D1079" s="10">
+        <v>391</v>
+      </c>
       <c r="E1079" s="10" t="s">
         <v>4202</v>
       </c>
@@ -49058,9 +49432,15 @@
     </row>
     <row r="1080" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1080" s="10"/>
-      <c r="B1080" s="10"/>
-      <c r="C1080" s="10"/>
-      <c r="D1080" s="10"/>
+      <c r="B1080" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1080" s="10">
+        <v>3966</v>
+      </c>
+      <c r="D1080" s="10">
+        <v>437</v>
+      </c>
       <c r="E1080" s="10" t="s">
         <v>4203</v>
       </c>
@@ -49085,9 +49465,15 @@
     </row>
     <row r="1081" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1081" s="10"/>
-      <c r="B1081" s="10"/>
-      <c r="C1081" s="10"/>
-      <c r="D1081" s="10"/>
+      <c r="B1081" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1081" s="10">
+        <v>2401</v>
+      </c>
+      <c r="D1081" s="10">
+        <v>359</v>
+      </c>
       <c r="E1081" s="10" t="s">
         <v>4204</v>
       </c>
@@ -49112,9 +49498,15 @@
     </row>
     <row r="1082" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1082" s="10"/>
-      <c r="B1082" s="10"/>
-      <c r="C1082" s="10"/>
-      <c r="D1082" s="10"/>
+      <c r="B1082" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1082" s="10">
+        <v>2615</v>
+      </c>
+      <c r="D1082" s="10">
+        <v>369</v>
+      </c>
       <c r="E1082" s="10" t="s">
         <v>4205</v>
       </c>
@@ -49139,9 +49531,15 @@
     </row>
     <row r="1083" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1083" s="10"/>
-      <c r="B1083" s="10"/>
-      <c r="C1083" s="10"/>
-      <c r="D1083" s="10"/>
+      <c r="B1083" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1083" s="10">
+        <v>2931</v>
+      </c>
+      <c r="D1083" s="10">
+        <v>384</v>
+      </c>
       <c r="E1083" s="10" t="s">
         <v>4206</v>
       </c>
@@ -49166,9 +49564,15 @@
     </row>
     <row r="1084" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1084" s="10"/>
-      <c r="B1084" s="10"/>
-      <c r="C1084" s="10"/>
-      <c r="D1084" s="10"/>
+      <c r="B1084" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1084" s="10">
+        <v>3390</v>
+      </c>
+      <c r="D1084" s="10">
+        <v>408</v>
+      </c>
       <c r="E1084" s="10" t="s">
         <v>4207</v>
       </c>
@@ -49220,9 +49624,15 @@
     </row>
     <row r="1086" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1086" s="10"/>
-      <c r="B1086" s="10"/>
-      <c r="C1086" s="10"/>
-      <c r="D1086" s="10"/>
+      <c r="B1086" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1086" s="10">
+        <v>1196</v>
+      </c>
+      <c r="D1086" s="10">
+        <v>295</v>
+      </c>
       <c r="E1086" s="10" t="s">
         <v>4209</v>
       </c>
@@ -49245,9 +49655,15 @@
     </row>
     <row r="1087" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1087" s="10"/>
-      <c r="B1087" s="10"/>
-      <c r="C1087" s="10"/>
-      <c r="D1087" s="10"/>
+      <c r="B1087" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1087" s="10">
+        <v>3515</v>
+      </c>
+      <c r="D1087" s="10">
+        <v>414</v>
+      </c>
       <c r="E1087" s="10" t="s">
         <v>4210</v>
       </c>
@@ -49272,9 +49688,15 @@
     </row>
     <row r="1088" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1088" s="10"/>
-      <c r="B1088" s="10"/>
-      <c r="C1088" s="10"/>
-      <c r="D1088" s="10"/>
+      <c r="B1088" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1088" s="10">
+        <v>120</v>
+      </c>
+      <c r="D1088" s="10">
+        <v>242</v>
+      </c>
       <c r="E1088" s="10" t="s">
         <v>4211</v>
       </c>
@@ -49297,9 +49719,15 @@
     </row>
     <row r="1089" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1089" s="10"/>
-      <c r="B1089" s="10"/>
-      <c r="C1089" s="10"/>
-      <c r="D1089" s="10"/>
+      <c r="B1089" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1089" s="10">
+        <v>2451</v>
+      </c>
+      <c r="D1089" s="10">
+        <v>362</v>
+      </c>
       <c r="E1089" s="10" t="s">
         <v>4212</v>
       </c>
@@ -49324,9 +49752,15 @@
     </row>
     <row r="1090" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1090" s="10"/>
-      <c r="B1090" s="10"/>
-      <c r="C1090" s="10"/>
-      <c r="D1090" s="10"/>
+      <c r="B1090" s="10">
+        <v>1994</v>
+      </c>
+      <c r="C1090" s="10">
+        <v>4297</v>
+      </c>
+      <c r="D1090" s="10">
+        <v>453</v>
+      </c>
       <c r="E1090" s="10" t="s">
         <v>4213</v>
       </c>
@@ -49349,9 +49783,15 @@
     </row>
     <row r="1091" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1091" s="10"/>
-      <c r="B1091" s="10"/>
-      <c r="C1091" s="10"/>
-      <c r="D1091" s="10"/>
+      <c r="B1091" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1091" s="10">
+        <v>590</v>
+      </c>
+      <c r="D1091" s="10">
+        <v>385</v>
+      </c>
       <c r="E1091" s="10" t="s">
         <v>4214</v>
       </c>
@@ -49376,9 +49816,15 @@
     </row>
     <row r="1092" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1092" s="10"/>
-      <c r="B1092" s="10"/>
-      <c r="C1092" s="10"/>
-      <c r="D1092" s="10"/>
+      <c r="B1092" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1092" s="10">
+        <v>5417</v>
+      </c>
+      <c r="D1092" s="10">
+        <v>635</v>
+      </c>
       <c r="E1092" s="10" t="s">
         <v>4215</v>
       </c>
@@ -49403,9 +49849,15 @@
     </row>
     <row r="1093" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1093" s="10"/>
-      <c r="B1093" s="10"/>
-      <c r="C1093" s="10"/>
-      <c r="D1093" s="10"/>
+      <c r="B1093" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1093" s="10">
+        <v>5275</v>
+      </c>
+      <c r="D1093" s="10">
+        <v>628</v>
+      </c>
       <c r="E1093" s="10" t="s">
         <v>4216</v>
       </c>
@@ -49430,9 +49882,15 @@
     </row>
     <row r="1094" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1094" s="10"/>
-      <c r="B1094" s="10"/>
-      <c r="C1094" s="10"/>
-      <c r="D1094" s="10"/>
+      <c r="B1094" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1094" s="10">
+        <v>5424</v>
+      </c>
+      <c r="D1094" s="10">
+        <v>636</v>
+      </c>
       <c r="E1094" s="10" t="s">
         <v>4217</v>
       </c>
@@ -49457,9 +49915,15 @@
     </row>
     <row r="1095" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1095" s="10"/>
-      <c r="B1095" s="10"/>
-      <c r="C1095" s="10"/>
-      <c r="D1095" s="10"/>
+      <c r="B1095" s="10">
+        <v>1995</v>
+      </c>
+      <c r="C1095" s="10">
+        <v>1245</v>
+      </c>
+      <c r="D1095" s="10">
+        <v>419</v>
+      </c>
       <c r="E1095" s="10" t="s">
         <v>4218</v>
       </c>
@@ -49482,9 +49946,15 @@
     </row>
     <row r="1096" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1096" s="10"/>
-      <c r="B1096" s="10"/>
-      <c r="C1096" s="10"/>
-      <c r="D1096" s="10"/>
+      <c r="B1096" s="10">
+        <v>1999</v>
+      </c>
+      <c r="C1096" s="10">
+        <v>4157</v>
+      </c>
+      <c r="D1096" s="10">
+        <v>570</v>
+      </c>
       <c r="E1096" s="10" t="s">
         <v>4219</v>
       </c>

</xml_diff>

<commit_message>
added page and year for two ivpr
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -14247,8 +14247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1095" sqref="C1095"/>
+    <sheetView tabSelected="1" topLeftCell="A1024" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1027" sqref="L1027"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47745,11 +47745,15 @@
     </row>
     <row r="1027" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1027" s="7"/>
-      <c r="B1027" s="7"/>
+      <c r="B1027" s="7">
+        <v>2020</v>
+      </c>
       <c r="C1027" s="7">
         <v>225</v>
       </c>
-      <c r="D1027" s="7"/>
+      <c r="D1027" s="7">
+        <v>198</v>
+      </c>
       <c r="E1027" s="7" t="s">
         <v>3871</v>
       </c>
@@ -53715,11 +53719,15 @@
     </row>
     <row r="1215" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A1215" s="10"/>
-      <c r="B1215" s="10"/>
+      <c r="B1215" s="10">
+        <v>2015</v>
+      </c>
       <c r="C1215" s="10">
         <v>261</v>
       </c>
-      <c r="D1215" s="10"/>
+      <c r="D1215" s="10">
+        <v>156</v>
+      </c>
       <c r="E1215" s="10" t="s">
         <v>4338</v>
       </c>

</xml_diff>

<commit_message>
added newly received phone numbers upto 3:49pm 16-feb-2024
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7599" uniqueCount="4485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7620" uniqueCount="4487">
   <si>
     <t>1994</t>
   </si>
@@ -13728,6 +13728,12 @@
   </si>
   <si>
     <t>UPDATE PHONE AND NAME</t>
+  </si>
+  <si>
+    <t>UPDATE PHONE (2)</t>
+  </si>
+  <si>
+    <t>JUPDATE PHONE (2)</t>
   </si>
 </sst>
 </file>
@@ -14265,8 +14271,8 @@
   </sheetPr>
   <dimension ref="A1:K1240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B125" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F127" sqref="A1:K1240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14320,8 +14326,8 @@
       <c r="A2" s="1">
         <v>4431</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+      <c r="B2" s="1">
+        <v>1994</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -14375,8 +14381,12 @@
       <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="5">
+        <v>9435050847</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -14930,8 +14940,12 @@
       <c r="I20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="1"/>
+      <c r="J20" s="5">
+        <v>8638580902</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -15358,7 +15372,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>4463</v>
       </c>
@@ -15386,8 +15400,12 @@
       <c r="I34" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="1"/>
+      <c r="J34" s="5">
+        <v>9864328100</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -16432,8 +16450,12 @@
       <c r="I66" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="J66" s="5"/>
-      <c r="K66" s="1"/>
+      <c r="J66" s="5">
+        <v>9435016076</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -16464,9 +16486,11 @@
         <v>292</v>
       </c>
       <c r="J67" s="6">
-        <v>9435109106</v>
-      </c>
-      <c r="K67" s="1"/>
+        <v>9101087240</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -20014,9 +20038,11 @@
         <v>735</v>
       </c>
       <c r="J175" s="6">
-        <v>9864848639</v>
-      </c>
-      <c r="K175" s="1"/>
+        <v>7002771001</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="176" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
@@ -20875,7 +20901,7 @@
         <v>9435312957</v>
       </c>
       <c r="K201" s="12" t="s">
-        <v>3779</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="202" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -23078,8 +23104,12 @@
       <c r="I268" s="1" t="s">
         <v>1151</v>
       </c>
-      <c r="J268" s="5"/>
-      <c r="K268" s="1"/>
+      <c r="J268" s="5">
+        <v>8638870192</v>
+      </c>
+      <c r="K268" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="269" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
@@ -24384,8 +24414,12 @@
       <c r="I308" s="1" t="s">
         <v>1322</v>
       </c>
-      <c r="J308" s="5"/>
-      <c r="K308" s="1"/>
+      <c r="J308" s="5">
+        <v>9435061785</v>
+      </c>
+      <c r="K308" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="309" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
@@ -26717,8 +26751,12 @@
       <c r="I379" s="1" t="s">
         <v>1630</v>
       </c>
-      <c r="J379" s="5"/>
-      <c r="K379" s="1"/>
+      <c r="J379" s="5">
+        <v>7002347341</v>
+      </c>
+      <c r="K379" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="380" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
@@ -27297,8 +27335,12 @@
       <c r="I397" s="1" t="s">
         <v>1703</v>
       </c>
-      <c r="J397" s="5"/>
-      <c r="K397" s="1"/>
+      <c r="J397" s="5">
+        <v>9916133405</v>
+      </c>
+      <c r="K397" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="398" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
@@ -28081,8 +28123,12 @@
       <c r="I421" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="J421" s="5"/>
-      <c r="K421" s="1"/>
+      <c r="J421" s="5">
+        <v>9678009368</v>
+      </c>
+      <c r="K421" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="422" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
@@ -28145,8 +28191,12 @@
       <c r="I423" s="1" t="s">
         <v>1809</v>
       </c>
-      <c r="J423" s="5"/>
-      <c r="K423" s="1"/>
+      <c r="J423" s="5">
+        <v>9435095751</v>
+      </c>
+      <c r="K423" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="424" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
@@ -28473,8 +28523,12 @@
       <c r="I433" s="1" t="s">
         <v>1852</v>
       </c>
-      <c r="J433" s="5"/>
-      <c r="K433" s="1"/>
+      <c r="J433" s="5">
+        <v>9435020575</v>
+      </c>
+      <c r="K433" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="434" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
@@ -29389,8 +29443,12 @@
       <c r="I461" s="1" t="s">
         <v>1974</v>
       </c>
-      <c r="J461" s="5"/>
-      <c r="K461" s="1"/>
+      <c r="J461" s="5">
+        <v>9586170777</v>
+      </c>
+      <c r="K461" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="462" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
@@ -30691,8 +30749,12 @@
       <c r="I501" s="1" t="s">
         <v>2141</v>
       </c>
-      <c r="J501" s="5"/>
-      <c r="K501" s="1"/>
+      <c r="J501" s="5">
+        <v>9971550644</v>
+      </c>
+      <c r="K501" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="502" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A502" s="1">
@@ -32430,8 +32492,12 @@
       <c r="I554" s="1" t="s">
         <v>2362</v>
       </c>
-      <c r="J554" s="5"/>
-      <c r="K554" s="1"/>
+      <c r="J554" s="5">
+        <v>9859910394</v>
+      </c>
+      <c r="K554" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="555" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A555" s="1">
@@ -32494,8 +32560,12 @@
       <c r="I556" s="1" t="s">
         <v>2371</v>
       </c>
-      <c r="J556" s="5"/>
-      <c r="K556" s="1"/>
+      <c r="J556" s="5">
+        <v>9864382221</v>
+      </c>
+      <c r="K556" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="557" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A557" s="1">
@@ -32620,8 +32690,12 @@
       <c r="I560" s="1" t="s">
         <v>2386</v>
       </c>
-      <c r="J560" s="5"/>
-      <c r="K560" s="1"/>
+      <c r="J560" s="5">
+        <v>9707024408</v>
+      </c>
+      <c r="K560" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="561" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A561" s="1">
@@ -32973,8 +33047,12 @@
       <c r="I571" s="1" t="s">
         <v>2433</v>
       </c>
-      <c r="J571" s="5"/>
-      <c r="K571" s="1"/>
+      <c r="J571" s="5">
+        <v>9707681843</v>
+      </c>
+      <c r="K571" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="572" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A572" s="1">
@@ -33204,8 +33282,12 @@
       <c r="I578" s="1" t="s">
         <v>2460</v>
       </c>
-      <c r="J578" s="5"/>
-      <c r="K578" s="1"/>
+      <c r="J578" s="5">
+        <v>9864743034</v>
+      </c>
+      <c r="K578" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="579" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A579" s="1">
@@ -33301,8 +33383,12 @@
       <c r="I581" s="1" t="s">
         <v>2473</v>
       </c>
-      <c r="J581" s="5"/>
-      <c r="K581" s="1"/>
+      <c r="J581" s="5">
+        <v>9864811414</v>
+      </c>
+      <c r="K581" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="582" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A582" s="1">
@@ -38585,9 +38671,11 @@
         <v>3040</v>
       </c>
       <c r="J740" s="6">
-        <v>8011501506</v>
-      </c>
-      <c r="K740" s="1"/>
+        <v>6001576058</v>
+      </c>
+      <c r="K740" s="1" t="s">
+        <v>4485</v>
+      </c>
     </row>
     <row r="741" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A741" s="1">
@@ -47680,9 +47768,11 @@
       <c r="I1018" s="7" t="s">
         <v>3913</v>
       </c>
-      <c r="J1018" s="9"/>
+      <c r="J1018" s="9">
+        <v>8059556620</v>
+      </c>
       <c r="K1018" s="7" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1019" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -49561,9 +49651,11 @@
       <c r="I1077" s="10" t="s">
         <v>3971</v>
       </c>
-      <c r="J1077" s="10"/>
+      <c r="J1077" s="10">
+        <v>9101477435</v>
+      </c>
       <c r="K1077" s="10" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1078" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -51409,9 +51501,11 @@
       <c r="I1135" s="10" t="s">
         <v>4029</v>
       </c>
-      <c r="J1135" s="10"/>
+      <c r="J1135" s="10">
+        <v>9401274039</v>
+      </c>
       <c r="K1135" s="10" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1136" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -52148,9 +52242,11 @@
       <c r="I1158" s="10" t="s">
         <v>4052</v>
       </c>
-      <c r="J1158" s="10"/>
+      <c r="J1158" s="10">
+        <v>9854119126</v>
+      </c>
       <c r="K1158" s="10" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1159" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -52433,9 +52529,11 @@
       <c r="I1167" s="10" t="s">
         <v>4061</v>
       </c>
-      <c r="J1167" s="10"/>
+      <c r="J1167" s="10">
+        <v>8133019095</v>
+      </c>
       <c r="K1167" s="10" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1168" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -53643,7 +53741,9 @@
       <c r="I1205" s="10" t="s">
         <v>4099</v>
       </c>
-      <c r="J1205" s="10"/>
+      <c r="J1205" s="10">
+        <v>8463803076</v>
+      </c>
       <c r="K1205" s="10" t="s">
         <v>3866</v>
       </c>
@@ -53740,9 +53840,11 @@
       <c r="I1208" s="10" t="s">
         <v>4102</v>
       </c>
-      <c r="J1208" s="10"/>
+      <c r="J1208" s="10">
+        <v>8638789035</v>
+      </c>
       <c r="K1208" s="10" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="1209" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -53928,9 +54030,11 @@
       <c r="I1214" s="10" t="s">
         <v>4108</v>
       </c>
-      <c r="J1214" s="10"/>
+      <c r="J1214" s="10">
+        <v>8146550405</v>
+      </c>
       <c r="K1214" s="10" t="s">
-        <v>3866</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="1215" spans="1:11" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new phone numbers upto 11:55am on 17-feb-2024
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -14268,8 +14268,8 @@
   </sheetPr>
   <dimension ref="A1:K1240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E161" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J167" sqref="J167"/>
+    <sheetView tabSelected="1" topLeftCell="E376" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E379" sqref="E379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46972,10 +46972,10 @@
         <v>3887</v>
       </c>
       <c r="J992" s="9">
-        <v>7086409597</v>
+        <v>9435064120</v>
       </c>
       <c r="K992" s="7" t="s">
-        <v>3866</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="993" spans="1:11" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added phone number upto 17 feb 2024
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -13294,9 +13294,6 @@
     <t>Production Officer. Institute of Vety. Biologicals, Khanapara, Guwahati-22</t>
   </si>
   <si>
-    <t>VAS. State Vety. Hospital, Nalbari, Dist. Nalbari</t>
-  </si>
-  <si>
     <t>Epidemiologist, NERDDL, Animal Health Centre, Khanapara,</t>
   </si>
   <si>
@@ -13731,6 +13728,9 @@
   </si>
   <si>
     <t>UPDATE PHONE (2)</t>
+  </si>
+  <si>
+    <t>Fodder Development Officer, Chenikuthi, Guwahati-03</t>
   </si>
 </sst>
 </file>
@@ -14268,8 +14268,8 @@
   </sheetPr>
   <dimension ref="A1:K1240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E376" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E379" sqref="E379"/>
+    <sheetView tabSelected="1" topLeftCell="E1065" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I1068" sqref="I1068"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14382,7 +14382,7 @@
         <v>9435050847</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -14471,7 +14471,7 @@
         <v>21459</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>4482</v>
+        <v>4481</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>5</v>
@@ -14483,7 +14483,7 @@
         <v>9435516621</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -14729,7 +14729,7 @@
         <v>21155</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>4478</v>
+        <v>4477</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>5</v>
@@ -14741,7 +14741,7 @@
         <v>7002191047</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>4483</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -14941,7 +14941,7 @@
         <v>8638580902</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -15401,7 +15401,7 @@
         <v>9864328100</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -15795,7 +15795,7 @@
         <v>9435328038</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -15989,7 +15989,7 @@
         <v>8135027078</v>
       </c>
       <c r="K52" s="12" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -16451,7 +16451,7 @@
         <v>9435016076</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -16486,7 +16486,7 @@
         <v>9101087240</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -19721,13 +19721,13 @@
         <v>565</v>
       </c>
       <c r="E166" s="12" t="s">
-        <v>4479</v>
+        <v>4478</v>
       </c>
       <c r="F166" s="13">
         <v>24699</v>
       </c>
       <c r="G166" s="12" t="s">
-        <v>4480</v>
+        <v>4479</v>
       </c>
       <c r="H166" s="12" t="s">
         <v>5</v>
@@ -19739,7 +19739,7 @@
         <v>7002102453</v>
       </c>
       <c r="K166" s="12" t="s">
-        <v>4481</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -20038,7 +20038,7 @@
         <v>7002771001</v>
       </c>
       <c r="K175" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="176" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -20898,7 +20898,7 @@
         <v>9435312957</v>
       </c>
       <c r="K201" s="12" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="202" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -22765,7 +22765,7 @@
         <v>25476</v>
       </c>
       <c r="G258" s="12" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
       <c r="H258" s="12" t="s">
         <v>5</v>
@@ -22777,7 +22777,7 @@
         <v>8876405881</v>
       </c>
       <c r="K258" s="12" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="259" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -23105,7 +23105,7 @@
         <v>8638870192</v>
       </c>
       <c r="K268" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="269" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -23448,7 +23448,7 @@
         <v>1191</v>
       </c>
       <c r="E279" s="17" t="s">
-        <v>4431</v>
+        <v>4430</v>
       </c>
       <c r="F279" s="18" t="s">
         <v>1195</v>
@@ -23458,13 +23458,13 @@
         <v>5</v>
       </c>
       <c r="I279" s="17" t="s">
-        <v>4432</v>
+        <v>4431</v>
       </c>
       <c r="J279" s="19">
         <v>9859085665</v>
       </c>
       <c r="K279" s="17" t="s">
-        <v>4437</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="280" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -24415,7 +24415,7 @@
         <v>9435061785</v>
       </c>
       <c r="K308" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="309" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -25224,7 +25224,7 @@
         <v>26755</v>
       </c>
       <c r="G333" s="12" t="s">
-        <v>4473</v>
+        <v>4472</v>
       </c>
       <c r="H333" s="12" t="s">
         <v>5</v>
@@ -25236,7 +25236,7 @@
         <v>9508103776</v>
       </c>
       <c r="K333" s="12" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="334" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -25725,7 +25725,7 @@
         <v>5</v>
       </c>
       <c r="I348" s="1" t="s">
-        <v>4427</v>
+        <v>4426</v>
       </c>
       <c r="J348" s="5"/>
       <c r="K348" s="1"/>
@@ -26752,7 +26752,7 @@
         <v>7002347341</v>
       </c>
       <c r="K379" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="380" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -26841,7 +26841,7 @@
         <v>27572</v>
       </c>
       <c r="G382" s="12" t="s">
-        <v>4476</v>
+        <v>4475</v>
       </c>
       <c r="H382" s="12" t="s">
         <v>5</v>
@@ -26853,7 +26853,7 @@
         <v>7002540689</v>
       </c>
       <c r="K382" s="12" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="383" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -27336,7 +27336,7 @@
         <v>9916133405</v>
       </c>
       <c r="K397" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="398" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -28124,7 +28124,7 @@
         <v>9678009368</v>
       </c>
       <c r="K421" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="422" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -28192,7 +28192,7 @@
         <v>9435095751</v>
       </c>
       <c r="K423" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="424" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -28524,7 +28524,7 @@
         <v>9435020575</v>
       </c>
       <c r="K433" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="434" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -29312,7 +29312,7 @@
         <v>9854323619</v>
       </c>
       <c r="K457" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="458" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -29446,7 +29446,7 @@
         <v>9586170777</v>
       </c>
       <c r="K461" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="462" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -30340,7 +30340,7 @@
         <v>2087</v>
       </c>
       <c r="E489" s="12" t="s">
-        <v>4472</v>
+        <v>4471</v>
       </c>
       <c r="F489" s="13">
         <v>29573</v>
@@ -30358,7 +30358,7 @@
         <v>9864348963</v>
       </c>
       <c r="K489" s="12" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="490" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -30752,7 +30752,7 @@
         <v>9971550644</v>
       </c>
       <c r="K501" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="502" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -30833,7 +30833,7 @@
         <v>923</v>
       </c>
       <c r="E504" s="12" t="s">
-        <v>4475</v>
+        <v>4474</v>
       </c>
       <c r="F504" s="13">
         <v>29688</v>
@@ -30851,7 +30851,7 @@
         <v>9864238491</v>
       </c>
       <c r="K504" s="12" t="s">
-        <v>4484</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="505" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -31163,7 +31163,7 @@
         <v>1531</v>
       </c>
       <c r="E514" s="12" t="s">
-        <v>4470</v>
+        <v>4469</v>
       </c>
       <c r="F514" s="13">
         <v>30589</v>
@@ -31181,7 +31181,7 @@
         <v>7002908690</v>
       </c>
       <c r="K514" s="12" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="515" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -32495,7 +32495,7 @@
         <v>9859910394</v>
       </c>
       <c r="K554" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="555" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -32563,7 +32563,7 @@
         <v>9864382221</v>
       </c>
       <c r="K556" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="557" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -32693,7 +32693,7 @@
         <v>9707024408</v>
       </c>
       <c r="K560" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="561" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -33050,7 +33050,7 @@
         <v>9707681843</v>
       </c>
       <c r="K571" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="572" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -33285,7 +33285,7 @@
         <v>9864743034</v>
       </c>
       <c r="K578" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="579" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -33386,7 +33386,7 @@
         <v>9864811414</v>
       </c>
       <c r="K581" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="582" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -36821,7 +36821,7 @@
         <v>8876161334</v>
       </c>
       <c r="K684" s="12" t="s">
-        <v>4477</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="685" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -38673,7 +38673,7 @@
         <v>6001576058</v>
       </c>
       <c r="K740" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="741" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -42027,7 +42027,7 @@
         <v>292</v>
       </c>
       <c r="E842" s="12" t="s">
-        <v>4474</v>
+        <v>4473</v>
       </c>
       <c r="F842" s="13">
         <v>35446</v>
@@ -42045,7 +42045,7 @@
         <v>7086752581</v>
       </c>
       <c r="K842" s="12" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="843" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -42938,7 +42938,7 @@
         <v>9435673248</v>
       </c>
       <c r="K869" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="870" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -43270,7 +43270,7 @@
         <v>9101763282</v>
       </c>
       <c r="K879" s="1" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="880" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -46288,29 +46288,29 @@
         <v>0</v>
       </c>
       <c r="C971" s="17" t="s">
-        <v>4433</v>
+        <v>4432</v>
       </c>
       <c r="D971" s="17" t="s">
         <v>303</v>
       </c>
       <c r="E971" s="17" t="s">
-        <v>4434</v>
+        <v>4433</v>
       </c>
       <c r="F971" s="18"/>
       <c r="G971" s="17" t="s">
+        <v>4434</v>
+      </c>
+      <c r="H971" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I971" s="17" t="s">
         <v>4435</v>
-      </c>
-      <c r="H971" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I971" s="17" t="s">
-        <v>4436</v>
       </c>
       <c r="J971" s="19">
         <v>9435345578</v>
       </c>
       <c r="K971" s="17" t="s">
-        <v>4437</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="972" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -46325,7 +46325,7 @@
         <v>274</v>
       </c>
       <c r="E972" s="7" t="s">
-        <v>4438</v>
+        <v>4437</v>
       </c>
       <c r="F972" s="8">
         <v>21922</v>
@@ -46391,7 +46391,7 @@
         <v>27</v>
       </c>
       <c r="E974" s="7" t="s">
-        <v>4439</v>
+        <v>4438</v>
       </c>
       <c r="F974" s="8">
         <v>22706</v>
@@ -46418,7 +46418,7 @@
       <c r="C975" s="7"/>
       <c r="D975" s="7"/>
       <c r="E975" s="7" t="s">
-        <v>4440</v>
+        <v>4439</v>
       </c>
       <c r="F975" s="8">
         <v>22288</v>
@@ -46445,7 +46445,7 @@
       <c r="C976" s="7"/>
       <c r="D976" s="7"/>
       <c r="E976" s="7" t="s">
-        <v>4441</v>
+        <v>4440</v>
       </c>
       <c r="F976" s="8">
         <v>21620</v>
@@ -46511,7 +46511,7 @@
         <v>46</v>
       </c>
       <c r="E978" s="7" t="s">
-        <v>4442</v>
+        <v>4441</v>
       </c>
       <c r="F978" s="8">
         <v>20375</v>
@@ -46577,7 +46577,7 @@
         <v>47</v>
       </c>
       <c r="E980" s="7" t="s">
-        <v>4443</v>
+        <v>4442</v>
       </c>
       <c r="F980" s="8">
         <v>23429</v>
@@ -46610,7 +46610,7 @@
         <v>49</v>
       </c>
       <c r="E981" s="7" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
       <c r="F981" s="8">
         <v>23102</v>
@@ -46643,7 +46643,7 @@
         <v>48</v>
       </c>
       <c r="E982" s="7" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
       <c r="F982" s="8">
         <v>22287</v>
@@ -46676,7 +46676,7 @@
         <v>53</v>
       </c>
       <c r="E983" s="7" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
       <c r="F983" s="8">
         <v>24110</v>
@@ -46703,7 +46703,7 @@
       <c r="C984" s="7"/>
       <c r="D984" s="7"/>
       <c r="E984" s="7" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
       <c r="F984" s="8">
         <v>23224</v>
@@ -46734,7 +46734,7 @@
         <v>234</v>
       </c>
       <c r="E985" s="7" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
       <c r="F985" s="8">
         <v>24166</v>
@@ -46827,7 +46827,7 @@
       <c r="C988" s="7"/>
       <c r="D988" s="7"/>
       <c r="E988" s="7" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
       <c r="F988" s="8">
         <v>24193</v>
@@ -46975,7 +46975,7 @@
         <v>9435064120</v>
       </c>
       <c r="K992" s="7" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="993" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -47389,7 +47389,7 @@
         <v>179</v>
       </c>
       <c r="E1006" s="7" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
       <c r="F1006" s="8">
         <v>27426</v>
@@ -47705,7 +47705,7 @@
         <v>27819</v>
       </c>
       <c r="G1016" s="7" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
       <c r="H1016" s="7" t="s">
         <v>5</v>
@@ -47775,7 +47775,7 @@
         <v>8059556620</v>
       </c>
       <c r="K1018" s="7" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1019" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -48049,19 +48049,19 @@
       <c r="C1028" s="7"/>
       <c r="D1028" s="7"/>
       <c r="E1028" s="7" t="s">
-        <v>4428</v>
+        <v>4427</v>
       </c>
       <c r="F1028" s="8">
         <v>35330</v>
       </c>
       <c r="G1028" s="7" t="s">
+        <v>4428</v>
+      </c>
+      <c r="H1028" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1028" s="7" t="s">
         <v>4429</v>
-      </c>
-      <c r="H1028" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1028" s="7" t="s">
-        <v>4430</v>
       </c>
       <c r="J1028" s="9">
         <v>7086516495</v>
@@ -48371,7 +48371,7 @@
         <v>273</v>
       </c>
       <c r="E1038" s="10" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
       <c r="F1038" s="11">
         <v>21489</v>
@@ -48470,7 +48470,7 @@
         <v>269</v>
       </c>
       <c r="E1041" s="10" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
       <c r="F1041" s="11">
         <v>19993</v>
@@ -48503,7 +48503,7 @@
         <v>263</v>
       </c>
       <c r="E1042" s="10" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
       <c r="F1042" s="11">
         <v>17292</v>
@@ -48691,7 +48691,7 @@
         <v>281</v>
       </c>
       <c r="E1048" s="10" t="s">
-        <v>4454</v>
+        <v>4453</v>
       </c>
       <c r="F1048" s="11">
         <v>22240</v>
@@ -48955,7 +48955,7 @@
         <v>286</v>
       </c>
       <c r="E1056" s="10" t="s">
-        <v>4455</v>
+        <v>4454</v>
       </c>
       <c r="F1056" s="11"/>
       <c r="G1056" s="10" t="s">
@@ -49019,7 +49019,7 @@
         <v>285</v>
       </c>
       <c r="E1058" s="10" t="s">
-        <v>4456</v>
+        <v>4455</v>
       </c>
       <c r="F1058" s="11">
         <v>21980</v>
@@ -49283,7 +49283,7 @@
         <v>293</v>
       </c>
       <c r="E1066" s="10" t="s">
-        <v>4457</v>
+        <v>4456</v>
       </c>
       <c r="F1066" s="11">
         <v>23802</v>
@@ -49355,7 +49355,7 @@
         <v>24108</v>
       </c>
       <c r="G1068" s="10" t="s">
-        <v>4342</v>
+        <v>4485</v>
       </c>
       <c r="H1068" s="10" t="s">
         <v>5</v>
@@ -49363,9 +49363,11 @@
       <c r="I1068" s="10" t="s">
         <v>3962</v>
       </c>
-      <c r="J1068" s="10"/>
+      <c r="J1068" s="10">
+        <v>6002683761</v>
+      </c>
       <c r="K1068" s="10" t="s">
-        <v>3866</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1069" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -49380,7 +49382,7 @@
         <v>292</v>
       </c>
       <c r="E1069" s="10" t="s">
-        <v>4458</v>
+        <v>4457</v>
       </c>
       <c r="F1069" s="11">
         <v>24167</v>
@@ -49413,13 +49415,13 @@
         <v>294</v>
       </c>
       <c r="E1070" s="10" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
       <c r="F1070" s="11">
         <v>24529</v>
       </c>
       <c r="G1070" s="10" t="s">
-        <v>4343</v>
+        <v>4342</v>
       </c>
       <c r="H1070" s="10" t="s">
         <v>5</v>
@@ -49452,7 +49454,7 @@
         <v>23986</v>
       </c>
       <c r="G1071" s="10" t="s">
-        <v>4344</v>
+        <v>4343</v>
       </c>
       <c r="H1071" s="10" t="s">
         <v>5</v>
@@ -49477,7 +49479,7 @@
         <v>293</v>
       </c>
       <c r="E1072" s="10" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
       <c r="F1072" s="11">
         <v>22883</v>
@@ -49516,7 +49518,7 @@
         <v>23380</v>
       </c>
       <c r="G1073" s="10" t="s">
-        <v>4345</v>
+        <v>4344</v>
       </c>
       <c r="H1073" s="10" t="s">
         <v>5</v>
@@ -49543,7 +49545,7 @@
         <v>294</v>
       </c>
       <c r="E1074" s="10" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
       <c r="F1074" s="11">
         <v>23071</v>
@@ -49580,7 +49582,7 @@
         <v>24532</v>
       </c>
       <c r="G1075" s="10" t="s">
-        <v>4346</v>
+        <v>4345</v>
       </c>
       <c r="H1075" s="10" t="s">
         <v>5</v>
@@ -49613,7 +49615,7 @@
         <v>24504</v>
       </c>
       <c r="G1076" s="10" t="s">
-        <v>4347</v>
+        <v>4346</v>
       </c>
       <c r="H1076" s="10" t="s">
         <v>5</v>
@@ -49658,7 +49660,7 @@
         <v>9101477435</v>
       </c>
       <c r="K1077" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1078" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -49679,7 +49681,7 @@
         <v>19176</v>
       </c>
       <c r="G1078" s="10" t="s">
-        <v>4348</v>
+        <v>4347</v>
       </c>
       <c r="H1078" s="10" t="s">
         <v>5</v>
@@ -49706,7 +49708,7 @@
         <v>391</v>
       </c>
       <c r="E1079" s="10" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
       <c r="F1079" s="11">
         <v>24706</v>
@@ -49778,7 +49780,7 @@
         <v>24504</v>
       </c>
       <c r="G1081" s="10" t="s">
-        <v>4349</v>
+        <v>4348</v>
       </c>
       <c r="H1081" s="10" t="s">
         <v>5</v>
@@ -49805,7 +49807,7 @@
         <v>369</v>
       </c>
       <c r="E1082" s="10" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
       <c r="F1082" s="11">
         <v>25263</v>
@@ -49910,7 +49912,7 @@
         <v>24838</v>
       </c>
       <c r="G1085" s="10" t="s">
-        <v>4350</v>
+        <v>4349</v>
       </c>
       <c r="H1085" s="10" t="s">
         <v>5</v>
@@ -50067,7 +50069,7 @@
         <v>453</v>
       </c>
       <c r="E1090" s="10" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
       <c r="F1090" s="11">
         <v>24898</v>
@@ -50104,7 +50106,7 @@
         <v>23822</v>
       </c>
       <c r="G1091" s="10" t="s">
-        <v>4351</v>
+        <v>4350</v>
       </c>
       <c r="H1091" s="10" t="s">
         <v>5</v>
@@ -50267,7 +50269,7 @@
         <v>21667</v>
       </c>
       <c r="G1096" s="10" t="s">
-        <v>4352</v>
+        <v>4351</v>
       </c>
       <c r="H1096" s="10" t="s">
         <v>5</v>
@@ -50294,7 +50296,7 @@
         <v>25842</v>
       </c>
       <c r="G1097" s="10" t="s">
-        <v>4353</v>
+        <v>4352</v>
       </c>
       <c r="H1097" s="10" t="s">
         <v>5</v>
@@ -50327,7 +50329,7 @@
         <v>26360</v>
       </c>
       <c r="G1098" s="10" t="s">
-        <v>4354</v>
+        <v>4353</v>
       </c>
       <c r="H1098" s="10" t="s">
         <v>5</v>
@@ -50424,7 +50426,7 @@
         <v>25263</v>
       </c>
       <c r="G1101" s="10" t="s">
-        <v>4355</v>
+        <v>4354</v>
       </c>
       <c r="H1101" s="10" t="s">
         <v>5</v>
@@ -50490,7 +50492,7 @@
         <v>26665</v>
       </c>
       <c r="G1103" s="10" t="s">
-        <v>4356</v>
+        <v>4355</v>
       </c>
       <c r="H1103" s="10" t="s">
         <v>5</v>
@@ -50523,7 +50525,7 @@
         <v>26765</v>
       </c>
       <c r="G1104" s="10" t="s">
-        <v>4357</v>
+        <v>4356</v>
       </c>
       <c r="H1104" s="10" t="s">
         <v>5</v>
@@ -50622,7 +50624,7 @@
         <v>26531</v>
       </c>
       <c r="G1107" s="10" t="s">
-        <v>4358</v>
+        <v>4357</v>
       </c>
       <c r="H1107" s="10" t="s">
         <v>5</v>
@@ -50674,7 +50676,7 @@
       <c r="C1109" s="10"/>
       <c r="D1109" s="10"/>
       <c r="E1109" s="10" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
       <c r="F1109" s="11">
         <v>26665</v>
@@ -50765,7 +50767,7 @@
         <v>26313</v>
       </c>
       <c r="G1112" s="10" t="s">
-        <v>4353</v>
+        <v>4352</v>
       </c>
       <c r="H1112" s="10" t="s">
         <v>5</v>
@@ -50864,7 +50866,7 @@
         <v>27065</v>
       </c>
       <c r="G1115" s="10" t="s">
-        <v>4359</v>
+        <v>4358</v>
       </c>
       <c r="H1115" s="10" t="s">
         <v>5</v>
@@ -50928,7 +50930,7 @@
         <v>26359</v>
       </c>
       <c r="G1117" s="10" t="s">
-        <v>4360</v>
+        <v>4359</v>
       </c>
       <c r="H1117" s="10" t="s">
         <v>5</v>
@@ -51015,7 +51017,7 @@
         <v>26951</v>
       </c>
       <c r="G1120" s="10" t="s">
-        <v>4361</v>
+        <v>4360</v>
       </c>
       <c r="H1120" s="10" t="s">
         <v>5</v>
@@ -51112,7 +51114,7 @@
         <v>27030</v>
       </c>
       <c r="G1123" s="10" t="s">
-        <v>4362</v>
+        <v>4361</v>
       </c>
       <c r="H1123" s="10" t="s">
         <v>5</v>
@@ -51139,7 +51141,7 @@
         <v>181</v>
       </c>
       <c r="E1124" s="10" t="s">
-        <v>4466</v>
+        <v>4465</v>
       </c>
       <c r="F1124" s="11">
         <v>27061</v>
@@ -51207,7 +51209,7 @@
         <v>27454</v>
       </c>
       <c r="G1126" s="10" t="s">
-        <v>4363</v>
+        <v>4362</v>
       </c>
       <c r="H1126" s="10" t="s">
         <v>5</v>
@@ -51240,7 +51242,7 @@
         <v>27089</v>
       </c>
       <c r="G1127" s="10" t="s">
-        <v>4364</v>
+        <v>4363</v>
       </c>
       <c r="H1127" s="10" t="s">
         <v>5</v>
@@ -51304,7 +51306,7 @@
         <v>27058</v>
       </c>
       <c r="G1129" s="10" t="s">
-        <v>4365</v>
+        <v>4364</v>
       </c>
       <c r="H1129" s="10" t="s">
         <v>5</v>
@@ -51399,7 +51401,7 @@
         <v>28127</v>
       </c>
       <c r="G1132" s="10" t="s">
-        <v>4366</v>
+        <v>4365</v>
       </c>
       <c r="H1132" s="10" t="s">
         <v>5</v>
@@ -51432,7 +51434,7 @@
         <v>27303</v>
       </c>
       <c r="G1133" s="10" t="s">
-        <v>4367</v>
+        <v>4366</v>
       </c>
       <c r="H1133" s="10" t="s">
         <v>5</v>
@@ -51510,7 +51512,7 @@
         <v>9401274039</v>
       </c>
       <c r="K1135" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1136" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -51562,7 +51564,7 @@
         <v>28229</v>
       </c>
       <c r="G1137" s="10" t="s">
-        <v>4368</v>
+        <v>4367</v>
       </c>
       <c r="H1137" s="10" t="s">
         <v>5</v>
@@ -51595,7 +51597,7 @@
         <v>27420</v>
       </c>
       <c r="G1138" s="10" t="s">
-        <v>4369</v>
+        <v>4368</v>
       </c>
       <c r="H1138" s="10" t="s">
         <v>5</v>
@@ -51692,7 +51694,7 @@
         <v>28725</v>
       </c>
       <c r="G1141" s="10" t="s">
-        <v>4370</v>
+        <v>4369</v>
       </c>
       <c r="H1141" s="10" t="s">
         <v>5</v>
@@ -51725,7 +51727,7 @@
         <v>28516</v>
       </c>
       <c r="G1142" s="10" t="s">
-        <v>4371</v>
+        <v>4370</v>
       </c>
       <c r="H1142" s="10" t="s">
         <v>5</v>
@@ -51789,7 +51791,7 @@
         <v>29038</v>
       </c>
       <c r="G1144" s="10" t="s">
-        <v>4372</v>
+        <v>4371</v>
       </c>
       <c r="H1144" s="10" t="s">
         <v>5</v>
@@ -51884,7 +51886,7 @@
         <v>28887</v>
       </c>
       <c r="G1147" s="10" t="s">
-        <v>4373</v>
+        <v>4372</v>
       </c>
       <c r="H1147" s="10" t="s">
         <v>5</v>
@@ -51917,7 +51919,7 @@
         <v>29281</v>
       </c>
       <c r="G1148" s="10" t="s">
-        <v>4357</v>
+        <v>4356</v>
       </c>
       <c r="H1148" s="10" t="s">
         <v>5</v>
@@ -52014,7 +52016,7 @@
         <v>29271</v>
       </c>
       <c r="G1151" s="10" t="s">
-        <v>4374</v>
+        <v>4373</v>
       </c>
       <c r="H1151" s="10" t="s">
         <v>5</v>
@@ -52251,7 +52253,7 @@
         <v>9854119126</v>
       </c>
       <c r="K1158" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1159" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -52460,7 +52462,7 @@
         <v>30637</v>
       </c>
       <c r="G1165" s="10" t="s">
-        <v>4375</v>
+        <v>4374</v>
       </c>
       <c r="H1165" s="10" t="s">
         <v>5</v>
@@ -52493,7 +52495,7 @@
         <v>30852</v>
       </c>
       <c r="G1166" s="10" t="s">
-        <v>4376</v>
+        <v>4375</v>
       </c>
       <c r="H1166" s="10" t="s">
         <v>5</v>
@@ -52538,7 +52540,7 @@
         <v>8133019095</v>
       </c>
       <c r="K1167" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1168" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -52685,7 +52687,7 @@
         <v>30830</v>
       </c>
       <c r="G1172" s="10" t="s">
-        <v>4377</v>
+        <v>4376</v>
       </c>
       <c r="H1172" s="10" t="s">
         <v>5</v>
@@ -52718,7 +52720,7 @@
         <v>30920</v>
       </c>
       <c r="G1173" s="10" t="s">
-        <v>4378</v>
+        <v>4377</v>
       </c>
       <c r="H1173" s="10" t="s">
         <v>5</v>
@@ -52844,7 +52846,7 @@
         <v>30011</v>
       </c>
       <c r="G1177" s="10" t="s">
-        <v>4379</v>
+        <v>4378</v>
       </c>
       <c r="H1177" s="10" t="s">
         <v>5</v>
@@ -52910,7 +52912,7 @@
         <v>30742</v>
       </c>
       <c r="G1179" s="10" t="s">
-        <v>4380</v>
+        <v>4379</v>
       </c>
       <c r="H1179" s="10" t="s">
         <v>5</v>
@@ -52943,7 +52945,7 @@
         <v>30681</v>
       </c>
       <c r="G1180" s="10" t="s">
-        <v>4381</v>
+        <v>4380</v>
       </c>
       <c r="H1180" s="10" t="s">
         <v>5</v>
@@ -53292,7 +53294,7 @@
         <v>31442</v>
       </c>
       <c r="G1191" s="10" t="s">
-        <v>4378</v>
+        <v>4377</v>
       </c>
       <c r="H1191" s="10" t="s">
         <v>5</v>
@@ -53325,7 +53327,7 @@
         <v>31494</v>
       </c>
       <c r="G1192" s="10" t="s">
-        <v>4382</v>
+        <v>4381</v>
       </c>
       <c r="H1192" s="10" t="s">
         <v>5</v>
@@ -53420,7 +53422,7 @@
         <v>31837</v>
       </c>
       <c r="G1195" s="10" t="s">
-        <v>4383</v>
+        <v>4382</v>
       </c>
       <c r="H1195" s="10" t="s">
         <v>5</v>
@@ -53484,7 +53486,7 @@
         <v>32539</v>
       </c>
       <c r="G1197" s="10" t="s">
-        <v>4384</v>
+        <v>4383</v>
       </c>
       <c r="H1197" s="10" t="s">
         <v>5</v>
@@ -53515,7 +53517,7 @@
         <v>32178</v>
       </c>
       <c r="G1198" s="10" t="s">
-        <v>4385</v>
+        <v>4384</v>
       </c>
       <c r="H1198" s="10" t="s">
         <v>5</v>
@@ -53546,7 +53548,7 @@
         <v>32568</v>
       </c>
       <c r="G1199" s="10" t="s">
-        <v>4386</v>
+        <v>4385</v>
       </c>
       <c r="H1199" s="10" t="s">
         <v>5</v>
@@ -53579,7 +53581,7 @@
         <v>32504</v>
       </c>
       <c r="G1200" s="10" t="s">
-        <v>4387</v>
+        <v>4386</v>
       </c>
       <c r="H1200" s="10" t="s">
         <v>5</v>
@@ -53612,7 +53614,7 @@
         <v>29646</v>
       </c>
       <c r="G1201" s="10" t="s">
-        <v>4388</v>
+        <v>4387</v>
       </c>
       <c r="H1201" s="10" t="s">
         <v>5</v>
@@ -53643,7 +53645,7 @@
         <v>31331</v>
       </c>
       <c r="G1202" s="10" t="s">
-        <v>4389</v>
+        <v>4388</v>
       </c>
       <c r="H1202" s="10" t="s">
         <v>5</v>
@@ -53674,7 +53676,7 @@
         <v>31833</v>
       </c>
       <c r="G1203" s="10" t="s">
-        <v>4390</v>
+        <v>4389</v>
       </c>
       <c r="H1203" s="10" t="s">
         <v>5</v>
@@ -53707,7 +53709,7 @@
         <v>28785</v>
       </c>
       <c r="G1204" s="10" t="s">
-        <v>4391</v>
+        <v>4390</v>
       </c>
       <c r="H1204" s="10" t="s">
         <v>5</v>
@@ -53738,7 +53740,7 @@
         <v>32403</v>
       </c>
       <c r="G1205" s="10" t="s">
-        <v>4392</v>
+        <v>4391</v>
       </c>
       <c r="H1205" s="10" t="s">
         <v>5</v>
@@ -53771,7 +53773,7 @@
         <v>32164</v>
       </c>
       <c r="G1206" s="10" t="s">
-        <v>4393</v>
+        <v>4392</v>
       </c>
       <c r="H1206" s="10" t="s">
         <v>5</v>
@@ -53804,7 +53806,7 @@
         <v>32870</v>
       </c>
       <c r="G1207" s="10" t="s">
-        <v>4394</v>
+        <v>4393</v>
       </c>
       <c r="H1207" s="10" t="s">
         <v>5</v>
@@ -53837,7 +53839,7 @@
         <v>32774</v>
       </c>
       <c r="G1208" s="10" t="s">
-        <v>4395</v>
+        <v>4394</v>
       </c>
       <c r="H1208" s="10" t="s">
         <v>5</v>
@@ -53849,7 +53851,7 @@
         <v>8638789035</v>
       </c>
       <c r="K1208" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1209" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -53870,7 +53872,7 @@
         <v>33266</v>
       </c>
       <c r="G1209" s="10" t="s">
-        <v>4396</v>
+        <v>4395</v>
       </c>
       <c r="H1209" s="10" t="s">
         <v>5</v>
@@ -53901,7 +53903,7 @@
         <v>33693</v>
       </c>
       <c r="G1210" s="10" t="s">
-        <v>4397</v>
+        <v>4396</v>
       </c>
       <c r="H1210" s="10" t="s">
         <v>5</v>
@@ -53934,7 +53936,7 @@
         <v>32842</v>
       </c>
       <c r="G1211" s="10" t="s">
-        <v>4398</v>
+        <v>4397</v>
       </c>
       <c r="H1211" s="10" t="s">
         <v>5</v>
@@ -53965,7 +53967,7 @@
         <v>32690</v>
       </c>
       <c r="G1212" s="10" t="s">
-        <v>4399</v>
+        <v>4398</v>
       </c>
       <c r="H1212" s="10" t="s">
         <v>5</v>
@@ -53996,7 +53998,7 @@
         <v>31199</v>
       </c>
       <c r="G1213" s="10" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
       <c r="H1213" s="10" t="s">
         <v>5</v>
@@ -54027,7 +54029,7 @@
         <v>32896</v>
       </c>
       <c r="G1214" s="10" t="s">
-        <v>4401</v>
+        <v>4400</v>
       </c>
       <c r="H1214" s="10" t="s">
         <v>5</v>
@@ -54039,7 +54041,7 @@
         <v>8146550405</v>
       </c>
       <c r="K1214" s="10" t="s">
-        <v>4485</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1215" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -54060,7 +54062,7 @@
         <v>33216</v>
       </c>
       <c r="G1215" s="10" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
       <c r="H1215" s="10" t="s">
         <v>5</v>
@@ -54093,7 +54095,7 @@
         <v>31826</v>
       </c>
       <c r="G1216" s="10" t="s">
-        <v>4403</v>
+        <v>4402</v>
       </c>
       <c r="H1216" s="10" t="s">
         <v>5</v>
@@ -54126,7 +54128,7 @@
         <v>33134</v>
       </c>
       <c r="G1217" s="10" t="s">
-        <v>4404</v>
+        <v>4403</v>
       </c>
       <c r="H1217" s="10" t="s">
         <v>5</v>
@@ -54159,7 +54161,7 @@
         <v>33078</v>
       </c>
       <c r="G1218" s="10" t="s">
-        <v>4405</v>
+        <v>4404</v>
       </c>
       <c r="H1218" s="10" t="s">
         <v>5</v>
@@ -54192,7 +54194,7 @@
         <v>33451</v>
       </c>
       <c r="G1219" s="10" t="s">
-        <v>4406</v>
+        <v>4405</v>
       </c>
       <c r="H1219" s="10" t="s">
         <v>5</v>
@@ -54225,7 +54227,7 @@
         <v>33238</v>
       </c>
       <c r="G1220" s="10" t="s">
-        <v>4407</v>
+        <v>4406</v>
       </c>
       <c r="H1220" s="10" t="s">
         <v>5</v>
@@ -54258,7 +54260,7 @@
         <v>32143</v>
       </c>
       <c r="G1221" s="10" t="s">
-        <v>4408</v>
+        <v>4407</v>
       </c>
       <c r="H1221" s="10" t="s">
         <v>5</v>
@@ -54291,7 +54293,7 @@
         <v>33680</v>
       </c>
       <c r="G1222" s="10" t="s">
-        <v>4409</v>
+        <v>4408</v>
       </c>
       <c r="H1222" s="10" t="s">
         <v>5</v>
@@ -54324,7 +54326,7 @@
         <v>33159</v>
       </c>
       <c r="G1223" s="10" t="s">
-        <v>4410</v>
+        <v>4409</v>
       </c>
       <c r="H1223" s="10" t="s">
         <v>5</v>
@@ -54357,7 +54359,7 @@
         <v>33099</v>
       </c>
       <c r="G1224" s="10" t="s">
-        <v>4411</v>
+        <v>4410</v>
       </c>
       <c r="H1224" s="10" t="s">
         <v>5</v>
@@ -54390,7 +54392,7 @@
         <v>33645</v>
       </c>
       <c r="G1225" s="10" t="s">
-        <v>4412</v>
+        <v>4411</v>
       </c>
       <c r="H1225" s="10" t="s">
         <v>5</v>
@@ -54423,7 +54425,7 @@
         <v>33820</v>
       </c>
       <c r="G1226" s="10" t="s">
-        <v>4413</v>
+        <v>4412</v>
       </c>
       <c r="H1226" s="10" t="s">
         <v>5</v>
@@ -54456,7 +54458,7 @@
         <v>33970</v>
       </c>
       <c r="G1227" s="10" t="s">
-        <v>4414</v>
+        <v>4413</v>
       </c>
       <c r="H1227" s="10" t="s">
         <v>5</v>
@@ -54489,7 +54491,7 @@
         <v>33848</v>
       </c>
       <c r="G1228" s="10" t="s">
-        <v>4415</v>
+        <v>4414</v>
       </c>
       <c r="H1228" s="10" t="s">
         <v>5</v>
@@ -54522,7 +54524,7 @@
         <v>34022</v>
       </c>
       <c r="G1229" s="10" t="s">
-        <v>4416</v>
+        <v>4415</v>
       </c>
       <c r="H1229" s="10" t="s">
         <v>5</v>
@@ -54555,7 +54557,7 @@
         <v>33258</v>
       </c>
       <c r="G1230" s="10" t="s">
-        <v>4417</v>
+        <v>4416</v>
       </c>
       <c r="H1230" s="10" t="s">
         <v>5</v>
@@ -54588,7 +54590,7 @@
         <v>33580</v>
       </c>
       <c r="G1231" s="10" t="s">
-        <v>4418</v>
+        <v>4417</v>
       </c>
       <c r="H1231" s="10" t="s">
         <v>5</v>
@@ -54621,7 +54623,7 @@
         <v>34161</v>
       </c>
       <c r="G1232" s="10" t="s">
-        <v>4419</v>
+        <v>4418</v>
       </c>
       <c r="H1232" s="10" t="s">
         <v>5</v>
@@ -54654,7 +54656,7 @@
         <v>34394</v>
       </c>
       <c r="G1233" s="10" t="s">
-        <v>4420</v>
+        <v>4419</v>
       </c>
       <c r="H1233" s="10" t="s">
         <v>5</v>
@@ -54687,7 +54689,7 @@
         <v>33425</v>
       </c>
       <c r="G1234" s="10" t="s">
-        <v>4421</v>
+        <v>4420</v>
       </c>
       <c r="H1234" s="10" t="s">
         <v>5</v>
@@ -54720,7 +54722,7 @@
         <v>33434</v>
       </c>
       <c r="G1235" s="10" t="s">
-        <v>4422</v>
+        <v>4421</v>
       </c>
       <c r="H1235" s="10" t="s">
         <v>5</v>
@@ -54753,7 +54755,7 @@
         <v>33434</v>
       </c>
       <c r="G1236" s="10" t="s">
-        <v>4422</v>
+        <v>4421</v>
       </c>
       <c r="H1236" s="10" t="s">
         <v>5</v>
@@ -54786,7 +54788,7 @@
         <v>33586</v>
       </c>
       <c r="G1237" s="10" t="s">
-        <v>4423</v>
+        <v>4422</v>
       </c>
       <c r="H1237" s="10" t="s">
         <v>5</v>
@@ -54819,7 +54821,7 @@
         <v>34608</v>
       </c>
       <c r="G1238" s="10" t="s">
-        <v>4424</v>
+        <v>4423</v>
       </c>
       <c r="H1238" s="10" t="s">
         <v>5</v>
@@ -54852,7 +54854,7 @@
         <v>34000</v>
       </c>
       <c r="G1239" s="10" t="s">
-        <v>4425</v>
+        <v>4424</v>
       </c>
       <c r="H1239" s="10" t="s">
         <v>5</v>
@@ -54885,7 +54887,7 @@
         <v>33351</v>
       </c>
       <c r="G1240" s="10" t="s">
-        <v>4426</v>
+        <v>4425</v>
       </c>
       <c r="H1240" s="10" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added received phone numbers up to 19 feb 2024
</commit_message>
<xml_diff>
--- a/ASSAM_ELECROLL.xlsx
+++ b/ASSAM_ELECROLL.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7623" uniqueCount="4486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7624" uniqueCount="4486">
   <si>
     <t>1994</t>
   </si>
@@ -14268,8 +14268,8 @@
   </sheetPr>
   <dimension ref="A1:K1240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1065" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I1068" sqref="I1068"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24479,8 +24479,12 @@
       <c r="I310" s="1" t="s">
         <v>1330</v>
       </c>
-      <c r="J310" s="5"/>
-      <c r="K310" s="1"/>
+      <c r="J310" s="5">
+        <v>9435349301</v>
+      </c>
+      <c r="K310" s="1" t="s">
+        <v>4484</v>
+      </c>
     </row>
     <row r="311" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
@@ -47621,10 +47625,10 @@
         <v>3908</v>
       </c>
       <c r="J1013" s="9">
-        <v>8981558104</v>
+        <v>8017719660</v>
       </c>
       <c r="K1013" s="7" t="s">
-        <v>3866</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1014" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -47824,10 +47828,10 @@
         <v>3915</v>
       </c>
       <c r="J1020" s="9">
-        <v>7002039865</v>
+        <v>7002039861</v>
       </c>
       <c r="K1020" s="7" t="s">
-        <v>3866</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1021" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -50246,9 +50250,11 @@
       <c r="I1095" s="10" t="s">
         <v>3989</v>
       </c>
-      <c r="J1095" s="10"/>
+      <c r="J1095" s="10">
+        <v>8638039391</v>
+      </c>
       <c r="K1095" s="10" t="s">
-        <v>3866</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1096" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -51347,9 +51353,11 @@
       <c r="I1130" s="10" t="s">
         <v>4024</v>
       </c>
-      <c r="J1130" s="10"/>
+      <c r="J1130" s="10">
+        <v>9440616346</v>
+      </c>
       <c r="K1130" s="10" t="s">
-        <v>3866</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="1131" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -54903,8 +54911,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1240"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="73" fitToHeight="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup scale="72" fitToHeight="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>